<commit_message>
Add some useful functions.
1. Bug fixes for merges. Now grade is a ordinal categorical variable.
2. Add a useful function plotcorr.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="670">
   <si>
     <t>符号判断</t>
   </si>
@@ -2646,6 +2646,10 @@
   </si>
   <si>
     <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3298,11 +3302,11 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="A34:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5230,7 +5234,9 @@
       <c r="L34" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="M34" s="18"/>
+      <c r="M34" t="s">
+        <v>669</v>
+      </c>
       <c r="P34" s="22" t="s">
         <v>185</v>
       </c>
@@ -5288,7 +5294,9 @@
       <c r="L35" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="M35" s="18"/>
+      <c r="M35" t="s">
+        <v>669</v>
+      </c>
       <c r="P35" s="22" t="s">
         <v>185</v>
       </c>
@@ -5344,7 +5352,9 @@
       <c r="L36" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="M36" s="18"/>
+      <c r="M36" t="s">
+        <v>669</v>
+      </c>
       <c r="P36" s="22" t="s">
         <v>185</v>
       </c>
@@ -5402,7 +5412,9 @@
       <c r="L37" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="M37" s="18"/>
+      <c r="M37" t="s">
+        <v>669</v>
+      </c>
       <c r="P37" s="22" t="s">
         <v>185</v>
       </c>

</xml_diff>

<commit_message>
Polish works and compatibility works.
Add a new parameter specification for CPT2 task.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -2035,10 +2035,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>STIM RT ACC Resp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>efficiency</t>
   </si>
   <si>
@@ -2650,6 +2646,10 @@
   </si>
   <si>
     <t>CountTotalTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STIM RT ACC Resp\STIM RT ACC Resp SCat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3301,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
@@ -3346,22 +3346,22 @@
         <v>156</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>236</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>167</v>
@@ -3373,28 +3373,28 @@
         <v>496</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>168</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>514</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -3419,7 +3419,7 @@
         <v>214</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>166</v>
@@ -3432,16 +3432,16 @@
         <v>169</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>188</v>
@@ -3450,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -3475,7 +3475,7 @@
         <v>214</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>166</v>
@@ -3488,16 +3488,16 @@
         <v>169</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>188</v>
@@ -3506,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -3531,7 +3531,7 @@
         <v>214</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>166</v>
@@ -3544,16 +3544,16 @@
         <v>169</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>188</v>
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -3587,7 +3587,7 @@
         <v>214</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>166</v>
@@ -3600,16 +3600,16 @@
         <v>169</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>188</v>
@@ -3618,7 +3618,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -3643,7 +3643,7 @@
         <v>214</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>166</v>
@@ -3656,16 +3656,16 @@
         <v>169</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>188</v>
@@ -3674,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3699,7 +3699,7 @@
         <v>214</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>166</v>
@@ -3712,16 +3712,16 @@
         <v>169</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>188</v>
@@ -3730,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3751,26 +3751,26 @@
       <c r="F8" s="5"/>
       <c r="G8" s="20"/>
       <c r="H8" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3794,10 +3794,10 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>174</v>
@@ -3806,19 +3806,19 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Q9" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>191</v>
@@ -3827,7 +3827,7 @@
         <v>2</v>
       </c>
       <c r="U9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -3851,10 +3851,10 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>174</v>
@@ -3863,19 +3863,19 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Q10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>191</v>
@@ -3884,7 +3884,7 @@
         <v>2</v>
       </c>
       <c r="U10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -3908,28 +3908,28 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="P11" s="21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Q11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="R11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>193</v>
@@ -3938,7 +3938,7 @@
         <v>2</v>
       </c>
       <c r="U11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -3950,7 +3950,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>140</v>
@@ -3962,27 +3962,27 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>177</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="P12" s="21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Q12" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="R12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>193</v>
@@ -3991,7 +3991,7 @@
         <v>2</v>
       </c>
       <c r="U12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -4018,26 +4018,26 @@
         <v>185</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I13" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>660</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>661</v>
       </c>
       <c r="M13" s="18"/>
       <c r="P13" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q13" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="R13">
         <v>3000</v>
@@ -4049,7 +4049,7 @@
         <v>2</v>
       </c>
       <c r="U13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -4074,7 +4074,7 @@
         <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>170</v>
@@ -4086,16 +4086,16 @@
       <c r="L14" s="2"/>
       <c r="M14" s="19"/>
       <c r="O14" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q14" t="s">
+        <v>627</v>
+      </c>
+      <c r="R14" t="s">
         <v>628</v>
-      </c>
-      <c r="R14" t="s">
-        <v>629</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>189</v>
@@ -4104,7 +4104,7 @@
         <v>3</v>
       </c>
       <c r="U14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -4129,7 +4129,7 @@
         <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>170</v>
@@ -4141,16 +4141,16 @@
       <c r="L15" s="2"/>
       <c r="M15" s="19"/>
       <c r="O15" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q15" t="s">
+        <v>627</v>
+      </c>
+      <c r="R15" t="s">
         <v>628</v>
-      </c>
-      <c r="R15" t="s">
-        <v>629</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>189</v>
@@ -4159,7 +4159,7 @@
         <v>3</v>
       </c>
       <c r="U15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -4184,7 +4184,7 @@
         <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>170</v>
@@ -4196,16 +4196,16 @@
       <c r="L16" s="2"/>
       <c r="M16" s="19"/>
       <c r="O16" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q16" t="s">
+        <v>627</v>
+      </c>
+      <c r="R16" t="s">
         <v>628</v>
-      </c>
-      <c r="R16" t="s">
-        <v>629</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>189</v>
@@ -4214,7 +4214,7 @@
         <v>3</v>
       </c>
       <c r="U16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -4239,7 +4239,7 @@
         <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>170</v>
@@ -4251,16 +4251,16 @@
       <c r="L17" s="2"/>
       <c r="M17" s="19"/>
       <c r="O17" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q17" t="s">
+        <v>627</v>
+      </c>
+      <c r="R17" t="s">
         <v>628</v>
-      </c>
-      <c r="R17" t="s">
-        <v>629</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>189</v>
@@ -4269,7 +4269,7 @@
         <v>3</v>
       </c>
       <c r="U17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -4296,7 +4296,7 @@
         <v>498</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>166</v>
@@ -4310,16 +4310,16 @@
       </c>
       <c r="M18" s="19"/>
       <c r="O18" s="24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>188</v>
@@ -4328,7 +4328,7 @@
         <v>3</v>
       </c>
       <c r="U18" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -4355,7 +4355,7 @@
         <v>498</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>166</v>
@@ -4369,16 +4369,16 @@
       </c>
       <c r="M19" s="19"/>
       <c r="O19" s="24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>188</v>
@@ -4387,7 +4387,7 @@
         <v>3</v>
       </c>
       <c r="U19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -4414,7 +4414,7 @@
         <v>498</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>166</v>
@@ -4428,16 +4428,16 @@
       </c>
       <c r="M20" s="19"/>
       <c r="O20" s="24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q20" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="R20" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>188</v>
@@ -4446,7 +4446,7 @@
         <v>3</v>
       </c>
       <c r="U20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -4473,7 +4473,7 @@
         <v>498</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>166</v>
@@ -4487,16 +4487,16 @@
       </c>
       <c r="M21" s="19"/>
       <c r="O21" s="24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>188</v>
@@ -4505,7 +4505,7 @@
         <v>3</v>
       </c>
       <c r="U21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -4529,10 +4529,10 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>170</v>
@@ -4546,16 +4546,16 @@
       </c>
       <c r="M22" s="19"/>
       <c r="O22" s="24" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q22" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R22" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>191</v>
@@ -4564,7 +4564,7 @@
         <v>3</v>
       </c>
       <c r="U22" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -4588,10 +4588,10 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>170</v>
@@ -4605,16 +4605,16 @@
       </c>
       <c r="M23" s="19"/>
       <c r="O23" s="24" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q23" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>191</v>
@@ -4623,7 +4623,7 @@
         <v>3</v>
       </c>
       <c r="U23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
@@ -4647,10 +4647,10 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>170</v>
@@ -4664,16 +4664,16 @@
       </c>
       <c r="M24" s="19"/>
       <c r="O24" s="24" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q24" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R24" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>191</v>
@@ -4682,7 +4682,7 @@
         <v>3</v>
       </c>
       <c r="U24" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -4707,7 +4707,7 @@
         <v>47</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>170</v>
@@ -4719,16 +4719,16 @@
       <c r="L25" s="2"/>
       <c r="M25" s="19"/>
       <c r="O25" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R25" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>191</v>
@@ -4737,7 +4737,7 @@
         <v>3</v>
       </c>
       <c r="U25" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -4762,7 +4762,7 @@
         <v>47</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>170</v>
@@ -4774,16 +4774,16 @@
       <c r="L26" s="2"/>
       <c r="M26" s="19"/>
       <c r="O26" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P26" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q26" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R26" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>191</v>
@@ -4792,7 +4792,7 @@
         <v>3</v>
       </c>
       <c r="U26" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -4815,7 +4815,7 @@
         <v>182</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>175</v>
@@ -4823,17 +4823,17 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="M27" s="19"/>
       <c r="O27" s="24" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R27">
         <v>600</v>
@@ -4845,7 +4845,7 @@
         <v>4</v>
       </c>
       <c r="U27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -4870,7 +4870,7 @@
         <v>214</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>166</v>
@@ -4880,17 +4880,17 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M28" s="19"/>
       <c r="O28" s="24" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>188</v>
@@ -4899,7 +4899,7 @@
         <v>4</v>
       </c>
       <c r="U28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -4924,38 +4924,38 @@
         <v>214</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I29" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>508</v>
-      </c>
       <c r="K29" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L29" s="18" t="s">
         <v>169</v>
       </c>
       <c r="M29" s="19"/>
       <c r="O29" s="25" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="T29">
         <v>4</v>
       </c>
       <c r="U29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
@@ -4982,7 +4982,7 @@
         <v>504</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>166</v>
@@ -4996,19 +4996,19 @@
       </c>
       <c r="M30" s="19"/>
       <c r="N30" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="P30" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Q30" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="R30" s="17" t="s">
         <v>636</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>637</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>188</v>
@@ -5017,7 +5017,7 @@
         <v>4</v>
       </c>
       <c r="U30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
@@ -5044,7 +5044,7 @@
         <v>504</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>166</v>
@@ -5054,23 +5054,23 @@
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="M31" s="19"/>
       <c r="N31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="P31" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>188</v>
@@ -5079,7 +5079,7 @@
         <v>4</v>
       </c>
       <c r="U31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
@@ -5106,7 +5106,7 @@
         <v>493</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>166</v>
@@ -5120,13 +5120,13 @@
       </c>
       <c r="M32" s="19"/>
       <c r="O32" s="26" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P32" s="22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="2" t="s">
@@ -5136,7 +5136,7 @@
         <v>5</v>
       </c>
       <c r="U32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -5163,7 +5163,7 @@
         <v>494</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>166</v>
@@ -5177,13 +5177,13 @@
       </c>
       <c r="M33" s="19"/>
       <c r="O33" s="26" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P33" s="22" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="2" t="s">
@@ -5193,7 +5193,7 @@
         <v>5</v>
       </c>
       <c r="U33" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -5220,28 +5220,28 @@
         <v>185</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I34" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>661</v>
-      </c>
       <c r="M34" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q34" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="R34" s="17">
         <v>2000</v>
@@ -5253,7 +5253,7 @@
         <v>5</v>
       </c>
       <c r="U34" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
@@ -5280,28 +5280,28 @@
         <v>185</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I35" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>661</v>
-      </c>
       <c r="M35" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P35" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q35" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="R35" s="17">
         <v>3000</v>
@@ -5313,7 +5313,7 @@
         <v>5</v>
       </c>
       <c r="U35" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -5338,28 +5338,28 @@
         <v>185</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I36" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="L36" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>661</v>
-      </c>
       <c r="M36" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q36" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="R36" s="17">
         <v>3000</v>
@@ -5371,7 +5371,7 @@
         <v>5</v>
       </c>
       <c r="U36" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
@@ -5398,28 +5398,28 @@
         <v>185</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I37" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>661</v>
-      </c>
       <c r="M37" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P37" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q37" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="R37" s="17">
         <v>3000</v>
@@ -5431,7 +5431,7 @@
         <v>5</v>
       </c>
       <c r="U37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
@@ -5455,28 +5455,28 @@
         <v>0.5</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I38" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="O38" s="24" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P38" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Q38" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R38" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S38" s="2" t="s">
         <v>189</v>
@@ -5485,7 +5485,7 @@
         <v>5</v>
       </c>
       <c r="U38" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
@@ -5509,28 +5509,28 @@
         <v>0.5</v>
       </c>
       <c r="G39" s="30" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="O39" s="24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="Q39" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R39" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="S39" s="2" t="s">
         <v>189</v>
@@ -5539,7 +5539,7 @@
         <v>5</v>
       </c>
       <c r="U39" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -5562,7 +5562,7 @@
         <v>164</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I40" s="28" t="s">
         <v>175</v>
@@ -5571,13 +5571,13 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="O40" s="24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P40" s="22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R40" s="17">
         <v>400</v>
@@ -5589,7 +5589,7 @@
         <v>6</v>
       </c>
       <c r="U40" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
@@ -5612,7 +5612,7 @@
         <v>164</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I41" s="28" t="s">
         <v>175</v>
@@ -5621,13 +5621,13 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="O41" s="24" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="P41" s="22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R41" s="17">
         <v>500</v>
@@ -5639,7 +5639,7 @@
         <v>6</v>
       </c>
       <c r="U41" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
@@ -5648,7 +5648,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>118</v>
@@ -5662,7 +5662,7 @@
         <v>164</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I42" s="28" t="s">
         <v>175</v>
@@ -5671,13 +5671,13 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="O42" s="24" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="P42" s="22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R42" s="17">
         <v>600</v>
@@ -5689,7 +5689,7 @@
         <v>6</v>
       </c>
       <c r="U42" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
@@ -5716,7 +5716,7 @@
         <v>183</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>187</v>
@@ -5727,16 +5727,16 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="O43" s="24" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P43" s="22" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q43" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="R43" s="17" t="s">
         <v>642</v>
-      </c>
-      <c r="R43" s="17" t="s">
-        <v>643</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>193</v>
@@ -5745,7 +5745,7 @@
         <v>6</v>
       </c>
       <c r="U43" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
@@ -5772,38 +5772,38 @@
         <v>184</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I44" s="28" t="s">
         <v>176</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P44" s="22" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q44" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="R44" s="17" t="s">
         <v>644</v>
       </c>
-      <c r="R44" s="17" t="s">
-        <v>645</v>
-      </c>
       <c r="S44" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="T44">
         <v>6</v>
       </c>
       <c r="U44" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
@@ -5830,38 +5830,38 @@
         <v>184</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I45" s="28" t="s">
         <v>179</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P45" s="22" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q45" s="17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="T45">
         <v>6</v>
       </c>
       <c r="U45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
@@ -5888,7 +5888,7 @@
         <v>183</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I46" s="20" t="s">
         <v>177</v>
@@ -5899,16 +5899,16 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="O46" s="24" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P46" s="22" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q46" s="17" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>193</v>
@@ -5917,7 +5917,7 @@
         <v>6</v>
       </c>
       <c r="U46" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
@@ -5938,7 +5938,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="20"/>
       <c r="H47" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="2"/>
@@ -5964,7 +5964,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="20"/>
       <c r="H48" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="2"/>
@@ -5992,7 +5992,7 @@
         <v>48</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I49" s="20" t="s">
         <v>178</v>
@@ -7683,8 +7683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -7700,7 +7700,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -7827,7 +7827,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -7849,7 +7849,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -7871,7 +7871,7 @@
         <v>62</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -7893,7 +7893,7 @@
         <v>60</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -7959,7 +7959,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>505</v>
+        <v>669</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -7987,7 +7987,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -8079,7 +8079,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -8119,7 +8119,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -8207,7 +8207,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -8335,7 +8335,7 @@
         <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -8437,10 +8437,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C8" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -8482,10 +8482,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>656</v>
+      </c>
+      <c r="C11" t="s">
         <v>657</v>
-      </c>
-      <c r="C11" t="s">
-        <v>658</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -8516,36 +8516,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B1" t="s">
         <v>533</v>
-      </c>
-      <c r="B1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>445</v>
@@ -8561,7 +8561,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>447</v>
@@ -8569,7 +8569,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>448</v>
@@ -8577,7 +8577,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>449</v>
@@ -8585,7 +8585,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>450</v>
@@ -8593,7 +8593,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>451</v>
@@ -8605,7 +8605,7 @@
         <v>一年级</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8614,7 +8614,7 @@
         <v>二年级</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8699,36 +8699,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>445</v>
@@ -8744,7 +8744,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>447</v>
@@ -8752,7 +8752,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>448</v>
@@ -8760,7 +8760,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>449</v>
@@ -8768,7 +8768,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>450</v>
@@ -8776,7 +8776,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>451</v>
@@ -8801,170 +8801,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B1" t="s">
         <v>555</v>
-      </c>
-      <c r="B1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B2" t="s">
         <v>557</v>
-      </c>
-      <c r="B2" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B3" t="s">
         <v>559</v>
-      </c>
-      <c r="B3" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" t="s">
         <v>561</v>
-      </c>
-      <c r="B4" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>563</v>
+      </c>
+      <c r="B6" t="s">
         <v>564</v>
-      </c>
-      <c r="B6" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>565</v>
+      </c>
+      <c r="B7" t="s">
         <v>566</v>
-      </c>
-      <c r="B7" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>570</v>
+      </c>
+      <c r="B11" t="s">
         <v>571</v>
-      </c>
-      <c r="B11" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>572</v>
+      </c>
+      <c r="B12" t="s">
         <v>573</v>
-      </c>
-      <c r="B12" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B13" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>575</v>
+      </c>
+      <c r="B14" t="s">
         <v>576</v>
-      </c>
-      <c r="B14" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B15" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B16" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>580</v>
+      </c>
+      <c r="B18" t="s">
         <v>581</v>
-      </c>
-      <c r="B18" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B19" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>583</v>
+      </c>
+      <c r="B20" t="s">
         <v>584</v>
-      </c>
-      <c r="B20" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B21" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the performance indices selection for the memory tasks. Bug fixes.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Libraries\git\CCDPro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\CCDPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="672">
   <si>
     <t>符号判断</t>
   </si>
@@ -2098,14 +2098,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hitRate simFARate newFARate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hitRate lureFARate foilFARate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Overall_hitRate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2355,14 +2347,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2574,18 +2558,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>dprimeUnion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2650,6 +2622,41 @@
   </si>
   <si>
     <t>STIM RT ACC Resp\STIM RT ACC Resp SCat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effc</t>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hitRate simFARate newFARate FARate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hitRate lureFARate foilFARate FARate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3301,12 +3308,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="A34:XFD36"/>
+      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3346,16 +3353,16 @@
         <v>156</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>236</v>
@@ -3376,16 +3383,16 @@
         <v>509</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>168</v>
@@ -3419,7 +3426,7 @@
         <v>214</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>166</v>
@@ -3432,16 +3439,16 @@
         <v>169</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="Q2" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>188</v>
@@ -3475,7 +3482,7 @@
         <v>214</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>166</v>
@@ -3488,16 +3495,16 @@
         <v>169</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="Q3" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>188</v>
@@ -3531,7 +3538,7 @@
         <v>214</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>166</v>
@@ -3544,16 +3551,16 @@
         <v>169</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="Q4" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>188</v>
@@ -3587,7 +3594,7 @@
         <v>214</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>166</v>
@@ -3600,16 +3607,16 @@
         <v>169</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="Q5" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>188</v>
@@ -3643,7 +3650,7 @@
         <v>214</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>166</v>
@@ -3656,16 +3663,16 @@
         <v>169</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="Q6" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>188</v>
@@ -3699,7 +3706,7 @@
         <v>214</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>166</v>
@@ -3712,16 +3719,16 @@
         <v>169</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="Q7" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>188</v>
@@ -3751,20 +3758,20 @@
       <c r="F8" s="5"/>
       <c r="G8" s="20"/>
       <c r="H8" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="T8">
         <v>1</v>
@@ -3794,10 +3801,10 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>174</v>
@@ -3806,19 +3813,19 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="Q9" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="R9" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>191</v>
@@ -3851,10 +3858,10 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>174</v>
@@ -3863,19 +3870,19 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="Q10" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="R10" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>191</v>
@@ -3908,28 +3915,28 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="P11" s="21" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="Q11" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="R11" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>193</v>
@@ -3950,7 +3957,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>140</v>
@@ -3962,27 +3969,27 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>177</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="P12" s="21" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="Q12" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="R12" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>193</v>
@@ -4018,26 +4025,26 @@
         <v>185</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="M13" s="18"/>
       <c r="P13" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q13" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="R13">
         <v>3000</v>
@@ -4074,7 +4081,7 @@
         <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>170</v>
@@ -4084,18 +4091,20 @@
         <v>172</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="19"/>
-      <c r="O14" s="24" t="s">
-        <v>595</v>
+      <c r="M14" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q14" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R14" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>189</v>
@@ -4129,7 +4138,7 @@
         <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>170</v>
@@ -4139,18 +4148,20 @@
         <v>172</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="19"/>
-      <c r="O15" s="24" t="s">
-        <v>595</v>
+      <c r="M15" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q15" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R15" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>189</v>
@@ -4184,7 +4195,7 @@
         <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>170</v>
@@ -4194,18 +4205,20 @@
         <v>172</v>
       </c>
       <c r="L16" s="2"/>
-      <c r="M16" s="19"/>
-      <c r="O16" s="24" t="s">
-        <v>595</v>
+      <c r="M16" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q16" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R16" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>189</v>
@@ -4239,7 +4252,7 @@
         <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>170</v>
@@ -4249,18 +4262,20 @@
         <v>495</v>
       </c>
       <c r="L17" s="2"/>
-      <c r="M17" s="19"/>
-      <c r="O17" s="24" t="s">
-        <v>595</v>
+      <c r="M17" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O17" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q17" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R17" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>189</v>
@@ -4296,7 +4311,7 @@
         <v>498</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>166</v>
@@ -4308,18 +4323,20 @@
       <c r="L18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="19"/>
-      <c r="O18" s="24" t="s">
-        <v>596</v>
+      <c r="M18" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>188</v>
@@ -4355,7 +4372,7 @@
         <v>498</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>166</v>
@@ -4367,18 +4384,20 @@
       <c r="L19" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M19" s="19"/>
-      <c r="O19" s="24" t="s">
-        <v>596</v>
+      <c r="M19" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>188</v>
@@ -4414,7 +4433,7 @@
         <v>498</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>166</v>
@@ -4426,18 +4445,20 @@
       <c r="L20" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="O20" s="24" t="s">
-        <v>596</v>
+      <c r="M20" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q20" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="R20" s="32" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>188</v>
@@ -4473,7 +4494,7 @@
         <v>498</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>166</v>
@@ -4485,18 +4506,20 @@
       <c r="L21" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M21" s="19"/>
-      <c r="O21" s="24" t="s">
-        <v>596</v>
+      <c r="M21" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>188</v>
@@ -4529,10 +4552,10 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>170</v>
@@ -4544,18 +4567,20 @@
       <c r="L22" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M22" s="19"/>
-      <c r="O22" s="24" t="s">
-        <v>651</v>
+      <c r="M22" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q22" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R22" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>191</v>
@@ -4588,10 +4613,10 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>170</v>
@@ -4603,18 +4628,20 @@
       <c r="L23" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M23" s="19"/>
-      <c r="O23" s="24" t="s">
-        <v>652</v>
+      <c r="M23" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q23" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R23" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>191</v>
@@ -4647,10 +4674,10 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>170</v>
@@ -4662,18 +4689,20 @@
       <c r="L24" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M24" s="19"/>
-      <c r="O24" s="24" t="s">
-        <v>652</v>
+      <c r="M24" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O24" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q24" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R24" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>191</v>
@@ -4707,7 +4736,7 @@
         <v>47</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>170</v>
@@ -4717,18 +4746,20 @@
         <v>172</v>
       </c>
       <c r="L25" s="2"/>
-      <c r="M25" s="19"/>
-      <c r="O25" s="24" t="s">
-        <v>595</v>
+      <c r="M25" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q25" t="s">
+        <v>623</v>
+      </c>
+      <c r="R25" t="s">
         <v>627</v>
-      </c>
-      <c r="R25" t="s">
-        <v>631</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>191</v>
@@ -4762,7 +4793,7 @@
         <v>47</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>170</v>
@@ -4772,18 +4803,20 @@
         <v>172</v>
       </c>
       <c r="L26" s="2"/>
-      <c r="M26" s="19"/>
-      <c r="O26" s="24" t="s">
-        <v>595</v>
+      <c r="M26" s="17" t="s">
+        <v>663</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>663</v>
       </c>
       <c r="P26" s="21" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="Q26" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R26" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>191</v>
@@ -4815,7 +4848,7 @@
         <v>182</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>175</v>
@@ -4823,17 +4856,17 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="5" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="M27" s="19"/>
       <c r="O27" s="24" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="R27">
         <v>600</v>
@@ -4870,7 +4903,7 @@
         <v>214</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>166</v>
@@ -4880,17 +4913,17 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="M28" s="19"/>
       <c r="O28" s="24" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>188</v>
@@ -4924,7 +4957,7 @@
         <v>214</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>506</v>
@@ -4940,13 +4973,13 @@
       </c>
       <c r="M29" s="19"/>
       <c r="O29" s="25" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="S29" s="2" t="s">
         <v>508</v>
@@ -4982,7 +5015,7 @@
         <v>504</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>166</v>
@@ -4999,16 +5032,16 @@
         <v>510</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="P30" s="22" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="Q30" s="17" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>188</v>
@@ -5044,7 +5077,7 @@
         <v>504</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>166</v>
@@ -5061,16 +5094,16 @@
         <v>510</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="P31" s="22" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>188</v>
@@ -5106,7 +5139,7 @@
         <v>493</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>166</v>
@@ -5120,13 +5153,13 @@
       </c>
       <c r="M32" s="19"/>
       <c r="O32" s="26" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="P32" s="22" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="2" t="s">
@@ -5163,7 +5196,7 @@
         <v>494</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>166</v>
@@ -5177,13 +5210,13 @@
       </c>
       <c r="M33" s="19"/>
       <c r="O33" s="26" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="P33" s="22" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="2" t="s">
@@ -5220,28 +5253,28 @@
         <v>185</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="J34" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="M34" t="s">
         <v>661</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="M34" t="s">
-        <v>668</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q34" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="R34" s="17">
         <v>2000</v>
@@ -5280,28 +5313,28 @@
         <v>185</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="J35" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="M35" t="s">
         <v>661</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="M35" t="s">
-        <v>668</v>
       </c>
       <c r="P35" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q35" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="R35" s="17">
         <v>3000</v>
@@ -5338,28 +5371,28 @@
         <v>185</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I36" s="28" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="J36" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="M36" t="s">
         <v>661</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="M36" t="s">
-        <v>668</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q36" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="R36" s="17">
         <v>3000</v>
@@ -5398,28 +5431,28 @@
         <v>185</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I37" s="28" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="J37" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="M37" t="s">
         <v>661</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>662</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>660</v>
-      </c>
-      <c r="M37" t="s">
-        <v>668</v>
       </c>
       <c r="P37" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q37" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="R37" s="17">
         <v>3000</v>
@@ -5455,28 +5488,28 @@
         <v>0.5</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I38" s="20" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="O38" s="24" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="P38" s="22" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="Q38" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R38" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="S38" s="2" t="s">
         <v>189</v>
@@ -5509,28 +5542,28 @@
         <v>0.5</v>
       </c>
       <c r="G39" s="30" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="O39" s="24" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="Q39" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="R39" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="S39" s="2" t="s">
         <v>189</v>
@@ -5562,7 +5595,7 @@
         <v>164</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I40" s="28" t="s">
         <v>175</v>
@@ -5571,13 +5604,13 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="O40" s="24" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="P40" s="22" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="R40" s="17">
         <v>400</v>
@@ -5612,7 +5645,7 @@
         <v>164</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I41" s="28" t="s">
         <v>175</v>
@@ -5621,13 +5654,13 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="O41" s="24" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="P41" s="22" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="R41" s="17">
         <v>500</v>
@@ -5648,7 +5681,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>118</v>
@@ -5662,7 +5695,7 @@
         <v>164</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I42" s="28" t="s">
         <v>175</v>
@@ -5671,13 +5704,13 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="O42" s="24" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="P42" s="22" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="R42" s="17">
         <v>600</v>
@@ -5716,7 +5749,7 @@
         <v>183</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>187</v>
@@ -5727,16 +5760,16 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="O43" s="24" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="P43" s="22" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="Q43" s="17" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="R43" s="17" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>193</v>
@@ -5772,32 +5805,35 @@
         <v>184</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I44" s="28" t="s">
         <v>176</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>521</v>
+        <v>668</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="5" t="s">
-        <v>647</v>
+        <v>643</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>666</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>650</v>
+        <v>664</v>
       </c>
       <c r="P44" s="22" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="Q44" s="17" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="R44" s="17" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="T44">
         <v>6</v>
@@ -5830,32 +5866,35 @@
         <v>184</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I45" s="28" t="s">
         <v>179</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>522</v>
+        <v>669</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="5" t="s">
-        <v>648</v>
+        <v>644</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>667</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>650</v>
+        <v>665</v>
       </c>
       <c r="P45" s="22" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="Q45" s="17" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="T45">
         <v>6</v>
@@ -5885,30 +5924,30 @@
         <v>0.5</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>183</v>
+        <v>670</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I46" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>180</v>
+        <v>166</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="L46" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="O46" s="24" t="s">
-        <v>649</v>
-      </c>
-      <c r="P46" s="22" t="s">
-        <v>615</v>
-      </c>
+        <v>671</v>
+      </c>
+      <c r="P46" s="22"/>
       <c r="Q46" s="17" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>193</v>
@@ -5938,7 +5977,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="20"/>
       <c r="H47" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="2"/>
@@ -5964,7 +6003,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="20"/>
       <c r="H48" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="2"/>
@@ -5992,7 +6031,7 @@
         <v>48</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I49" s="20" t="s">
         <v>178</v>
@@ -7683,8 +7722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -7700,7 +7739,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -7827,7 +7866,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -7849,7 +7888,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -7871,7 +7910,7 @@
         <v>62</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -7893,7 +7932,7 @@
         <v>60</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -7959,7 +7998,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -7987,7 +8026,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -8079,7 +8118,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -8119,7 +8158,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -8207,7 +8246,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -8335,7 +8374,7 @@
         <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -8437,10 +8476,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="C8" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -8482,10 +8521,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="C11" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -8516,36 +8555,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>445</v>
@@ -8561,7 +8600,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>447</v>
@@ -8569,7 +8608,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>448</v>
@@ -8577,7 +8616,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>449</v>
@@ -8585,7 +8624,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>450</v>
@@ -8593,7 +8632,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>451</v>
@@ -8605,7 +8644,7 @@
         <v>一年级</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8614,7 +8653,7 @@
         <v>二年级</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8699,36 +8738,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="B1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>445</v>
@@ -8744,7 +8783,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>447</v>
@@ -8752,7 +8791,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>448</v>
@@ -8760,7 +8799,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>449</v>
@@ -8768,7 +8807,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>450</v>
@@ -8776,7 +8815,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>451</v>
@@ -8801,170 +8840,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B7" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B8" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B9" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B10" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B11" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B12" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B13" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B14" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B15" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B16" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B17" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B18" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B19" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B20" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B21" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes in DRT and etc.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -174,6 +174,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>张亮:</t>
@@ -183,6 +184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -314,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="671">
   <si>
     <t>符号判断</t>
   </si>
@@ -2035,628 +2037,626 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Count RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit FA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count_hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MergeCond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VarsCond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlideSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SectionSummary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Languange Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Processing Speed Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attention Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Executive Function &amp; Updating Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span &amp; Memory Tasks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall_hitRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三</t>
+  </si>
+  <si>
+    <t>五</t>
+  </si>
+  <si>
+    <t>六</t>
+  </si>
+  <si>
+    <t>七</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>八</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>九</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GradeStr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountAccTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalScore MeanScore</t>
+  </si>
+  <si>
+    <t>TotalTime CountTotalTrl CountAccTrl TotalScore MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subitizing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NRRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnalysisVars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECORD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRECORD RRECORD|left right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRECORD RRECORD</t>
+  </si>
+  <si>
+    <t>STUDY TEST|学习阶段 测试阶段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STime RT ACC\RT ACC Resp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EZDiff</t>
+  </si>
+  <si>
+    <t>STIM RT ACC Resp\RT ACC STIM Resp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condition STIM ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fmt</t>
+  </si>
+  <si>
+    <t>ext</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpeg</t>
+  </si>
+  <si>
+    <t>.jpg</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>.png</t>
+  </si>
+  <si>
+    <t>tiff</t>
+  </si>
+  <si>
+    <t>.tif</t>
+  </si>
+  <si>
+    <t>tiffn</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>.emf</t>
+  </si>
+  <si>
+    <t>bmpmono</t>
+  </si>
+  <si>
+    <t>.bmp</t>
+  </si>
+  <si>
+    <t>bmp</t>
+  </si>
+  <si>
+    <t>bmp16m</t>
+  </si>
+  <si>
+    <t>bmp256</t>
+  </si>
+  <si>
+    <t>hdf</t>
+  </si>
+  <si>
+    <t>.hdf</t>
+  </si>
+  <si>
+    <t>pbm</t>
+  </si>
+  <si>
+    <t>.pbm</t>
+  </si>
+  <si>
+    <t>pbmraw</t>
+  </si>
+  <si>
+    <t>pcxmono</t>
+  </si>
+  <si>
+    <t>.pcx</t>
+  </si>
+  <si>
+    <t>pcx24b</t>
+  </si>
+  <si>
+    <t>pcx256</t>
+  </si>
+  <si>
+    <t>pcx16</t>
+  </si>
+  <si>
+    <t>pgm</t>
+  </si>
+  <si>
+    <t>.pgm</t>
+  </si>
+  <si>
+    <t>pgmraw</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>.ppm</t>
+  </si>
+  <si>
+    <t>ppmraw</t>
+  </si>
+  <si>
+    <t>ACC MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S1 S2 Resp ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S1 S2 CResp Resp ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RUN S1 S2 CResp NL NR Resp ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mentcompare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UltimateIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl CountAccTrl TotalScore MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeanScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GNG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Span</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScoringPara</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3001 3000 3000</t>
+  </si>
+  <si>
+    <t>ScoringVars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TotalTime TotalScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall D1 D2 D3 D4 D5 D6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC RT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_Overall ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_Overall ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overall D1 D2 D3 D4 D5 D8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2500 2000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2800 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3200 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_hit Count_FA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScoringFun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500 1500 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1500 1500 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000 3000 3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLACC MLNextACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ML MLACC MLNextACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC_R1 ACC_R2 RT_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>150 100 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1_hitRate R2_hitRate MRT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 40 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 35 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50 35 20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeTM dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeTM dprimeFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprimeUnion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChanceACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClsStr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怀北学校</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怀北学校</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>棠湖中学实验学校</t>
+  </si>
+  <si>
+    <t>MRT ACC VRT v a Ter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT_Overall ACC_Overall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Congruent Incongruent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT_CongEffect ACC_CongEffect v_CongEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT_Overall ACC_Overall MRT_CongEffect ACC_CongEffect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置记忆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT_hit Rate_hit Count_FA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STIM RT ACC Resp\STIM RT ACC Resp SCat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hitRate simFARate newFARate FARate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hitRate lureFARate foilFARate FARate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>efficiency</t>
-  </si>
-  <si>
-    <t>Count RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hit FA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count_hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MergeCond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>L R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VarsCond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SlideSection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SectionSummary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Languange Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Math Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Processing Speed Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attention Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Executive Function &amp; Updating Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Span &amp; Memory Tasks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall_hitRate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>二</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三</t>
-  </si>
-  <si>
-    <t>五</t>
-  </si>
-  <si>
-    <t>六</t>
-  </si>
-  <si>
-    <t>七</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>八</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>九</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GradeStr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Encode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CountAccTrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalScore MeanScore</t>
-  </si>
-  <si>
-    <t>TotalTime CountTotalTrl CountAccTrl TotalScore MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Subitizing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NRRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnalysisVars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RECORD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LRECORD RRECORD|left right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LRECORD RRECORD</t>
-  </si>
-  <si>
-    <t>STUDY TEST|学习阶段 测试阶段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STime RT ACC\RT ACC Resp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EZDiff</t>
-  </si>
-  <si>
-    <t>STIM RT ACC Resp\RT ACC STIM Resp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Condition STIM ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fmt</t>
-  </si>
-  <si>
-    <t>ext</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jpeg</t>
-  </si>
-  <si>
-    <t>.jpg</t>
-  </si>
-  <si>
-    <t>png</t>
-  </si>
-  <si>
-    <t>.png</t>
-  </si>
-  <si>
-    <t>tiff</t>
-  </si>
-  <si>
-    <t>.tif</t>
-  </si>
-  <si>
-    <t>tiffn</t>
-  </si>
-  <si>
-    <t>meta</t>
-  </si>
-  <si>
-    <t>.emf</t>
-  </si>
-  <si>
-    <t>bmpmono</t>
-  </si>
-  <si>
-    <t>.bmp</t>
-  </si>
-  <si>
-    <t>bmp</t>
-  </si>
-  <si>
-    <t>bmp16m</t>
-  </si>
-  <si>
-    <t>bmp256</t>
-  </si>
-  <si>
-    <t>hdf</t>
-  </si>
-  <si>
-    <t>.hdf</t>
-  </si>
-  <si>
-    <t>pbm</t>
-  </si>
-  <si>
-    <t>.pbm</t>
-  </si>
-  <si>
-    <t>pbmraw</t>
-  </si>
-  <si>
-    <t>pcxmono</t>
-  </si>
-  <si>
-    <t>.pcx</t>
-  </si>
-  <si>
-    <t>pcx24b</t>
-  </si>
-  <si>
-    <t>pcx256</t>
-  </si>
-  <si>
-    <t>pcx16</t>
-  </si>
-  <si>
-    <t>pgm</t>
-  </si>
-  <si>
-    <t>.pgm</t>
-  </si>
-  <si>
-    <t>pgmraw</t>
-  </si>
-  <si>
-    <t>ppm</t>
-  </si>
-  <si>
-    <t>.ppm</t>
-  </si>
-  <si>
-    <t>ppmraw</t>
-  </si>
-  <si>
-    <t>ACC MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S1 S2 Resp ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S1 S2 CResp Resp ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RUN S1 S2 CResp NL NR Resp ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mentcompare</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UltimateIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CountTotalTrl CountAccTrl TotalScore MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MeanScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Span</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GNG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Span</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScoringPara</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3001 3000 3000</t>
-  </si>
-  <si>
-    <t>ScoringVars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalTime TotalScore</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall D1 D2 D3 D4 D5 D6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC RT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_Overall ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_Overall ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overall D1 D2 D3 D4 D5 D8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2500 2000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2800 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3200 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_hit Count_FA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ScoringFun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500 1500 1500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1500 1500 1500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3000 3000 3000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MLACC MLNextACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ML MLACC MLNextACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC_R1 ACC_R2 RT_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>150 100 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1_hitRate R2_hitRate MRT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>60 40 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50 35 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50 35 20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeTM dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeTM dprimeFM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprimeUnion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ChanceACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ClsStr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>怀北学校</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>怀北学校</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>棠湖中学实验学校</t>
-  </si>
-  <si>
-    <t>MRT ACC VRT v a Ter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT_Overall ACC_Overall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Congruent Incongruent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT_CongEffect ACC_CongEffect v_CongEffect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MRT_Overall ACC_Overall MRT_CongEffect ACC_CongEffect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>位置记忆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RT_hit Rate_hit Count_FA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CountTotalTrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STIM RT ACC Resp\STIM RT ACC Resp SCat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Effc</t>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hitRate simFARate newFARate FARate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hitRate lureFARate foilFARate FARate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dprime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2664,7 +2664,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2844,19 +2844,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3309,11 +3296,11 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3353,22 +3340,22 @@
         <v>156</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>236</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>167</v>
@@ -3380,28 +3367,28 @@
         <v>496</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>168</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -3426,7 +3413,7 @@
         <v>214</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>166</v>
@@ -3439,16 +3426,16 @@
         <v>169</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>188</v>
@@ -3457,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -3482,7 +3469,7 @@
         <v>214</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>166</v>
@@ -3495,16 +3482,16 @@
         <v>169</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>188</v>
@@ -3513,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -3538,7 +3525,7 @@
         <v>214</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>166</v>
@@ -3551,16 +3538,16 @@
         <v>169</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>188</v>
@@ -3569,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -3594,7 +3581,7 @@
         <v>214</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>166</v>
@@ -3607,16 +3594,16 @@
         <v>169</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>188</v>
@@ -3625,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -3650,7 +3637,7 @@
         <v>214</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>166</v>
@@ -3663,16 +3650,16 @@
         <v>169</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>188</v>
@@ -3681,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3706,7 +3693,7 @@
         <v>214</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>166</v>
@@ -3719,16 +3706,16 @@
         <v>169</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>188</v>
@@ -3737,7 +3724,7 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3758,26 +3745,26 @@
       <c r="F8" s="5"/>
       <c r="G8" s="20"/>
       <c r="H8" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3801,10 +3788,10 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>174</v>
@@ -3813,19 +3800,19 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q9" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="R9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>191</v>
@@ -3834,7 +3821,7 @@
         <v>2</v>
       </c>
       <c r="U9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -3858,10 +3845,10 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>174</v>
@@ -3870,19 +3857,19 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="R10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>191</v>
@@ -3891,7 +3878,7 @@
         <v>2</v>
       </c>
       <c r="U10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -3915,28 +3902,28 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="P11" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>193</v>
@@ -3945,7 +3932,7 @@
         <v>2</v>
       </c>
       <c r="U11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -3957,7 +3944,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>140</v>
@@ -3969,27 +3956,27 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>177</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="P12" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R12" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>193</v>
@@ -3998,7 +3985,7 @@
         <v>2</v>
       </c>
       <c r="U12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -4025,26 +4012,26 @@
         <v>185</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I13" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>652</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>653</v>
       </c>
       <c r="M13" s="18"/>
       <c r="P13" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q13" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R13">
         <v>3000</v>
@@ -4056,7 +4043,7 @@
         <v>2</v>
       </c>
       <c r="U13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -4081,7 +4068,7 @@
         <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>170</v>
@@ -4092,19 +4079,19 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q14" t="s">
+        <v>622</v>
+      </c>
+      <c r="R14" t="s">
         <v>623</v>
-      </c>
-      <c r="R14" t="s">
-        <v>624</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>189</v>
@@ -4113,7 +4100,7 @@
         <v>3</v>
       </c>
       <c r="U14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -4138,7 +4125,7 @@
         <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>170</v>
@@ -4149,19 +4136,19 @@
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q15" t="s">
+        <v>622</v>
+      </c>
+      <c r="R15" t="s">
         <v>623</v>
-      </c>
-      <c r="R15" t="s">
-        <v>624</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>189</v>
@@ -4170,7 +4157,7 @@
         <v>3</v>
       </c>
       <c r="U15" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -4195,7 +4182,7 @@
         <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>170</v>
@@ -4206,19 +4193,19 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q16" t="s">
+        <v>622</v>
+      </c>
+      <c r="R16" t="s">
         <v>623</v>
-      </c>
-      <c r="R16" t="s">
-        <v>624</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>189</v>
@@ -4227,7 +4214,7 @@
         <v>3</v>
       </c>
       <c r="U16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -4252,7 +4239,7 @@
         <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>170</v>
@@ -4263,19 +4250,19 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q17" t="s">
+        <v>622</v>
+      </c>
+      <c r="R17" t="s">
         <v>623</v>
-      </c>
-      <c r="R17" t="s">
-        <v>624</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>189</v>
@@ -4284,7 +4271,7 @@
         <v>3</v>
       </c>
       <c r="U17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -4311,7 +4298,7 @@
         <v>498</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>166</v>
@@ -4324,19 +4311,19 @@
         <v>169</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>188</v>
@@ -4345,7 +4332,7 @@
         <v>3</v>
       </c>
       <c r="U18" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
@@ -4372,7 +4359,7 @@
         <v>498</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>166</v>
@@ -4385,19 +4372,19 @@
         <v>169</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>188</v>
@@ -4406,7 +4393,7 @@
         <v>3</v>
       </c>
       <c r="U19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -4433,7 +4420,7 @@
         <v>498</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>166</v>
@@ -4446,19 +4433,19 @@
         <v>169</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q20" s="31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R20" s="32" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>188</v>
@@ -4467,7 +4454,7 @@
         <v>3</v>
       </c>
       <c r="U20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -4494,7 +4481,7 @@
         <v>498</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>166</v>
@@ -4507,19 +4494,19 @@
         <v>169</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>188</v>
@@ -4528,7 +4515,7 @@
         <v>3</v>
       </c>
       <c r="U21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -4552,10 +4539,10 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>170</v>
@@ -4568,19 +4555,19 @@
         <v>196</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>191</v>
@@ -4589,7 +4576,7 @@
         <v>3</v>
       </c>
       <c r="U22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -4613,10 +4600,10 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>170</v>
@@ -4629,19 +4616,19 @@
         <v>196</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q23" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R23" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>191</v>
@@ -4650,7 +4637,7 @@
         <v>3</v>
       </c>
       <c r="U23" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
@@ -4674,10 +4661,10 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>170</v>
@@ -4690,19 +4677,19 @@
         <v>196</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q24" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R24" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>191</v>
@@ -4711,7 +4698,7 @@
         <v>3</v>
       </c>
       <c r="U24" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -4736,7 +4723,7 @@
         <v>47</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>170</v>
@@ -4747,19 +4734,19 @@
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q25" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>191</v>
@@ -4768,7 +4755,7 @@
         <v>3</v>
       </c>
       <c r="U25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -4793,7 +4780,7 @@
         <v>47</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>170</v>
@@ -4804,19 +4791,19 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="P26" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q26" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R26" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>191</v>
@@ -4825,7 +4812,7 @@
         <v>3</v>
       </c>
       <c r="U26" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -4848,7 +4835,7 @@
         <v>182</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>175</v>
@@ -4856,17 +4843,17 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="M27" s="19"/>
       <c r="O27" s="24" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R27">
         <v>600</v>
@@ -4878,7 +4865,7 @@
         <v>4</v>
       </c>
       <c r="U27" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -4903,7 +4890,7 @@
         <v>214</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>166</v>
@@ -4913,17 +4900,17 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="M28" s="19"/>
       <c r="O28" s="24" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>188</v>
@@ -4932,7 +4919,7 @@
         <v>4</v>
       </c>
       <c r="U28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -4957,38 +4944,36 @@
         <v>214</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I29" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>505</v>
-      </c>
+      <c r="K29" s="10"/>
       <c r="L29" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="19"/>
+      <c r="M29" s="10"/>
       <c r="O29" s="25" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="T29">
         <v>4</v>
       </c>
       <c r="U29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
@@ -5015,7 +5000,7 @@
         <v>504</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>166</v>
@@ -5029,19 +5014,19 @@
       </c>
       <c r="M30" s="19"/>
       <c r="N30" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="P30" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q30" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="R30" s="17" t="s">
         <v>631</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>632</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>188</v>
@@ -5050,7 +5035,7 @@
         <v>4</v>
       </c>
       <c r="U30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
@@ -5077,7 +5062,7 @@
         <v>504</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>166</v>
@@ -5087,23 +5072,23 @@
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="M31" s="19"/>
       <c r="N31" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="P31" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>188</v>
@@ -5112,7 +5097,7 @@
         <v>4</v>
       </c>
       <c r="U31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.3">
@@ -5139,7 +5124,7 @@
         <v>493</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>166</v>
@@ -5153,13 +5138,13 @@
       </c>
       <c r="M32" s="19"/>
       <c r="O32" s="26" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P32" s="22" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="2" t="s">
@@ -5169,7 +5154,7 @@
         <v>5</v>
       </c>
       <c r="U32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -5196,7 +5181,7 @@
         <v>494</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>166</v>
@@ -5210,13 +5195,13 @@
       </c>
       <c r="M33" s="19"/>
       <c r="O33" s="26" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P33" s="22" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="2" t="s">
@@ -5226,7 +5211,7 @@
         <v>5</v>
       </c>
       <c r="U33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -5253,28 +5238,28 @@
         <v>185</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I34" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>653</v>
-      </c>
       <c r="M34" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q34" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R34" s="17">
         <v>2000</v>
@@ -5286,7 +5271,7 @@
         <v>5</v>
       </c>
       <c r="U34" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
@@ -5313,28 +5298,28 @@
         <v>185</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I35" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>653</v>
-      </c>
       <c r="M35" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P35" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q35" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R35" s="17">
         <v>3000</v>
@@ -5346,7 +5331,7 @@
         <v>5</v>
       </c>
       <c r="U35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -5371,28 +5356,28 @@
         <v>185</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I36" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="L36" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>653</v>
-      </c>
       <c r="M36" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q36" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R36" s="17">
         <v>3000</v>
@@ -5404,7 +5389,7 @@
         <v>5</v>
       </c>
       <c r="U36" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
@@ -5431,28 +5416,28 @@
         <v>185</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I37" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>653</v>
-      </c>
       <c r="M37" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P37" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q37" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R37" s="17">
         <v>3000</v>
@@ -5464,7 +5449,7 @@
         <v>5</v>
       </c>
       <c r="U37" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
@@ -5488,28 +5473,28 @@
         <v>0.5</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I38" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="O38" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P38" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="S38" s="2" t="s">
         <v>189</v>
@@ -5518,7 +5503,7 @@
         <v>5</v>
       </c>
       <c r="U38" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
@@ -5542,28 +5527,28 @@
         <v>0.5</v>
       </c>
       <c r="G39" s="30" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I39" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="O39" s="24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="Q39" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="R39" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="S39" s="2" t="s">
         <v>189</v>
@@ -5572,7 +5557,7 @@
         <v>5</v>
       </c>
       <c r="U39" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -5595,7 +5580,7 @@
         <v>164</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I40" s="28" t="s">
         <v>175</v>
@@ -5604,13 +5589,13 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="O40" s="24" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P40" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R40" s="17">
         <v>400</v>
@@ -5622,7 +5607,7 @@
         <v>6</v>
       </c>
       <c r="U40" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
@@ -5645,7 +5630,7 @@
         <v>164</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I41" s="28" t="s">
         <v>175</v>
@@ -5654,13 +5639,13 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="O41" s="24" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P41" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R41" s="17">
         <v>500</v>
@@ -5672,7 +5657,7 @@
         <v>6</v>
       </c>
       <c r="U41" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
@@ -5681,7 +5666,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>118</v>
@@ -5695,7 +5680,7 @@
         <v>164</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I42" s="28" t="s">
         <v>175</v>
@@ -5704,13 +5689,13 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="O42" s="24" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="P42" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R42" s="17">
         <v>600</v>
@@ -5722,7 +5707,7 @@
         <v>6</v>
       </c>
       <c r="U42" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
@@ -5749,7 +5734,7 @@
         <v>183</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>187</v>
@@ -5760,16 +5745,16 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="O43" s="24" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="P43" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Q43" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="R43" s="17" t="s">
         <v>637</v>
-      </c>
-      <c r="R43" s="17" t="s">
-        <v>638</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>193</v>
@@ -5778,7 +5763,7 @@
         <v>6</v>
       </c>
       <c r="U43" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
@@ -5805,41 +5790,41 @@
         <v>184</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I44" s="28" t="s">
         <v>176</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="P44" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Q44" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="R44" s="17" t="s">
         <v>639</v>
       </c>
-      <c r="R44" s="17" t="s">
-        <v>640</v>
-      </c>
       <c r="S44" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T44">
         <v>6</v>
       </c>
       <c r="U44" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
@@ -5866,41 +5851,41 @@
         <v>184</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I45" s="28" t="s">
         <v>179</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="P45" s="22" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="Q45" s="17" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T45">
         <v>6</v>
       </c>
       <c r="U45" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
@@ -5924,10 +5909,10 @@
         <v>0.5</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I46" s="20" t="s">
         <v>166</v>
@@ -5940,14 +5925,14 @@
         <v>169</v>
       </c>
       <c r="O46" s="24" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="P46" s="22"/>
       <c r="Q46" s="17" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>193</v>
@@ -5956,7 +5941,7 @@
         <v>6</v>
       </c>
       <c r="U46" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
@@ -5977,7 +5962,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="20"/>
       <c r="H47" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="2"/>
@@ -6003,7 +5988,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="20"/>
       <c r="H48" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I48" s="20"/>
       <c r="J48" s="2"/>
@@ -6031,7 +6016,7 @@
         <v>48</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I49" s="20" t="s">
         <v>178</v>
@@ -7739,7 +7724,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>49</v>
@@ -7866,7 +7851,7 @@
         <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F6" s="4">
         <v>0</v>
@@ -7888,7 +7873,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -7910,7 +7895,7 @@
         <v>62</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -7932,7 +7917,7 @@
         <v>60</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -7998,7 +7983,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -8026,7 +8011,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -8118,7 +8103,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -8158,7 +8143,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -8246,7 +8231,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -8374,7 +8359,7 @@
         <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -8476,10 +8461,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -8521,10 +8506,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>648</v>
+      </c>
+      <c r="C11" t="s">
         <v>649</v>
-      </c>
-      <c r="C11" t="s">
-        <v>650</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -8555,36 +8540,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B1" t="s">
         <v>530</v>
-      </c>
-      <c r="B1" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>445</v>
@@ -8600,7 +8585,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>447</v>
@@ -8608,7 +8593,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>448</v>
@@ -8616,7 +8601,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>449</v>
@@ -8624,7 +8609,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>450</v>
@@ -8632,7 +8617,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>451</v>
@@ -8644,7 +8629,7 @@
         <v>一年级</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -8653,7 +8638,7 @@
         <v>二年级</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -8738,36 +8723,36 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>445</v>
@@ -8783,7 +8768,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>447</v>
@@ -8791,7 +8776,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>448</v>
@@ -8799,7 +8784,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>449</v>
@@ -8807,7 +8792,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>450</v>
@@ -8815,7 +8800,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>451</v>
@@ -8840,170 +8825,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" t="s">
         <v>552</v>
-      </c>
-      <c r="B1" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B2" t="s">
         <v>554</v>
-      </c>
-      <c r="B2" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>555</v>
+      </c>
+      <c r="B3" t="s">
         <v>556</v>
-      </c>
-      <c r="B3" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>557</v>
+      </c>
+      <c r="B4" t="s">
         <v>558</v>
-      </c>
-      <c r="B4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>560</v>
+      </c>
+      <c r="B6" t="s">
         <v>561</v>
-      </c>
-      <c r="B6" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B7" t="s">
         <v>563</v>
-      </c>
-      <c r="B7" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>567</v>
+      </c>
+      <c r="B11" t="s">
         <v>568</v>
-      </c>
-      <c r="B11" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>569</v>
+      </c>
+      <c r="B12" t="s">
         <v>570</v>
-      </c>
-      <c r="B12" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>572</v>
+      </c>
+      <c r="B14" t="s">
         <v>573</v>
-      </c>
-      <c r="B14" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B17" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>577</v>
+      </c>
+      <c r="B18" t="s">
         <v>578</v>
-      </c>
-      <c r="B18" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>580</v>
+      </c>
+      <c r="B20" t="s">
         <v>581</v>
-      </c>
-      <c r="B20" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B21" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes and modification to the score of the conflict tasks.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="675">
   <si>
     <t>符号判断</t>
   </si>
@@ -2616,10 +2616,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CountTotalTrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>STIM RT ACC Resp\STIM RT ACC Resp SCat</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2657,6 +2653,24 @@
   </si>
   <si>
     <t>efficiency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Repeat Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRT_SwitchCost ACC_SwitchCost v_SwitchCost</t>
+  </si>
+  <si>
+    <t>NIHScore</t>
+  </si>
+  <si>
+    <t>NIHScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CountTotalTrl NIHScore</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3296,11 +3310,11 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4026,7 +4040,13 @@
       <c r="L13" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="M13" s="18"/>
+      <c r="M13" s="18" t="s">
+        <v>672</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>673</v>
+      </c>
       <c r="P13" s="22" t="s">
         <v>185</v>
       </c>
@@ -4079,10 +4099,10 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P14" s="21" t="s">
         <v>602</v>
@@ -4136,10 +4156,10 @@
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P15" s="21" t="s">
         <v>602</v>
@@ -4193,10 +4213,10 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P16" s="21" t="s">
         <v>602</v>
@@ -4250,10 +4270,10 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P17" s="21" t="s">
         <v>602</v>
@@ -4311,10 +4331,10 @@
         <v>169</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P18" s="21" t="s">
         <v>602</v>
@@ -4372,10 +4392,10 @@
         <v>169</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P19" s="21" t="s">
         <v>602</v>
@@ -4433,10 +4453,10 @@
         <v>169</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P20" s="21" t="s">
         <v>602</v>
@@ -4494,10 +4514,10 @@
         <v>169</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P21" s="21" t="s">
         <v>602</v>
@@ -4555,10 +4575,10 @@
         <v>196</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P22" s="21" t="s">
         <v>602</v>
@@ -4616,10 +4636,10 @@
         <v>196</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P23" s="21" t="s">
         <v>602</v>
@@ -4677,10 +4697,10 @@
         <v>196</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P24" s="21" t="s">
         <v>602</v>
@@ -4734,10 +4754,10 @@
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P25" s="21" t="s">
         <v>602</v>
@@ -4791,10 +4811,10 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P26" s="21" t="s">
         <v>602</v>
@@ -5253,7 +5273,10 @@
         <v>652</v>
       </c>
       <c r="M34" t="s">
-        <v>660</v>
+        <v>674</v>
+      </c>
+      <c r="O34" t="s">
+        <v>672</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>185</v>
@@ -5313,7 +5336,10 @@
         <v>652</v>
       </c>
       <c r="M35" t="s">
-        <v>660</v>
+        <v>674</v>
+      </c>
+      <c r="O35" t="s">
+        <v>672</v>
       </c>
       <c r="P35" s="22" t="s">
         <v>185</v>
@@ -5371,7 +5397,10 @@
         <v>652</v>
       </c>
       <c r="M36" t="s">
-        <v>660</v>
+        <v>674</v>
+      </c>
+      <c r="O36" t="s">
+        <v>672</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>185</v>
@@ -5413,7 +5442,7 @@
         <v>0.5</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>185</v>
+        <v>503</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>540</v>
@@ -5422,23 +5451,21 @@
         <v>651</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>653</v>
+        <v>670</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>654</v>
+        <v>671</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>652</v>
       </c>
       <c r="M37" t="s">
-        <v>660</v>
-      </c>
-      <c r="P37" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>655</v>
-      </c>
+        <v>674</v>
+      </c>
+      <c r="O37" t="s">
+        <v>672</v>
+      </c>
+      <c r="P37" s="22"/>
       <c r="R37" s="17">
         <v>3000</v>
       </c>
@@ -5796,17 +5823,17 @@
         <v>176</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="5" t="s">
         <v>642</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P44" s="22" t="s">
         <v>610</v>
@@ -5857,17 +5884,17 @@
         <v>179</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="5" t="s">
         <v>643</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="P45" s="22" t="s">
         <v>610</v>
@@ -5909,7 +5936,7 @@
         <v>0.5</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>544</v>
@@ -5925,7 +5952,7 @@
         <v>169</v>
       </c>
       <c r="O46" s="24" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P46" s="22"/>
       <c r="Q46" s="17" t="s">
@@ -7983,7 +8010,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Bug fixes in updating function.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="675">
   <si>
     <t>符号判断</t>
   </si>
@@ -3310,11 +3310,11 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -6051,6 +6051,9 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
+      <c r="O49" s="20" t="s">
+        <v>178</v>
+      </c>
       <c r="S49" s="2" t="s">
         <v>178</v>
       </c>

</xml_diff>

<commit_message>
Add new metadata variable. Add name variable.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -3309,7 +3309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
@@ -8363,22 +8363,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>200</v>
       </c>
@@ -8392,7 +8390,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -8407,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A11" si="0">ROW()-1</f>
         <v>2</v>
@@ -8421,11 +8419,8 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8440,7 +8435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8455,7 +8450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8470,7 +8465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8485,7 +8480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8500,7 +8495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8515,7 +8510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8530,7 +8525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8562,7 +8557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
BUGFIXES+MEWFEATURE: Polishing works and new feature for additional tasks (modified in taskSettings.xlsx): stop-signal, delay discounting, and so on.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Flanker" sheetId="16" r:id="rId15"/>
     <sheet name="TaskSwitching" sheetId="18" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <customWorkbookViews>
     <customWorkbookView name="psychezl - 个人视图" guid="{EA03B590-7847-4E8E-A1B2-851363113915}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1066" activeSheetId="1"/>
   </customWorkbookViews>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,10 +199,37 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>张亮</author>
     <author>psychezl</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张亮:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Serially presents the delimiters for trials, variables, and sub-variable conditions.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -311,12 +338,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="E28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张亮:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+SSD = Stop signal delay</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="708">
   <si>
     <t>符号判断</t>
   </si>
@@ -2209,10 +2260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>fmt</t>
   </si>
   <si>
@@ -2671,6 +2718,140 @@
   </si>
   <si>
     <t>CountTotalTrl NIHScore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红绿灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StopSignal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红绿灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宇宙加氧站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anticipation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宇宙加氧站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Session NTrl SCat IsStop Resp ACC RT SSD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ntrl SCat TimeOnset TimeResp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消灭敌机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TempDiscounting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H1 R1 H2 R2 Delay Resp RT CurUtility TotalUtility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记忆尾巴（空间位置）</t>
+  </si>
+  <si>
+    <t>MemoryTail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记忆尾巴（位置）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>垫江县桂溪小学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>垫江县桂溪小学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成都市龙泉驿区第五小学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成都市龙泉驿区第五小学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成都市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆市垫江县桂溪小学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙洞小学</t>
+  </si>
+  <si>
+    <t>广州市</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2678,7 +2859,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2858,6 +3039,19 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3307,14 +3501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3323,9 +3516,8 @@
     <col min="2" max="2" width="12.265625" customWidth="1"/>
     <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.73046875" customWidth="1"/>
-    <col min="7" max="7" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.73046875" customWidth="1"/>
     <col min="9" max="9" width="15" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.265625" customWidth="1"/>
     <col min="11" max="11" width="14.73046875" customWidth="1"/>
@@ -3353,17 +3545,17 @@
       <c r="D1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>27</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>539</v>
+        <v>645</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>236</v>
@@ -3384,16 +3576,16 @@
         <v>508</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>168</v>
@@ -3419,15 +3611,15 @@
       <c r="D2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2">
+      <c r="E2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>166</v>
@@ -3443,13 +3635,13 @@
         <v>536</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Q2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>188</v>
@@ -3475,15 +3667,15 @@
       <c r="D3" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
+      <c r="E3" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>166</v>
@@ -3499,13 +3691,13 @@
         <v>536</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Q3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>188</v>
@@ -3531,15 +3723,15 @@
       <c r="D4" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2">
+      <c r="E4" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>166</v>
@@ -3555,13 +3747,13 @@
         <v>536</v>
       </c>
       <c r="O4" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Q4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>188</v>
@@ -3587,15 +3779,15 @@
       <c r="D5" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2">
+      <c r="E5" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>166</v>
@@ -3611,13 +3803,13 @@
         <v>536</v>
       </c>
       <c r="O5" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Q5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>188</v>
@@ -3643,15 +3835,15 @@
       <c r="D6" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2">
+      <c r="E6" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>166</v>
@@ -3667,13 +3859,13 @@
         <v>536</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Q6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>188</v>
@@ -3699,15 +3891,15 @@
       <c r="D7" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
+      <c r="E7" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>166</v>
@@ -3723,13 +3915,13 @@
         <v>536</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="Q7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>188</v>
@@ -3755,21 +3947,21 @@
       <c r="D8" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="2" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="20"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>534</v>
@@ -3795,17 +3987,17 @@
       <c r="D9" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="29" t="s">
+        <v>547</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G9" s="7">
         <v>3000</v>
       </c>
-      <c r="F9" s="8">
+      <c r="H9" s="8">
         <v>0.5</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>547</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>174</v>
@@ -3817,16 +4009,16 @@
         <v>535</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q9" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>191</v>
@@ -3852,17 +4044,17 @@
       <c r="D10" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="27" t="s">
+        <v>547</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G10" s="7">
         <v>3000</v>
       </c>
-      <c r="F10" s="8">
+      <c r="H10" s="8">
         <v>0.5</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>547</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>174</v>
@@ -3874,16 +4066,16 @@
         <v>535</v>
       </c>
       <c r="O10" s="24" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="R10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>191</v>
@@ -3909,35 +4101,35 @@
       <c r="D11" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="27" t="s">
+        <v>587</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G11" s="8">
         <v>2000</v>
       </c>
-      <c r="F11" s="8">
+      <c r="H11" s="8">
         <v>0.5</v>
       </c>
-      <c r="G11" s="27" t="s">
-        <v>588</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I11" s="27" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="P11" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="R11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>193</v>
@@ -3963,34 +4155,34 @@
       <c r="D12" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="27" t="s">
+        <v>587</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G12" s="8">
         <v>3000</v>
       </c>
-      <c r="F12" s="8">
+      <c r="H12" s="8">
         <v>0.5</v>
-      </c>
-      <c r="G12" s="27" t="s">
-        <v>588</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>177</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="P12" s="21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Q12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="R12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>193</v>
@@ -4016,42 +4208,42 @@
       <c r="D13" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G13" s="10">
         <v>2000</v>
       </c>
-      <c r="F13" s="8">
+      <c r="H13" s="8">
         <v>0.5</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I13" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>652</v>
-      </c>
       <c r="M13" s="18" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="P13" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q13" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="R13">
         <v>3000</v>
@@ -4080,16 +4272,16 @@
       <c r="D14" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G14" s="2">
         <v>3000</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="20" t="s">
         <v>170</v>
       </c>
@@ -4099,19 +4291,19 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q14" t="s">
+        <v>621</v>
+      </c>
+      <c r="R14" t="s">
         <v>622</v>
-      </c>
-      <c r="R14" t="s">
-        <v>623</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>189</v>
@@ -4137,16 +4329,16 @@
       <c r="D15" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G15" s="2">
         <v>3000</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="20" t="s">
         <v>170</v>
       </c>
@@ -4156,19 +4348,19 @@
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q15" t="s">
+        <v>621</v>
+      </c>
+      <c r="R15" t="s">
         <v>622</v>
-      </c>
-      <c r="R15" t="s">
-        <v>623</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>189</v>
@@ -4194,16 +4386,16 @@
       <c r="D16" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G16" s="2">
         <v>3000</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="20" t="s">
         <v>170</v>
       </c>
@@ -4213,19 +4405,19 @@
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O16" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q16" t="s">
+        <v>621</v>
+      </c>
+      <c r="R16" t="s">
         <v>622</v>
-      </c>
-      <c r="R16" t="s">
-        <v>623</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>189</v>
@@ -4251,16 +4443,16 @@
       <c r="D17" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G17" s="2">
         <v>3000</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="20" t="s">
         <v>170</v>
       </c>
@@ -4270,19 +4462,19 @@
       </c>
       <c r="L17" s="2"/>
       <c r="M17" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q17" t="s">
+        <v>621</v>
+      </c>
+      <c r="R17" t="s">
         <v>622</v>
-      </c>
-      <c r="R17" t="s">
-        <v>623</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>189</v>
@@ -4308,17 +4500,17 @@
       <c r="D18" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="20" t="s">
+        <v>498</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G18" s="2">
         <v>3000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="H18" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>166</v>
@@ -4331,19 +4523,19 @@
         <v>169</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q18" s="31" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>188</v>
@@ -4369,17 +4561,17 @@
       <c r="D19" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="20" t="s">
+        <v>498</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G19" s="2">
         <v>3000</v>
       </c>
-      <c r="F19" s="2">
+      <c r="H19" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>166</v>
@@ -4392,19 +4584,19 @@
         <v>169</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>188</v>
@@ -4430,17 +4622,17 @@
       <c r="D20" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="20" t="s">
+        <v>498</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G20" s="2">
         <v>3000</v>
       </c>
-      <c r="F20" s="2">
+      <c r="H20" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>166</v>
@@ -4453,19 +4645,19 @@
         <v>169</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q20" s="31" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="R20" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>188</v>
@@ -4491,17 +4683,17 @@
       <c r="D21" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="20" t="s">
+        <v>498</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G21" s="2">
         <v>3000</v>
       </c>
-      <c r="F21" s="2">
+      <c r="H21" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>166</v>
@@ -4514,19 +4706,19 @@
         <v>169</v>
       </c>
       <c r="M21" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>188</v>
@@ -4552,17 +4744,17 @@
       <c r="D22" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G22" s="2">
         <v>3000</v>
       </c>
-      <c r="F22" s="2">
+      <c r="H22" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>170</v>
@@ -4575,19 +4767,19 @@
         <v>196</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q22" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R22" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>191</v>
@@ -4613,17 +4805,17 @@
       <c r="D23" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G23" s="2">
         <v>3000</v>
       </c>
-      <c r="F23" s="2">
+      <c r="H23" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>170</v>
@@ -4636,19 +4828,19 @@
         <v>196</v>
       </c>
       <c r="M23" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P23" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q23" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R23" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>191</v>
@@ -4674,17 +4866,17 @@
       <c r="D24" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G24" s="2">
         <v>3000</v>
       </c>
-      <c r="F24" s="2">
+      <c r="H24" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>170</v>
@@ -4697,19 +4889,19 @@
         <v>196</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P24" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q24" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R24" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>191</v>
@@ -4735,16 +4927,16 @@
       <c r="D25" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G25" s="2">
         <v>3000</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H25" s="2"/>
       <c r="I25" s="20" t="s">
         <v>170</v>
       </c>
@@ -4754,19 +4946,19 @@
       </c>
       <c r="L25" s="2"/>
       <c r="M25" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P25" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q25" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>191</v>
@@ -4792,16 +4984,16 @@
       <c r="D26" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G26" s="2">
         <v>1000</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H26" s="2"/>
       <c r="I26" s="20" t="s">
         <v>170</v>
       </c>
@@ -4811,19 +5003,19 @@
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P26" s="21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="Q26" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R26" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>191</v>
@@ -4849,31 +5041,31 @@
       <c r="D27" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
       <c r="I27" s="28" t="s">
         <v>175</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="M27" s="19"/>
       <c r="O27" s="24" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R27">
         <v>600</v>
@@ -4902,16 +5094,16 @@
       <c r="D28" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G28" s="5">
         <v>1000</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="20" t="s">
         <v>166</v>
       </c>
@@ -4920,17 +5112,17 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="M28" s="19"/>
       <c r="O28" s="24" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="P28" s="21" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>188</v>
@@ -4956,16 +5148,16 @@
       <c r="D29" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G29" s="5">
         <v>500</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>540</v>
-      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="20" t="s">
         <v>505</v>
       </c>
@@ -4978,13 +5170,13 @@
       </c>
       <c r="M29" s="10"/>
       <c r="O29" s="25" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="S29" s="2" t="s">
         <v>507</v>
@@ -5010,17 +5202,17 @@
       <c r="D30" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="G30" s="5">
         <v>1000</v>
       </c>
-      <c r="F30" s="5">
+      <c r="H30" s="5">
         <v>0.5</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>504</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>542</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>166</v>
@@ -5037,16 +5229,16 @@
         <v>509</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="P30" s="22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q30" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="R30" s="17" t="s">
         <v>630</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>631</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>188</v>
@@ -5072,17 +5264,17 @@
       <c r="D31" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="G31" s="5">
         <v>1000</v>
       </c>
-      <c r="F31" s="5">
+      <c r="H31" s="5">
         <v>0.5</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>504</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>542</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>166</v>
@@ -5099,16 +5291,16 @@
         <v>509</v>
       </c>
       <c r="O31" s="26" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="P31" s="22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q31" s="17" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>188</v>
@@ -5134,17 +5326,17 @@
       <c r="D32" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="20" t="s">
+        <v>493</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G32" s="2">
         <v>2000</v>
       </c>
-      <c r="F32" s="2">
+      <c r="H32" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>493</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>166</v>
@@ -5158,13 +5350,13 @@
       </c>
       <c r="M32" s="19"/>
       <c r="O32" s="26" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P32" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R32" s="17"/>
       <c r="S32" s="2" t="s">
@@ -5191,17 +5383,17 @@
       <c r="D33" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="20" t="s">
+        <v>494</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G33" s="2">
         <v>0</v>
       </c>
-      <c r="F33" s="2">
+      <c r="H33" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>494</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>166</v>
@@ -5215,13 +5407,13 @@
       </c>
       <c r="M33" s="19"/>
       <c r="O33" s="26" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P33" s="22" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Q33" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="R33" s="17"/>
       <c r="S33" s="2" t="s">
@@ -5236,7 +5428,7 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <f t="shared" ref="A34:A51" si="1">ROW() - 1</f>
+        <f t="shared" ref="A34:A55" si="1">ROW() - 1</f>
         <v>33</v>
       </c>
       <c r="B34" s="34" t="s">
@@ -5248,41 +5440,41 @@
       <c r="D34" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G34" s="2">
         <v>3000</v>
       </c>
-      <c r="F34" s="2">
+      <c r="H34" s="2">
         <v>0.5</v>
       </c>
-      <c r="G34" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I34" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="L34" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>652</v>
-      </c>
       <c r="M34" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O34" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q34" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="R34" s="17">
         <v>2000</v>
@@ -5311,41 +5503,41 @@
       <c r="D35" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G35" s="2">
         <v>3000</v>
       </c>
-      <c r="F35" s="2">
+      <c r="H35" s="2">
         <v>0.25</v>
       </c>
-      <c r="G35" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I35" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>652</v>
-      </c>
       <c r="M35" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O35" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="P35" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q35" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="R35" s="17">
         <v>3000</v>
@@ -5374,39 +5566,39 @@
       <c r="D36" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2">
+      <c r="E36" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2">
         <v>0.25</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I36" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="L36" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>652</v>
-      </c>
       <c r="M36" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O36" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>185</v>
       </c>
       <c r="Q36" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="R36" s="17">
         <v>3000</v>
@@ -5435,35 +5627,35 @@
       <c r="D37" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G37" s="2">
         <v>3000</v>
       </c>
-      <c r="F37" s="2">
+      <c r="H37" s="2">
         <v>0.5</v>
       </c>
-      <c r="G37" s="20" t="s">
-        <v>503</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I37" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="K37" s="5" t="s">
+      <c r="M37" t="s">
+        <v>673</v>
+      </c>
+      <c r="O37" t="s">
         <v>671</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>652</v>
-      </c>
-      <c r="M37" t="s">
-        <v>674</v>
-      </c>
-      <c r="O37" t="s">
-        <v>672</v>
       </c>
       <c r="P37" s="22"/>
       <c r="R37" s="17">
@@ -5493,35 +5685,35 @@
       <c r="D38" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="28" t="s">
+        <v>547</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G38" s="2">
         <v>2000</v>
       </c>
-      <c r="F38" s="2">
+      <c r="H38" s="2">
         <v>0.5</v>
       </c>
-      <c r="G38" s="28" t="s">
-        <v>547</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I38" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="O38" s="24" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P38" s="22" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R38" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="S38" s="2" t="s">
         <v>189</v>
@@ -5547,35 +5739,35 @@
       <c r="D39" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G39" s="2">
         <v>2000</v>
       </c>
-      <c r="F39" s="2">
+      <c r="H39" s="2">
         <v>0.5</v>
       </c>
-      <c r="G39" s="30" t="s">
-        <v>547</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="I39" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="O39" s="24" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P39" s="22" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Q39" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="R39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="S39" s="2" t="s">
         <v>189</v>
@@ -5601,14 +5793,14 @@
       <c r="D40" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="20" t="s">
+      <c r="E40" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
       <c r="I40" s="28" t="s">
         <v>175</v>
       </c>
@@ -5616,13 +5808,13 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="O40" s="24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P40" s="22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="Q40" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R40" s="17">
         <v>400</v>
@@ -5651,14 +5843,14 @@
       <c r="D41" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="20" t="s">
+      <c r="E41" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
       <c r="I41" s="28" t="s">
         <v>175</v>
       </c>
@@ -5666,13 +5858,13 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="O41" s="24" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P41" s="22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="Q41" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R41" s="17">
         <v>500</v>
@@ -5693,7 +5885,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>118</v>
@@ -5701,14 +5893,14 @@
       <c r="D42" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="20" t="s">
+      <c r="E42" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
       <c r="I42" s="28" t="s">
         <v>175</v>
       </c>
@@ -5716,13 +5908,13 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="O42" s="24" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P42" s="22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="Q42" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="R42" s="17">
         <v>600</v>
@@ -5751,17 +5943,17 @@
       <c r="D43" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G43" s="2">
         <v>2000</v>
       </c>
-      <c r="F43" s="2">
+      <c r="H43" s="2">
         <v>0.25</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>187</v>
@@ -5772,16 +5964,16 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="O43" s="24" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="P43" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q43" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="R43" s="17" t="s">
         <v>636</v>
-      </c>
-      <c r="R43" s="17" t="s">
-        <v>637</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>193</v>
@@ -5807,42 +5999,42 @@
       <c r="D44" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G44" s="2">
         <v>2000</v>
       </c>
-      <c r="F44" s="2">
+      <c r="H44" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I44" s="28" t="s">
         <v>176</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="P44" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q44" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="R44" s="17" t="s">
         <v>638</v>
-      </c>
-      <c r="R44" s="17" t="s">
-        <v>639</v>
       </c>
       <c r="S44" s="2" t="s">
         <v>520</v>
@@ -5868,42 +6060,42 @@
       <c r="D45" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G45" s="2">
         <v>2000</v>
       </c>
-      <c r="F45" s="2">
+      <c r="H45" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="I45" s="28" t="s">
         <v>179</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P45" s="22" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="Q45" s="17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="S45" s="2" t="s">
         <v>520</v>
@@ -5929,17 +6121,17 @@
       <c r="D46" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="20" t="s">
+        <v>666</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="G46" s="2">
         <v>2000</v>
       </c>
-      <c r="F46" s="2">
+      <c r="H46" s="2">
         <v>0.5</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>544</v>
       </c>
       <c r="I46" s="20" t="s">
         <v>166</v>
@@ -5952,14 +6144,14 @@
         <v>169</v>
       </c>
       <c r="O46" s="24" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="P46" s="22"/>
       <c r="Q46" s="17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>193</v>
@@ -5985,12 +6177,12 @@
       <c r="D47" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="2" t="s">
+      <c r="E47" s="20"/>
+      <c r="F47" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
       <c r="I47" s="20"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -6011,12 +6203,12 @@
       <c r="D48" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="2" t="s">
+      <c r="E48" s="20"/>
+      <c r="F48" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
       <c r="I48" s="20"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
@@ -6037,14 +6229,14 @@
       <c r="D49" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="20" t="s">
+      <c r="E49" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
       <c r="I49" s="20" t="s">
         <v>178</v>
       </c>
@@ -6072,9 +6264,9 @@
       <c r="D50" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="20"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="20"/>
+      <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="20"/>
       <c r="J50" s="2"/>
@@ -6096,9 +6288,9 @@
       <c r="D51" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="20"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="20"/>
+      <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="20"/>
       <c r="J51" s="2"/>
@@ -6106,8 +6298,68 @@
       <c r="L51" s="2"/>
       <c r="S51" s="2"/>
     </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="C53" t="s">
+        <v>680</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C54" t="s">
+        <v>688</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>692</v>
+      </c>
+      <c r="C55" t="s">
+        <v>693</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>694</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:W51">
+  <sortState ref="A2:Y51">
     <sortCondition ref="T2:T51"/>
   </sortState>
   <customSheetViews>
@@ -7735,10 +7987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -7824,7 +8076,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A27" si="0">ROW() - 1</f>
+        <f t="shared" ref="A4:A31" si="0">ROW() - 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -7903,7 +8155,7 @@
         <v>62</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -7925,7 +8177,7 @@
         <v>62</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -7947,7 +8199,7 @@
         <v>60</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -8013,7 +8265,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -8345,6 +8597,75 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>695</v>
+      </c>
     </row>
   </sheetData>
   <customSheetViews>
@@ -8363,10 +8684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -8387,7 +8708,7 @@
         <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>550</v>
+        <v>697</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -8401,13 +8722,13 @@
       <c r="C2" t="s">
         <v>212</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" ref="A3:A11" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A15" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -8416,8 +8737,8 @@
       <c r="C3" t="s">
         <v>213</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -8431,8 +8752,8 @@
       <c r="C4" t="s">
         <v>211</v>
       </c>
-      <c r="D4">
-        <v>2</v>
+      <c r="D4" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -8446,8 +8767,8 @@
       <c r="C5" t="s">
         <v>207</v>
       </c>
-      <c r="D5">
-        <v>2</v>
+      <c r="D5" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8461,8 +8782,8 @@
       <c r="C6" t="s">
         <v>209</v>
       </c>
-      <c r="D6">
-        <v>3</v>
+      <c r="D6" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -8471,13 +8792,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>649</v>
       </c>
       <c r="C7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
+        <v>649</v>
+      </c>
+      <c r="D7" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8486,13 +8807,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="C8" t="s">
-        <v>650</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
+        <v>701</v>
+      </c>
+      <c r="D8" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8501,13 +8822,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>705</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
+        <v>701</v>
+      </c>
+      <c r="D9" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -8516,13 +8837,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>702</v>
       </c>
       <c r="C10" t="s">
-        <v>210</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
+        <v>703</v>
+      </c>
+      <c r="D10" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8531,13 +8852,73 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>647</v>
+      </c>
+      <c r="C14" t="s">
         <v>648</v>
       </c>
-      <c r="C11" t="s">
-        <v>649</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
+      <c r="D14" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>706</v>
+      </c>
+      <c r="C15" t="s">
+        <v>706</v>
+      </c>
+      <c r="D15" t="s">
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -8557,7 +8938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
@@ -8748,7 +9129,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B1" t="s">
         <v>530</v>
@@ -8850,170 +9231,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B1" t="s">
         <v>551</v>
-      </c>
-      <c r="B1" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B2" t="s">
         <v>553</v>
-      </c>
-      <c r="B2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>554</v>
+      </c>
+      <c r="B3" t="s">
         <v>555</v>
-      </c>
-      <c r="B3" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B4" t="s">
         <v>557</v>
-      </c>
-      <c r="B4" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>559</v>
+      </c>
+      <c r="B6" t="s">
         <v>560</v>
-      </c>
-      <c r="B6" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>561</v>
+      </c>
+      <c r="B7" t="s">
         <v>562</v>
-      </c>
-      <c r="B7" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B8" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B10" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>566</v>
+      </c>
+      <c r="B11" t="s">
         <v>567</v>
-      </c>
-      <c r="B11" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>568</v>
+      </c>
+      <c r="B12" t="s">
         <v>569</v>
-      </c>
-      <c r="B12" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>571</v>
+      </c>
+      <c r="B14" t="s">
         <v>572</v>
-      </c>
-      <c r="B14" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B16" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B18" t="s">
         <v>577</v>
-      </c>
-      <c r="B18" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B19" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>579</v>
+      </c>
+      <c r="B20" t="s">
         <v>580</v>
-      </c>
-      <c r="B20" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B21" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD FEATURE Add support for repetition test.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="827">
   <si>
     <t>符号判断</t>
   </si>
@@ -3253,6 +3253,14 @@
   </si>
   <si>
     <t>Memsep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3936,7 +3944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10530,10 +10538,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -10701,6 +10709,78 @@
         <v>九年级</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>440</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FIX BUGS: Compatibility & Better Performance Compatibility fix in Merges.m; Better performance in outlier.m (renamed from coutlier.m).
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="834">
   <si>
     <t>符号判断</t>
   </si>
@@ -3261,6 +3261,34 @@
   </si>
   <si>
     <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attention</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thinking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3501,7 +3529,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3629,12 +3657,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -3942,13 +3964,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q40" sqref="Q40"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3956,24 +3978,26 @@
     <col min="1" max="1" width="3.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.265625" customWidth="1"/>
     <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.73046875" customWidth="1"/>
-    <col min="9" max="9" width="15" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.265625" customWidth="1"/>
-    <col min="11" max="11" width="14.73046875" customWidth="1"/>
-    <col min="12" max="12" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" customWidth="1"/>
-    <col min="14" max="14" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.46484375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="57.1328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1328125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.1328125" customWidth="1"/>
+    <col min="6" max="6" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.73046875" customWidth="1"/>
+    <col min="11" max="11" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.265625" customWidth="1"/>
+    <col min="13" max="13" width="14.73046875" customWidth="1"/>
+    <col min="14" max="14" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.73046875" customWidth="1"/>
+    <col min="16" max="16" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.46484375" style="21" customWidth="1"/>
+    <col min="19" max="19" width="57.1328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="37.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -3983,62 +4007,68 @@
       <c r="C1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="41" t="s">
+        <v>692</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>693</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>576</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>616</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -4049,52 +4079,56 @@
       <c r="C2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
         <v>0.5</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="R2" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>602</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4105,52 +4139,56 @@
       <c r="C3" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="G3" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
         <v>0.5</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="K3" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="Q3" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>602</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4161,52 +4199,56 @@
       <c r="C4" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="G4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
         <v>0.5</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="K4" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="Q4" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="R4" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>602</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4217,52 +4259,56 @@
       <c r="C5" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="G5" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
         <v>0.5</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="K5" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="Q5" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="R5" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>602</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4273,52 +4319,56 @@
       <c r="C6" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="G6" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
         <v>0.5</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="K6" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2"/>
+      <c r="N6" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="Q6" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="R6" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>602</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4329,52 +4379,56 @@
       <c r="C7" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
         <v>0.5</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="Q7" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="R7" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>602</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7" t="s">
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4385,36 +4439,40 @@
       <c r="C8" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="20"/>
+      <c r="H8" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="2"/>
-      <c r="M8" t="s">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" t="s">
         <v>578</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="Q8" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4425,53 +4483,57 @@
       <c r="C9" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="42" t="s">
+        <v>828</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="G9" s="29" t="s">
         <v>535</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G9" s="7">
+      <c r="I9" s="7">
         <v>3000</v>
       </c>
-      <c r="H9" s="8">
+      <c r="J9" s="8">
         <v>0.5</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="K9" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
       <c r="L9" s="8"/>
-      <c r="M9" t="s">
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" t="s">
         <v>524</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="Q9" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="R9" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>603</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>599</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="U9" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="T9">
-        <v>2</v>
-      </c>
-      <c r="U9" t="s">
+      <c r="V9">
+        <v>2</v>
+      </c>
+      <c r="W9" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4482,53 +4544,57 @@
       <c r="C10" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="42" t="s">
+        <v>828</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="G10" s="27" t="s">
         <v>535</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G10" s="7">
+      <c r="I10" s="7">
         <v>3000</v>
       </c>
-      <c r="H10" s="8">
+      <c r="J10" s="8">
         <v>0.5</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="K10" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" t="s">
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" t="s">
         <v>524</v>
       </c>
-      <c r="O10" s="24" t="s">
+      <c r="Q10" s="24" t="s">
         <v>581</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="R10" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>603</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>599</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="U10" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="T10">
-        <v>2</v>
-      </c>
-      <c r="U10" t="s">
+      <c r="V10">
+        <v>2</v>
+      </c>
+      <c r="W10" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4539,52 +4605,56 @@
       <c r="C11" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="42" t="s">
+        <v>828</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="G11" s="27" t="s">
         <v>575</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G11" s="8">
+      <c r="I11" s="8">
         <v>2000</v>
       </c>
-      <c r="H11" s="8">
+      <c r="J11" s="8">
         <v>0.5</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="K11" s="27" t="s">
         <v>605</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="L11" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="21" t="s">
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>606</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>599</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="U11" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="T11">
-        <v>2</v>
-      </c>
-      <c r="U11" t="s">
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="W11" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4595,51 +4665,55 @@
       <c r="C12" s="14" t="s">
         <v>526</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="42" t="s">
+        <v>828</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="G12" s="27" t="s">
         <v>575</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G12" s="8">
+      <c r="I12" s="8">
         <v>3000</v>
       </c>
-      <c r="H12" s="8">
+      <c r="J12" s="8">
         <v>0.5</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="K12" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="21" t="s">
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>607</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>600</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="U12" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="T12">
-        <v>2</v>
-      </c>
-      <c r="U12" t="s">
+      <c r="V12">
+        <v>2</v>
+      </c>
+      <c r="W12" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4650,60 +4724,64 @@
       <c r="C13" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="42" t="s">
+        <v>829</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="G13" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G13" s="10">
+      <c r="I13" s="10">
         <v>2000</v>
       </c>
-      <c r="H13" s="8">
+      <c r="J13" s="8">
         <v>0.5</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="K13" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M13" s="18" t="s">
+      <c r="O13" s="18" t="s">
         <v>658</v>
       </c>
-      <c r="N13" s="40"/>
-      <c r="O13" s="5" t="s">
+      <c r="P13" s="40"/>
+      <c r="Q13" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="R13" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>642</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>3000</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="U13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="T13">
-        <v>2</v>
-      </c>
-      <c r="U13" t="s">
+      <c r="V13">
+        <v>2</v>
+      </c>
+      <c r="W13" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4714,54 +4792,58 @@
       <c r="C14" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="G14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G14" s="2">
+      <c r="I14" s="2">
         <v>3000</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="2"/>
+      <c r="K14" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="N14" s="39"/>
+      <c r="N14" s="2"/>
       <c r="O14" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="39"/>
+      <c r="Q14" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="R14" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>609</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>610</v>
       </c>
-      <c r="S14" s="2" t="s">
+      <c r="U14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>3</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4772,58 +4854,62 @@
       <c r="C15" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="G15" s="20" t="s">
         <v>487</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G15" s="2">
+      <c r="I15" s="2">
         <v>3000</v>
       </c>
-      <c r="H15" s="2">
+      <c r="J15" s="2">
         <v>0.5</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="K15" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M15" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="N15" s="39"/>
       <c r="O15" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="39"/>
+      <c r="Q15" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="R15" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="Q15" s="31" t="s">
+      <c r="S15" s="31" t="s">
         <v>614</v>
       </c>
-      <c r="R15" s="32" t="s">
+      <c r="T15" s="32" t="s">
         <v>611</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="U15" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>3</v>
       </c>
-      <c r="U15" t="s">
+      <c r="W15" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4834,58 +4920,62 @@
       <c r="C16" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="G16" s="20" t="s">
         <v>535</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G16" s="2">
+      <c r="I16" s="2">
         <v>3000</v>
       </c>
-      <c r="H16" s="2">
+      <c r="J16" s="2">
         <v>0.5</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="K16" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="M16" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="N16" s="39"/>
       <c r="O16" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P16" s="21" t="s">
+      <c r="P16" s="39"/>
+      <c r="Q16" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="R16" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>609</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>612</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="U16" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>3</v>
       </c>
-      <c r="U16" t="s">
+      <c r="W16" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4896,54 +4986,58 @@
       <c r="C17" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G17" s="2">
+      <c r="I17" s="2">
         <v>3000</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="20" t="s">
+      <c r="J17" s="2"/>
+      <c r="K17" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="N17" s="39"/>
+      <c r="N17" s="2"/>
       <c r="O17" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P17" s="21" t="s">
+      <c r="P17" s="39"/>
+      <c r="Q17" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="R17" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>609</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>613</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="T17">
+      <c r="V17">
         <v>3</v>
       </c>
-      <c r="U17" t="s">
+      <c r="W17" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4954,54 +5048,58 @@
       <c r="C18" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="42" t="s">
+        <v>827</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="G18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G18" s="2">
+      <c r="I18" s="2">
         <v>1000</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="20" t="s">
+      <c r="J18" s="2"/>
+      <c r="K18" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="17" t="s">
-        <v>655</v>
-      </c>
-      <c r="N18" s="39"/>
+      <c r="N18" s="2"/>
       <c r="O18" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P18" s="21" t="s">
+      <c r="P18" s="39"/>
+      <c r="Q18" s="17" t="s">
+        <v>655</v>
+      </c>
+      <c r="R18" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="S18" t="s">
         <v>609</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>599</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>3</v>
       </c>
-      <c r="U18" t="s">
+      <c r="W18" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5012,50 +5110,54 @@
       <c r="C19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="G19" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="5" t="s">
         <v>621</v>
       </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39" t="s">
+      <c r="O19" s="19"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39" t="s">
         <v>579</v>
       </c>
-      <c r="P19" s="21" t="s">
+      <c r="R19" s="21" t="s">
         <v>590</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="S19" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>600</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="U19" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>4</v>
       </c>
-      <c r="U19" t="s">
+      <c r="W19" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5066,51 +5168,55 @@
       <c r="C20" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="G20" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G20" s="5">
+      <c r="I20" s="5">
         <v>1000</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="20" t="s">
+      <c r="J20" s="5"/>
+      <c r="K20" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39" t="s">
+      <c r="O20" s="19"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39" t="s">
         <v>646</v>
       </c>
-      <c r="P20" s="21" t="s">
+      <c r="R20" s="21" t="s">
         <v>591</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="S20" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="U20" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>4</v>
       </c>
-      <c r="U20" t="s">
+      <c r="W20" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5121,50 +5227,54 @@
       <c r="C21" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="G21" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G21" s="5">
+      <c r="I21" s="5">
         <v>500</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="20" t="s">
+      <c r="J21" s="5"/>
+      <c r="K21" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="L21" s="18" t="s">
+      <c r="M21" s="10"/>
+      <c r="N21" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="O21" s="25" t="s">
+      <c r="O21" s="10"/>
+      <c r="Q21" s="25" t="s">
         <v>580</v>
       </c>
-      <c r="P21" s="21" t="s">
+      <c r="R21" s="21" t="s">
         <v>591</v>
       </c>
-      <c r="Q21" s="5" t="s">
+      <c r="S21" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>4</v>
       </c>
-      <c r="U21" t="s">
+      <c r="W21" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5175,58 +5285,62 @@
       <c r="C22" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="G22" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="G22" s="5">
+      <c r="I22" s="5">
         <v>1000</v>
       </c>
-      <c r="H22" s="5">
+      <c r="J22" s="5">
         <v>0.5</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="K22" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M22" s="19"/>
-      <c r="N22" t="s">
+      <c r="O22" s="19"/>
+      <c r="P22" t="s">
         <v>498</v>
       </c>
-      <c r="O22" s="26" t="s">
+      <c r="Q22" s="26" t="s">
         <v>632</v>
       </c>
-      <c r="P22" s="22" t="s">
+      <c r="R22" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="Q22" s="17" t="s">
+      <c r="S22" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="R22" s="17" t="s">
+      <c r="T22" s="17" t="s">
         <v>618</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>4</v>
       </c>
-      <c r="U22" t="s">
+      <c r="W22" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5237,58 +5351,62 @@
       <c r="C23" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="G23" s="5">
+      <c r="I23" s="5">
         <v>1000</v>
       </c>
-      <c r="H23" s="5">
+      <c r="J23" s="5">
         <v>0.5</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="K23" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="M23" s="19"/>
-      <c r="N23" t="s">
+      <c r="O23" s="19"/>
+      <c r="P23" t="s">
         <v>498</v>
       </c>
-      <c r="O23" s="26" t="s">
+      <c r="Q23" s="26" t="s">
         <v>632</v>
       </c>
-      <c r="P23" s="22" t="s">
+      <c r="R23" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="Q23" s="17" t="s">
+      <c r="S23" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="R23" s="17" t="s">
+      <c r="T23" s="17" t="s">
         <v>619</v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="U23" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>4</v>
       </c>
-      <c r="U23" t="s">
+      <c r="W23" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5299,53 +5417,57 @@
       <c r="C24" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="G24" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G24" s="2">
+      <c r="I24" s="2">
         <v>2000</v>
       </c>
-      <c r="H24" s="2">
+      <c r="J24" s="2">
         <v>0.5</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="K24" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2"/>
+      <c r="N24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M24" s="19"/>
-      <c r="O24" s="26" t="s">
+      <c r="O24" s="19"/>
+      <c r="Q24" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="P24" s="22" t="s">
+      <c r="R24" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="S24" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="R24" s="17"/>
-      <c r="S24" s="2" t="s">
+      <c r="T24" s="17"/>
+      <c r="U24" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>5</v>
       </c>
-      <c r="U24" t="s">
+      <c r="W24" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5356,53 +5478,57 @@
       <c r="C25" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G25" s="2">
+      <c r="I25" s="2">
         <v>0</v>
       </c>
-      <c r="H25" s="2">
+      <c r="J25" s="2">
         <v>0.5</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="K25" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2" t="s">
+      <c r="M25" s="2"/>
+      <c r="N25" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M25" s="19"/>
-      <c r="O25" s="26" t="s">
+      <c r="O25" s="19"/>
+      <c r="Q25" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="P25" s="22" t="s">
+      <c r="R25" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="Q25" s="5" t="s">
+      <c r="S25" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="R25" s="17"/>
-      <c r="S25" s="2" t="s">
+      <c r="T25" s="17"/>
+      <c r="U25" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>5</v>
       </c>
-      <c r="U25" t="s">
+      <c r="W25" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5413,59 +5539,63 @@
       <c r="C26" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="G26" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G26" s="2">
+      <c r="I26" s="2">
         <v>3000</v>
       </c>
-      <c r="H26" s="2">
+      <c r="J26" s="2">
         <v>0.5</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="K26" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="L26" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="N26" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>660</v>
       </c>
-      <c r="O26" t="s">
+      <c r="Q26" t="s">
         <v>658</v>
       </c>
-      <c r="P26" s="22" t="s">
+      <c r="R26" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="S26" t="s">
         <v>642</v>
       </c>
-      <c r="R26" s="17">
+      <c r="T26" s="17">
         <v>2000</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="U26" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <v>5</v>
       </c>
-      <c r="U26" t="s">
+      <c r="W26" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5476,59 +5606,63 @@
       <c r="C27" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G27" s="2">
+      <c r="I27" s="2">
         <v>3000</v>
       </c>
-      <c r="H27" s="2">
+      <c r="J27" s="2">
         <v>0.25</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="K27" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="N27" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>660</v>
       </c>
-      <c r="O27" t="s">
+      <c r="Q27" t="s">
         <v>658</v>
       </c>
-      <c r="P27" s="22" t="s">
+      <c r="R27" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="S27" t="s">
         <v>642</v>
       </c>
-      <c r="R27" s="17">
+      <c r="T27" s="17">
         <v>3000</v>
       </c>
-      <c r="S27" s="2" t="s">
+      <c r="U27" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="T27">
+      <c r="V27">
         <v>5</v>
       </c>
-      <c r="U27" t="s">
+      <c r="W27" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5539,57 +5673,61 @@
       <c r="C28" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2">
         <v>0.25</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="K28" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="M28" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="N28" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>660</v>
       </c>
-      <c r="O28" t="s">
+      <c r="Q28" t="s">
         <v>658</v>
       </c>
-      <c r="P28" s="22" t="s">
+      <c r="R28" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="S28" t="s">
         <v>642</v>
       </c>
-      <c r="R28" s="17">
+      <c r="T28" s="17">
         <v>3000</v>
       </c>
-      <c r="S28" s="2" t="s">
+      <c r="U28" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>5</v>
       </c>
-      <c r="U28" t="s">
+      <c r="W28" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5600,54 +5738,58 @@
       <c r="C29" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="42" t="s">
+        <v>832</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G29" s="2">
+      <c r="I29" s="2">
         <v>3000</v>
       </c>
-      <c r="H29" s="2">
+      <c r="J29" s="2">
         <v>0.5</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="K29" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="M29" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="N29" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
         <v>660</v>
       </c>
-      <c r="O29" t="s">
+      <c r="Q29" t="s">
         <v>658</v>
       </c>
-      <c r="P29" s="22"/>
-      <c r="R29" s="17">
+      <c r="R29" s="22"/>
+      <c r="T29" s="17">
         <v>3000</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="U29" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <v>5</v>
       </c>
-      <c r="U29" t="s">
+      <c r="W29" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5658,54 +5800,58 @@
       <c r="C30" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="42" t="s">
+        <v>832</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="23" t="s">
         <v>695</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G30" s="2">
+      <c r="I30" s="2">
         <v>3000</v>
       </c>
-      <c r="H30" s="2">
+      <c r="J30" s="2">
         <v>0.5</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="K30" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="L30" s="5" t="s">
+      <c r="N30" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>660</v>
       </c>
-      <c r="O30" t="s">
+      <c r="Q30" t="s">
         <v>658</v>
       </c>
-      <c r="P30" s="22"/>
-      <c r="R30" s="17">
+      <c r="R30" s="22"/>
+      <c r="T30" s="17">
         <v>3000</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="U30" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <v>5</v>
       </c>
-      <c r="U30" t="s">
+      <c r="W30" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5716,50 +5862,54 @@
       <c r="C31" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="G31" s="28" t="s">
         <v>535</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G31" s="2">
+      <c r="I31" s="2">
         <v>2000</v>
       </c>
-      <c r="H31" s="2">
+      <c r="J31" s="2">
         <v>0.5</v>
       </c>
-      <c r="I31" s="20" t="s">
+      <c r="K31" s="20" t="s">
         <v>570</v>
       </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="O31" s="24" t="s">
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="Q31" s="24" t="s">
         <v>582</v>
       </c>
-      <c r="P31" s="22" t="s">
+      <c r="R31" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="S31" t="s">
         <v>609</v>
       </c>
-      <c r="R31" t="s">
+      <c r="T31" t="s">
         <v>620</v>
       </c>
-      <c r="S31" s="2" t="s">
+      <c r="U31" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="T31">
+      <c r="V31">
         <v>5</v>
       </c>
-      <c r="U31" t="s">
+      <c r="W31" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5770,50 +5920,54 @@
       <c r="C32" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="42" t="s">
+        <v>831</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="G32" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G32" s="2">
+      <c r="I32" s="2">
         <v>2000</v>
       </c>
-      <c r="H32" s="2">
+      <c r="J32" s="2">
         <v>0.5</v>
       </c>
-      <c r="I32" s="20" t="s">
+      <c r="K32" s="20" t="s">
         <v>571</v>
       </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="O32" s="24" t="s">
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="Q32" s="24" t="s">
         <v>583</v>
       </c>
-      <c r="P32" s="22" t="s">
+      <c r="R32" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="S32" t="s">
         <v>609</v>
       </c>
-      <c r="R32" t="s">
+      <c r="T32" t="s">
         <v>620</v>
       </c>
-      <c r="S32" s="2" t="s">
+      <c r="U32" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="T32">
+      <c r="V32">
         <v>5</v>
       </c>
-      <c r="U32" t="s">
+      <c r="W32" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -5824,46 +5978,50 @@
       <c r="C33" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="28" t="s">
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="O33" s="24" t="s">
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="Q33" s="24" t="s">
         <v>584</v>
       </c>
-      <c r="P33" s="22" t="s">
+      <c r="R33" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="Q33" s="5" t="s">
+      <c r="S33" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="R33" s="17">
+      <c r="T33" s="17">
         <v>400</v>
       </c>
-      <c r="S33" s="2" t="s">
+      <c r="U33" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="T33">
+      <c r="V33">
         <v>6</v>
       </c>
-      <c r="U33" t="s">
+      <c r="W33" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A53" si="1">ROW() - 1</f>
         <v>33</v>
@@ -5874,46 +6032,50 @@
       <c r="C34" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="O34" s="24" t="s">
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="Q34" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="P34" s="22" t="s">
+      <c r="R34" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="Q34" s="5" t="s">
+      <c r="S34" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="R34" s="17">
+      <c r="T34" s="17">
         <v>500</v>
       </c>
-      <c r="S34" s="2" t="s">
+      <c r="U34" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="T34">
+      <c r="V34">
         <v>6</v>
       </c>
-      <c r="U34" t="s">
+      <c r="W34" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -5924,46 +6086,50 @@
       <c r="C35" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="28" t="s">
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="O35" s="24" t="s">
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="Q35" s="24" t="s">
         <v>586</v>
       </c>
-      <c r="P35" s="22" t="s">
+      <c r="R35" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="Q35" s="5" t="s">
+      <c r="S35" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="R35" s="17">
+      <c r="T35" s="17">
         <v>600</v>
       </c>
-      <c r="S35" s="2" t="s">
+      <c r="U35" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="T35">
+      <c r="V35">
         <v>6</v>
       </c>
-      <c r="U35" t="s">
+      <c r="W35" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -5974,52 +6140,56 @@
       <c r="C36" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G36" s="2">
+      <c r="I36" s="2">
         <v>2000</v>
       </c>
-      <c r="H36" s="2">
+      <c r="J36" s="2">
         <v>0.25</v>
       </c>
-      <c r="I36" s="20" t="s">
+      <c r="K36" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="L36" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="O36" s="24" t="s">
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="Q36" s="24" t="s">
         <v>631</v>
       </c>
-      <c r="P36" s="22" t="s">
+      <c r="R36" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="Q36" s="17" t="s">
+      <c r="S36" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="R36" s="17" t="s">
+      <c r="T36" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="S36" s="2" t="s">
+      <c r="U36" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="T36">
+      <c r="V36">
         <v>6</v>
       </c>
-      <c r="U36" t="s">
+      <c r="W36" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -6030,57 +6200,61 @@
       <c r="C37" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="F37" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G37" s="2">
+      <c r="I37" s="2">
         <v>2000</v>
       </c>
-      <c r="H37" s="2">
+      <c r="J37" s="2">
         <v>0.5</v>
       </c>
-      <c r="I37" s="28" t="s">
+      <c r="K37" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="L37" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="5" t="s">
+      <c r="M37" s="2"/>
+      <c r="N37" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="M37" s="5" t="s">
+      <c r="O37" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="O37" s="24" t="s">
+      <c r="Q37" s="24" t="s">
         <v>647</v>
       </c>
-      <c r="P37" s="22" t="s">
+      <c r="R37" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="Q37" s="17" t="s">
+      <c r="S37" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="R37" s="17" t="s">
+      <c r="T37" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="S37" s="2" t="s">
+      <c r="U37" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="T37">
+      <c r="V37">
         <v>6</v>
       </c>
-      <c r="U37" t="s">
+      <c r="W37" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -6091,57 +6265,61 @@
       <c r="C38" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G38" s="2">
+      <c r="I38" s="2">
         <v>2000</v>
       </c>
-      <c r="H38" s="2">
+      <c r="J38" s="2">
         <v>0.5</v>
       </c>
-      <c r="I38" s="28" t="s">
+      <c r="K38" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="5" t="s">
+      <c r="M38" s="2"/>
+      <c r="N38" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="M38" s="5" t="s">
+      <c r="O38" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="O38" s="24" t="s">
+      <c r="Q38" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="P38" s="22" t="s">
+      <c r="R38" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="Q38" s="17" t="s">
+      <c r="S38" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="R38" s="17" t="s">
+      <c r="T38" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="S38" s="2" t="s">
+      <c r="U38" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="T38">
+      <c r="V38">
         <v>6</v>
       </c>
-      <c r="U38" t="s">
+      <c r="W38" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -6152,57 +6330,61 @@
       <c r="C39" s="14" t="s">
         <v>822</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="23" t="s">
         <v>823</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>824</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G39" s="2">
+      <c r="I39" s="2">
         <v>2000</v>
       </c>
-      <c r="H39" s="2">
+      <c r="J39" s="2">
         <v>0.5</v>
       </c>
-      <c r="I39" s="28" t="s">
+      <c r="K39" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="5" t="s">
+      <c r="M39" s="2"/>
+      <c r="N39" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="O39" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="O39" s="24" t="s">
+      <c r="Q39" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="P39" s="22" t="s">
+      <c r="R39" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="Q39" s="17" t="s">
+      <c r="S39" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="R39" s="17" t="s">
+      <c r="T39" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="S39" s="2" t="s">
+      <c r="U39" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="T39">
+      <c r="V39">
         <v>6</v>
       </c>
-      <c r="U39" t="s">
+      <c r="W39" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -6213,52 +6395,56 @@
       <c r="C40" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="23" t="s">
+      <c r="D40" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>653</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="G40" s="2">
+      <c r="I40" s="2">
         <v>2000</v>
       </c>
-      <c r="H40" s="2">
+      <c r="J40" s="2">
         <v>0.5</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="K40" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2" t="s">
+      <c r="M40" s="2"/>
+      <c r="N40" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O40" s="24" t="s">
+      <c r="Q40" s="24" t="s">
         <v>654</v>
       </c>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="17" t="s">
+      <c r="R40" s="22"/>
+      <c r="S40" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="R40" s="17" t="s">
+      <c r="T40" s="17" t="s">
         <v>628</v>
       </c>
-      <c r="S40" s="2" t="s">
+      <c r="U40" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="T40">
+      <c r="V40">
         <v>6</v>
       </c>
-      <c r="U40" t="s">
+      <c r="W40" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -6269,22 +6455,26 @@
       <c r="C41" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="42" t="s">
+        <v>832</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="20"/>
+      <c r="H41" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="20"/>
+      <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
+      <c r="K41" s="20"/>
       <c r="L41" s="2"/>
-      <c r="S41" s="2"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="U41" s="2"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -6295,22 +6485,26 @@
       <c r="C42" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="42" t="s">
+        <v>832</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="20"/>
+      <c r="H42" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="20"/>
+      <c r="I42" s="2"/>
       <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
+      <c r="K42" s="20"/>
       <c r="L42" s="2"/>
-      <c r="S42" s="2"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -6321,31 +6515,33 @@
       <c r="C43" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="43"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="G43" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="20" t="s">
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="O43" s="20" t="s">
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="Q43" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="S43" s="2" t="s">
+      <c r="U43" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6356,20 +6552,22 @@
       <c r="C44" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="44"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="20"/>
+      <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+      <c r="K44" s="20"/>
       <c r="L44" s="2"/>
-      <c r="S44" s="2"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -6380,20 +6578,22 @@
       <c r="C45" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="30"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="G45" s="20"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="20"/>
+      <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="K45" s="20"/>
       <c r="L45" s="2"/>
-      <c r="S45" s="2"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -6404,11 +6604,11 @@
       <c r="C46" s="10" t="s">
         <v>662</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="F46" s="23" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -6419,11 +6619,13 @@
       <c r="C47" t="s">
         <v>667</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="27"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="23" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -6434,11 +6636,12 @@
       <c r="C48" t="s">
         <v>675</v>
       </c>
-      <c r="D48" s="23" t="s">
+      <c r="E48" s="5"/>
+      <c r="F48" s="23" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -6449,11 +6652,12 @@
       <c r="C49" t="s">
         <v>697</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="E49" s="5"/>
+      <c r="F49" s="23" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -6464,11 +6668,12 @@
       <c r="C50" t="s">
         <v>701</v>
       </c>
-      <c r="D50" s="23" t="s">
+      <c r="E50" s="5"/>
+      <c r="F50" s="23" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -6479,11 +6684,12 @@
       <c r="C51" t="s">
         <v>702</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="E51" s="5"/>
+      <c r="F51" s="23" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -6494,11 +6700,11 @@
       <c r="C52" t="s">
         <v>703</v>
       </c>
-      <c r="D52" s="23" t="s">
+      <c r="F52" s="23" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -6509,13 +6715,13 @@
       <c r="C53" t="s">
         <v>709</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="F53" s="24" t="s">
         <v>710</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AA51">
-    <sortCondition ref="T2:T51"/>
+  <sortState ref="A2:AC51">
+    <sortCondition ref="V2:V51"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">
@@ -8572,7 +8778,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -8924,27 +9130,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47">
+    <row r="16" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="45">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="46" t="s">
         <v>820</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="48">
-        <v>2</v>
-      </c>
-      <c r="G16" s="48"/>
+      <c r="F16" s="46">
+        <v>2</v>
+      </c>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
@@ -9293,10 +9499,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9304,11 +9510,9 @@
     <col min="1" max="1" width="37.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.53125" customWidth="1"/>
-    <col min="4" max="4" width="16.1328125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="16.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>816</v>
       </c>
@@ -9318,793 +9522,1037 @@
       <c r="C1" t="s">
         <v>819</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>692</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>814</v>
       </c>
       <c r="B2" t="s">
         <v>812</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B2, settings!B$2:B$53, 0))</f>
+        <v>SpatialSpan</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>813</v>
       </c>
       <c r="B3" t="s">
         <v>812</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B3, settings!B$2:B$53, 0))</f>
+        <v>SpatialSpan</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>811</v>
       </c>
       <c r="B4" t="s">
         <v>811</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B4, settings!B$2:B$53, 0))</f>
+        <v>BackSpan</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>807</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B5, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>810</v>
       </c>
       <c r="B6" t="s">
         <v>807</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B6, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>809</v>
       </c>
       <c r="B7" t="s">
         <v>807</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B7, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>808</v>
       </c>
       <c r="B8" t="s">
         <v>807</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B8, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B9, settings!B$2:B$53, 0))</f>
+        <v>DivAtten2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>805</v>
       </c>
       <c r="B10" t="s">
         <v>805</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B10, settings!B$2:B$53, 0))</f>
+        <v>DivAtten1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>806</v>
       </c>
       <c r="B11" t="s">
         <v>805</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B11, settings!B$2:B$53, 0))</f>
+        <v>DivAtten1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>804</v>
       </c>
       <c r="B12" t="s">
         <v>804</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B12, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>803</v>
       </c>
       <c r="B13" t="s">
         <v>803</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B13, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>802</v>
       </c>
       <c r="B14" t="s">
         <v>802</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B14, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>801</v>
       </c>
       <c r="B15" t="s">
         <v>801</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B15, settings!B$2:B$53, 0))</f>
+        <v>TaskSwitching</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>800</v>
       </c>
       <c r="B16" t="s">
         <v>797</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B16, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>799</v>
       </c>
       <c r="B17" t="s">
         <v>797</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C17" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B17, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>797</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C18" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B18, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>798</v>
       </c>
       <c r="B19" t="s">
         <v>797</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B19, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>796</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B20, settings!B$2:B$53, 0))</f>
+        <v>Homonym</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B21, settings!B$2:B$53, 0))</f>
+        <v>BART</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>795</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C22" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B22, settings!B$2:B$53, 0))</f>
+        <v>BART</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="44"/>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B23, settings!B$2:B$53, 0))</f>
+        <v>PicMemory</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>794</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C24" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B24, settings!B$2:B$53, 0))</f>
+        <v>PicMemory</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B25, settings!B$2:B$53, 0))</f>
+        <v>Tone</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>793</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B26, settings!B$2:B$53, 0))</f>
+        <v>Tone</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B27, settings!B$2:B$53, 0))</f>
+        <v>Orthograph</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>792</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B28, settings!B$2:B$53, 0))</f>
+        <v>Orthograph</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>791</v>
       </c>
       <c r="B29" t="s">
         <v>791</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B29, settings!B$2:B$53, 0))</f>
+        <v>Anticipation</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>790</v>
       </c>
       <c r="B30" t="s">
         <v>790</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B30, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>789</v>
       </c>
       <c r="B31" t="s">
         <v>789</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C31" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B31, settings!B$2:B$53, 0))</f>
+        <v>TaskSwitching</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C32" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B32, settings!B$2:B$53, 0))</f>
+        <v>GNGLure</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C33" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B33, settings!B$2:B$53, 0))</f>
+        <v>Pinyin</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>788</v>
       </c>
       <c r="B34" t="s">
         <v>787</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C34" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B34, settings!B$2:B$53, 0))</f>
+        <v>Pinyin</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>786</v>
       </c>
       <c r="B35" t="s">
         <v>786</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C35" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B35, settings!B$2:B$53, 0))</f>
+        <v>CPT1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>151</v>
       </c>
       <c r="B36" t="s">
         <v>151</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C36" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B36, settings!B$2:B$53, 0))</f>
+        <v>CPT2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>785</v>
       </c>
       <c r="B37" t="s">
         <v>784</v>
       </c>
-      <c r="D37" s="43"/>
-      <c r="E37" s="14"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C37" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B37, settings!B$2:B$53, 0))</f>
+        <v>CPT2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>783</v>
       </c>
       <c r="B38" t="s">
         <v>782</v>
       </c>
-      <c r="D38" s="43"/>
-      <c r="E38" s="14"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C38" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B38, settings!B$2:B$53, 0))</f>
+        <v>CPT1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>781</v>
       </c>
       <c r="B39" t="s">
         <v>781</v>
       </c>
-      <c r="D39" s="43"/>
-      <c r="E39" s="14"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C39" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B39, settings!B$2:B$53, 0))</f>
+        <v>DigitCmp</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>122</v>
       </c>
       <c r="B40" t="s">
         <v>122</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C40" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B40, settings!B$2:B$53, 0))</f>
+        <v>NumStroop</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>780</v>
       </c>
       <c r="B41" t="s">
         <v>780</v>
       </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C41" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B41, settings!B$2:B$53, 0))</f>
+        <v>Nback2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>779</v>
       </c>
       <c r="B42" t="s">
         <v>779</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C42" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B42, settings!B$2:B$53, 0))</f>
+        <v>Nback1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>778</v>
       </c>
       <c r="B43" t="s">
         <v>777</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C43" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B43, settings!B$2:B$53, 0))</f>
+        <v>Nback1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>9</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C44" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B44, settings!B$2:B$53, 0))</f>
+        <v>Subitizing</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>776</v>
       </c>
       <c r="B45" t="s">
         <v>776</v>
       </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C45" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B45, settings!B$2:B$53, 0))</f>
+        <v>Flanker</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>775</v>
       </c>
       <c r="B46" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C46" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B46, settings!B$2:B$53, 0))</f>
+        <v>GNGFruit</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>774</v>
       </c>
       <c r="B47" t="s">
         <v>773</v>
       </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="13"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C47" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B47, settings!B$2:B$53, 0))</f>
+        <v>GNGFruit</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>772</v>
       </c>
       <c r="B48" t="s">
         <v>771</v>
       </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C48" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B48, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>17</v>
       </c>
       <c r="B49" t="s">
         <v>17</v>
       </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C49" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B49, settings!B$2:B$53, 0))</f>
+        <v>AttenSearch</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>770</v>
       </c>
       <c r="B50" t="s">
         <v>770</v>
       </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C50" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B50, settings!B$2:B$53, 0))</f>
+        <v>TempDiscounting</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>0</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
       </c>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C51" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B51, settings!B$2:B$53, 0))</f>
+        <v>Symbol</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>769</v>
       </c>
       <c r="B52" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C52" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B52, settings!B$2:B$53, 0))</f>
+        <v>Symbol</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>767</v>
       </c>
       <c r="B53" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C53" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B53, settings!B$2:B$53, 0))</f>
+        <v>SymbolMemory</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>766</v>
       </c>
       <c r="B54" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C54" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B54, settings!B$2:B$53, 0))</f>
+        <v>StopSignal</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C55" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B55, settings!B$2:B$53, 0))</f>
+        <v>AssocMemory</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>765</v>
       </c>
       <c r="B56" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C56" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B56, settings!B$2:B$53, 0))</f>
+        <v>AssocMemory</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>763</v>
       </c>
       <c r="B57" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C57" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B57, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>39</v>
       </c>
       <c r="B58" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C58" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B58, settings!B$2:B$53, 0))</f>
+        <v>Jigsaw2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>762</v>
       </c>
       <c r="B59" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C59" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B59, settings!B$2:B$53, 0))</f>
+        <v>Jigsaw1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>761</v>
       </c>
       <c r="B60" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C60" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B60, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>760</v>
       </c>
       <c r="B61" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C61" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B61, settings!B$2:B$53, 0))</f>
+        <v>VisualSearch</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>13</v>
       </c>
       <c r="B62" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C62" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B62, settings!B$2:B$53, 0))</f>
+        <v>WordMemory</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>759</v>
       </c>
       <c r="B63" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C63" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B63, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailLetter</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>758</v>
       </c>
       <c r="B64" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B64, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailDigit</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>679</v>
       </c>
       <c r="B65" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B65, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailLocation</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>4</v>
       </c>
       <c r="B66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B66, settings!B$2:B$53, 0))</f>
+        <v>Lexic</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>757</v>
       </c>
       <c r="B67" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B67, settings!B$2:B$53, 0))</f>
+        <v>Lexic</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>755</v>
       </c>
       <c r="B68" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B68, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>754</v>
       </c>
       <c r="B69" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B69, settings!B$2:B$53, 0))</f>
+        <v>Semantic</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>753</v>
       </c>
       <c r="B70" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B70, settings!B$2:B$53, 0))</f>
+        <v>Semantic</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>751</v>
       </c>
       <c r="B71" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B71, settings!B$2:B$53, 0))</f>
+        <v>SemanticMemory</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>750</v>
       </c>
       <c r="B72" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B72, settings!B$2:B$53, 0))</f>
+        <v>SRTWatch</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>749</v>
       </c>
       <c r="B73" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B73, settings!B$2:B$53, 0))</f>
+        <v>SRTWatch</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>747</v>
       </c>
       <c r="B74" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B74, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>7</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B75, settings!B$2:B$53, 0))</f>
+        <v>CRT</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>746</v>
       </c>
       <c r="B76" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B76, settings!B$2:B$53, 0))</f>
+        <v>CRT</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>745</v>
       </c>
       <c r="B77" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B77, settings!B$2:B$53, 0))</f>
+        <v>CRT</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>31</v>
       </c>
       <c r="B78" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B78, settings!B$2:B$53, 0))</f>
+        <v>SpeedSubtract</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>743</v>
       </c>
       <c r="B79" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B79, settings!B$2:B$53, 0))</f>
+        <v>SpeedAdd</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>742</v>
       </c>
       <c r="B80" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B80, settings!B$2:B$53, 0))</f>
+        <v>SpeedAdd</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>10</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B81, settings!B$2:B$53, 0))</f>
+        <v>SusAtten</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>740</v>
       </c>
       <c r="B82" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B82, settings!B$2:B$53, 0))</f>
+        <v>SusAtten</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>8</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B83, settings!B$2:B$53, 0))</f>
+        <v>SRTBread</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>738</v>
       </c>
       <c r="B84" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B84, settings!B$2:B$53, 0))</f>
+        <v>ForSpan</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>737</v>
       </c>
       <c r="B85" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B85, settings!B$2:B$53, 0))</f>
+        <v>ForSpan</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>35</v>
       </c>
       <c r="B86" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B86, settings!B$2:B$53, 0))</f>
+        <v>Stroop2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>735</v>
       </c>
       <c r="B87" t="s">
         <v>735</v>
+      </c>
+      <c r="C87" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B87, settings!B$2:B$53, 0))</f>
+        <v>Stroop1</v>
       </c>
     </row>
   </sheetData>
@@ -10540,7 +10988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIX BUG: Better control of task names. Add some more task name checking.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11558"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -370,7 +370,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="854">
   <si>
     <t>符号判断</t>
   </si>
@@ -2785,17 +2785,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>成都市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>龙洞小学</t>
   </si>
   <si>
-    <t>广州市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Dimension</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2949,10 +2941,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>成都市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>北京市</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2960,335 +2948,402 @@
     <t>颜色达人初级</t>
   </si>
   <si>
+    <t>顺背数-v4</t>
+  </si>
+  <si>
     <t>顺背数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>顺背数-v4</t>
-  </si>
-  <si>
-    <t>顺背数</t>
-  </si>
-  <si>
-    <t>雷达追踪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>雷达追踪-v4</t>
   </si>
   <si>
+    <t>速算师-初级-v4</t>
+  </si>
+  <si>
     <t>速算师-初级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>速算师-初级-v4</t>
-  </si>
-  <si>
-    <t>速算师-初级</t>
+  </si>
+  <si>
+    <t>选择速度儿童版（月亮向左，太阳向右）</t>
+  </si>
+  <si>
+    <t>选择速度-v4</t>
+  </si>
+  <si>
+    <t>连线</t>
+  </si>
+  <si>
+    <t>超级秒表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级秒表-v4</t>
+  </si>
+  <si>
+    <t>超级秒表</t>
+  </si>
+  <si>
+    <t>语义记忆</t>
+  </si>
+  <si>
+    <t>语义判断(高级)-v4</t>
+  </si>
+  <si>
+    <t>语义判断(高级)</t>
+  </si>
+  <si>
+    <t>语义判断</t>
+  </si>
+  <si>
+    <t>词语判断</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>词语判断-v4</t>
+  </si>
+  <si>
+    <t>记忆尾巴（数字）</t>
+  </si>
+  <si>
+    <t>记忆尾巴（字母）</t>
+  </si>
+  <si>
+    <t>视觉搜索</t>
+  </si>
+  <si>
+    <t>蝴蝶照相机初级</t>
+  </si>
+  <si>
+    <t>自由拼图（黑白版）</t>
+  </si>
+  <si>
+    <t>联系记忆高级版</t>
+  </si>
+  <si>
+    <t>联系记忆-v4</t>
+  </si>
+  <si>
+    <t>红绿灯</t>
+  </si>
+  <si>
+    <t>符号记忆</t>
+  </si>
+  <si>
+    <t>符号判断-v4</t>
+  </si>
+  <si>
+    <t>消灭敌机</t>
+  </si>
+  <si>
+    <t>水果忍者（中级）-v4</t>
+  </si>
+  <si>
+    <t>水果忍者-v4</t>
+  </si>
+  <si>
+    <t>水果忍者</t>
+  </si>
+  <si>
+    <t>方向达人</t>
+  </si>
+  <si>
+    <t>数字魔法师初级-v4</t>
+  </si>
+  <si>
+    <t>数字魔法师初级</t>
+  </si>
+  <si>
+    <t>数字魔法师中级</t>
+  </si>
+  <si>
+    <t>数字大小比较</t>
+  </si>
+  <si>
+    <t>捉虫-v4</t>
+  </si>
+  <si>
+    <t>捉虫(高级版)-v4</t>
+  </si>
+  <si>
+    <t>捉虫</t>
+  </si>
+  <si>
+    <t>拼音判断-v4</t>
+  </si>
+  <si>
+    <t>思维转换</t>
+  </si>
+  <si>
+    <t>快速译码</t>
+  </si>
+  <si>
+    <t>字形判断-v4</t>
+  </si>
+  <si>
+    <t>声调判断-v4</t>
+  </si>
+  <si>
+    <t>图片记忆-v4</t>
+  </si>
+  <si>
+    <t>吹气球-v4</t>
+  </si>
+  <si>
+    <t>反应速度（蓝色）</t>
+  </si>
+  <si>
+    <t>反应速度儿童版（月亮）</t>
+  </si>
+  <si>
+    <t>反应速度儿童版（太阳）</t>
+  </si>
+  <si>
+    <t>反应转换</t>
+  </si>
+  <si>
+    <t>卡片分类</t>
+  </si>
+  <si>
+    <t>动物达人（初级）</t>
+  </si>
+  <si>
+    <t>动物达人（中级）</t>
+  </si>
+  <si>
+    <t>分配注意初级</t>
+  </si>
+  <si>
+    <t>分配注意初级-v4</t>
+  </si>
+  <si>
+    <t>分辨速度儿童版(月亮向右、太阳不操作)</t>
+  </si>
+  <si>
+    <t>分辨速度儿童版(太阳向右、月亮不操作)</t>
+  </si>
+  <si>
+    <t>分辨速度(蓝色向左，红色不操作)</t>
+  </si>
+  <si>
+    <t>倒背数</t>
+  </si>
+  <si>
+    <t>位置记忆-v4</t>
+  </si>
+  <si>
+    <t>位置记忆</t>
+  </si>
+  <si>
+    <t>TaskOrigName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STUDY TEST|s t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STIM RT ACC Resp\STIM RT ACC Resp SCat\STIM RT ACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskIDName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片记忆、言语记忆、符号记忆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>符号记忆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SymbolMemory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memsep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attention</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thinking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丰台第一小学</t>
+  </si>
+  <si>
+    <t>北京市牌坊小学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京师范大学</t>
+  </si>
+  <si>
+    <t>北京师范大学实验小学</t>
+  </si>
+  <si>
+    <t>华南师范大学</t>
+  </si>
+  <si>
+    <t>和顺中心小学</t>
+  </si>
+  <si>
+    <t>和顺小学</t>
+  </si>
+  <si>
+    <t>恒大小学</t>
+  </si>
+  <si>
+    <t>旗峰小学</t>
+  </si>
+  <si>
+    <t>景山学校远洋分校</t>
+  </si>
+  <si>
+    <t>状元小学</t>
+  </si>
+  <si>
+    <t>绿地小学</t>
+  </si>
+  <si>
+    <t>里水中心小学</t>
+  </si>
+  <si>
+    <t>里水小学</t>
+  </si>
+  <si>
+    <t>里水镇麻奢小学</t>
+  </si>
+  <si>
+    <t>金溪小学</t>
+  </si>
+  <si>
+    <t>北京市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东省</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四川省</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班务达人</t>
+  </si>
+  <si>
+    <t>蝴蝶照相机（中级）</t>
+  </si>
+  <si>
+    <t>记忆尾巴（词语）</t>
+  </si>
+  <si>
+    <t>科学达人</t>
+  </si>
+  <si>
+    <t>热执行控制</t>
+  </si>
+  <si>
+    <t>时间预测任务</t>
+  </si>
+  <si>
+    <t>速算师中级</t>
+  </si>
+  <si>
+    <t>图片空间记忆</t>
+  </si>
+  <si>
+    <t>吹气球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红绿灯任务</t>
+  </si>
+  <si>
+    <t>蝴蝶照相机（初级）</t>
+  </si>
+  <si>
+    <t>联系记忆（高级版）</t>
+  </si>
+  <si>
+    <t>方向达人-v4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>选择速度</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>选择速度儿童版（月亮向左，太阳向右）</t>
-  </si>
-  <si>
-    <t>选择速度-v4</t>
-  </si>
-  <si>
-    <t>连线</t>
-  </si>
-  <si>
-    <t>超级秒表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超级秒表-v4</t>
-  </si>
-  <si>
-    <t>超级秒表</t>
-  </si>
-  <si>
-    <t>语义记忆</t>
-  </si>
-  <si>
-    <t>语义判断(高级)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>语义判断(高级)-v4</t>
-  </si>
-  <si>
-    <t>语义判断(高级)</t>
-  </si>
-  <si>
-    <t>语义判断</t>
-  </si>
-  <si>
-    <t>词语判断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>词语判断-v4</t>
-  </si>
-  <si>
-    <t>记忆尾巴（数字）</t>
-  </si>
-  <si>
-    <t>记忆尾巴（字母）</t>
-  </si>
-  <si>
-    <t>视觉搜索</t>
-  </si>
-  <si>
-    <t>蝴蝶照相机初级</t>
-  </si>
-  <si>
-    <t>自由拼图（黑白版）</t>
-  </si>
-  <si>
-    <t>联系记忆高级版</t>
-  </si>
-  <si>
-    <t>联系记忆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>联系记忆-v4</t>
-  </si>
-  <si>
-    <t>红绿灯</t>
-  </si>
-  <si>
-    <t>符号记忆</t>
-  </si>
-  <si>
-    <t>符号判断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>符号判断-v4</t>
-  </si>
-  <si>
-    <t>消灭敌机</t>
-  </si>
-  <si>
-    <t>水果忍者（中级）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>水果忍者（中级）-v4</t>
-  </si>
-  <si>
-    <t>水果忍者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>水果忍者-v4</t>
-  </si>
-  <si>
-    <t>水果忍者</t>
-  </si>
-  <si>
-    <t>方向达人</t>
-  </si>
-  <si>
-    <t>数字魔法师初级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数字魔法师初级-v4</t>
-  </si>
-  <si>
-    <t>数字魔法师初级</t>
-  </si>
-  <si>
-    <t>数字魔法师中级</t>
-  </si>
-  <si>
-    <t>数字大小比较</t>
-  </si>
-  <si>
-    <t>捉虫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>捉虫-v4</t>
-  </si>
-  <si>
-    <t>捉虫(高级版)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>捉虫(高级版)-v4</t>
-  </si>
-  <si>
-    <t>捉虫</t>
-  </si>
-  <si>
-    <t>拼音判断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拼音判断-v4</t>
-  </si>
-  <si>
-    <t>思维转换</t>
-  </si>
-  <si>
-    <t>快速译码</t>
-  </si>
-  <si>
-    <t>宇宙加氧站</t>
-  </si>
-  <si>
-    <t>字形判断-v4</t>
-  </si>
-  <si>
-    <t>声调判断-v4</t>
-  </si>
-  <si>
-    <t>图片记忆-v4</t>
-  </si>
-  <si>
-    <t>吹气球-v4</t>
-  </si>
-  <si>
-    <t>同音判断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>反应速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>反应速度（蓝色）</t>
-  </si>
-  <si>
-    <t>反应速度儿童版（月亮）</t>
-  </si>
-  <si>
-    <t>反应速度儿童版（太阳）</t>
-  </si>
-  <si>
-    <t>反应转换</t>
-  </si>
-  <si>
-    <t>卡片分类</t>
-  </si>
-  <si>
-    <t>动物达人（初级）</t>
-  </si>
-  <si>
-    <t>动物达人（中级）</t>
-  </si>
-  <si>
-    <t>分配注意初级</t>
-  </si>
-  <si>
-    <t>分配注意初级-v4</t>
-  </si>
-  <si>
-    <t>分辨速度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>分辨速度儿童版(月亮向右、太阳不操作)</t>
-  </si>
-  <si>
-    <t>分辨速度儿童版(太阳向右、月亮不操作)</t>
-  </si>
-  <si>
-    <t>分辨速度(蓝色向左，红色不操作)</t>
-  </si>
-  <si>
-    <t>倒背数</t>
-  </si>
-  <si>
-    <t>位置记忆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>位置记忆-v4</t>
-  </si>
-  <si>
-    <t>位置记忆</t>
+    <t>抵制诱惑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分辨速度儿童版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择速度儿童版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>反应速度儿童版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskNameCN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TaskName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TaskOrigName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STUDY TEST|s t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STIM RT ACC Resp\STIM RT ACC Resp SCat\STIM RT ACC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TaskIDName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图片记忆、言语记忆、符号记忆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>符号记忆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SymbolMemory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memsep</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reaction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Math</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Control</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attention</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Control</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thinking</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memory</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3966,11 +4021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4008,10 +4063,10 @@
         <v>79</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>147</v>
@@ -4080,7 +4135,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="23" t="s">
@@ -4140,7 +4195,7 @@
         <v>81</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="23" t="s">
@@ -4200,7 +4255,7 @@
         <v>82</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="23" t="s">
@@ -4260,7 +4315,7 @@
         <v>83</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="23" t="s">
@@ -4320,7 +4375,7 @@
         <v>84</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="23" t="s">
@@ -4380,7 +4435,7 @@
         <v>85</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="23" t="s">
@@ -4440,7 +4495,7 @@
         <v>219</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="23" t="s">
@@ -4484,7 +4539,7 @@
         <v>113</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="23" t="s">
@@ -4545,7 +4600,7 @@
         <v>114</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="23" t="s">
@@ -4606,7 +4661,7 @@
         <v>89</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="23" t="s">
@@ -4666,7 +4721,7 @@
         <v>526</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="23" t="s">
@@ -4725,7 +4780,7 @@
         <v>104</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>829</v>
+        <v>807</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="23" t="s">
@@ -4793,7 +4848,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="23" t="s">
@@ -4855,7 +4910,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="23" t="s">
@@ -4921,7 +4976,7 @@
         <v>88</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="23" t="s">
@@ -4987,7 +5042,7 @@
         <v>117</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="23" t="s">
@@ -5049,7 +5104,7 @@
         <v>118</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="23" t="s">
@@ -5111,7 +5166,7 @@
         <v>94</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="23" t="s">
@@ -5169,7 +5224,7 @@
         <v>90</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="23" t="s">
@@ -5228,7 +5283,7 @@
         <v>91</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="23" t="s">
@@ -5286,7 +5341,7 @@
         <v>92</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="23" t="s">
@@ -5352,7 +5407,7 @@
         <v>93</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="23" t="s">
@@ -5418,7 +5473,7 @@
         <v>116</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="23" t="s">
@@ -5479,7 +5534,7 @@
         <v>119</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="23" t="s">
@@ -5540,7 +5595,7 @@
         <v>101</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="23" t="s">
@@ -5607,7 +5662,7 @@
         <v>102</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="23" t="s">
@@ -5674,7 +5729,7 @@
         <v>103</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="23" t="s">
@@ -5739,7 +5794,7 @@
         <v>106</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>832</v>
+        <v>810</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="23" t="s">
@@ -5795,17 +5850,17 @@
         <v>29</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>832</v>
+        <v>810</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="23" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>492</v>
@@ -5863,7 +5918,7 @@
         <v>154</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="23" t="s">
@@ -5921,7 +5976,7 @@
         <v>105</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="23" t="s">
@@ -5979,7 +6034,7 @@
         <v>95</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="23" t="s">
@@ -6033,7 +6088,7 @@
         <v>96</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="23" t="s">
@@ -6087,7 +6142,7 @@
         <v>110</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="23" t="s">
@@ -6141,7 +6196,7 @@
         <v>97</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="23" t="s">
@@ -6201,7 +6256,7 @@
         <v>98</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="23" t="s">
@@ -6266,7 +6321,7 @@
         <v>99</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="23" t="s">
@@ -6325,20 +6380,20 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="23" t="s">
-        <v>823</v>
+        <v>801</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>824</v>
+        <v>802</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>529</v>
@@ -6396,7 +6451,7 @@
         <v>100</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="23" t="s">
@@ -6456,7 +6511,7 @@
         <v>107</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>832</v>
+        <v>810</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="23" t="s">
@@ -6486,7 +6541,7 @@
         <v>108</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>832</v>
+        <v>810</v>
       </c>
       <c r="E42" s="13"/>
       <c r="F42" s="23" t="s">
@@ -6650,7 +6705,7 @@
         <v>679</v>
       </c>
       <c r="C49" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="23" t="s">
@@ -6663,10 +6718,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C50" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="23" t="s">
@@ -6679,10 +6734,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C51" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="23" t="s">
@@ -6695,10 +6750,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C52" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="F52" s="23" t="s">
         <v>680</v>
@@ -6710,13 +6765,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>706</v>
+      </c>
+      <c r="C53" t="s">
+        <v>707</v>
+      </c>
+      <c r="F53" s="24" t="s">
         <v>708</v>
-      </c>
-      <c r="C53" t="s">
-        <v>709</v>
-      </c>
-      <c r="F53" s="24" t="s">
-        <v>710</v>
       </c>
     </row>
   </sheetData>
@@ -9053,7 +9108,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>818</v>
+        <v>796</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -9136,7 +9191,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>820</v>
+        <v>798</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>137</v>
@@ -9173,7 +9228,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>817</v>
+        <v>795</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -9292,7 +9347,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>144</v>
@@ -9417,16 +9472,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>681</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>704</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>706</v>
       </c>
       <c r="F29">
         <v>124</v>
@@ -9470,16 +9525,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>711</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>707</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>712</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -9499,1063 +9554,1732 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.53125" customWidth="1"/>
+    <col min="2" max="2" width="37.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>816</v>
+        <v>833</v>
       </c>
       <c r="B1" t="s">
-        <v>815</v>
+        <v>794</v>
       </c>
       <c r="C1" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>814</v>
+        <v>852</v>
+      </c>
+      <c r="D1" t="s">
+        <v>853</v>
+      </c>
+      <c r="E1" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>97954</v>
       </c>
       <c r="B2" t="s">
-        <v>812</v>
-      </c>
-      <c r="C2" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B2, settings!B$2:B$53, 0))</f>
+        <v>834</v>
+      </c>
+      <c r="C2" t="s">
+        <v>834</v>
+      </c>
+      <c r="D2" t="s">
+        <v>834</v>
+      </c>
+      <c r="E2" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D2, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>100020</v>
+      </c>
+      <c r="B3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C3" t="s">
+        <v>743</v>
+      </c>
+      <c r="D3" t="s">
+        <v>743</v>
+      </c>
+      <c r="E3" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D3, settings!B$2:B$53, 0))</f>
+        <v>SRTWatch</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>97979</v>
+      </c>
+      <c r="B4" t="s">
+        <v>742</v>
+      </c>
+      <c r="C4" t="s">
+        <v>741</v>
+      </c>
+      <c r="D4" t="s">
+        <v>741</v>
+      </c>
+      <c r="E4" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D4, settings!B$2:B$53, 0))</f>
+        <v>SRTWatch</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>99969</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D5, settings!B$2:B$53, 0))</f>
+        <v>BART</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>97962</v>
+      </c>
+      <c r="B6" t="s">
+        <v>778</v>
+      </c>
+      <c r="C6" t="s">
+        <v>842</v>
+      </c>
+      <c r="D6" t="s">
+        <v>842</v>
+      </c>
+      <c r="E6" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D6, settings!B$2:B$53, 0))</f>
+        <v>BART</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>99976</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D7, settings!B$2:B$53, 0))</f>
+        <v>Lexic</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>97971</v>
+      </c>
+      <c r="B8" t="s">
+        <v>749</v>
+      </c>
+      <c r="C8" t="s">
+        <v>748</v>
+      </c>
+      <c r="D8" t="s">
+        <v>748</v>
+      </c>
+      <c r="E8" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D8, settings!B$2:B$53, 0))</f>
+        <v>Lexic</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>100003</v>
+      </c>
+      <c r="B9" t="s">
+        <v>791</v>
+      </c>
+      <c r="C9" t="s">
+        <v>791</v>
+      </c>
+      <c r="D9" t="s">
+        <v>791</v>
+      </c>
+      <c r="E9" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D9, settings!B$2:B$53, 0))</f>
+        <v>BackSpan</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>97950</v>
+      </c>
+      <c r="B10" t="s">
+        <v>791</v>
+      </c>
+      <c r="C10" t="s">
+        <v>791</v>
+      </c>
+      <c r="D10" t="s">
+        <v>791</v>
+      </c>
+      <c r="E10" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D10, settings!B$2:B$53, 0))</f>
+        <v>BackSpan</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>97988</v>
+      </c>
+      <c r="B11" t="s">
+        <v>784</v>
+      </c>
+      <c r="C11" t="s">
+        <v>784</v>
+      </c>
+      <c r="D11" t="s">
+        <v>784</v>
+      </c>
+      <c r="E11" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D11, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>97983</v>
+      </c>
+      <c r="B12" t="s">
+        <v>785</v>
+      </c>
+      <c r="C12" t="s">
+        <v>785</v>
+      </c>
+      <c r="D12" t="s">
+        <v>785</v>
+      </c>
+      <c r="E12" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D12, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>100022</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D13, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>100000</v>
+      </c>
+      <c r="B14" t="s">
+        <v>779</v>
+      </c>
+      <c r="C14" t="s">
+        <v>851</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D14, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>99994</v>
+      </c>
+      <c r="B15" t="s">
+        <v>781</v>
+      </c>
+      <c r="C15" t="s">
+        <v>851</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D15, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>99993</v>
+      </c>
+      <c r="B16" t="s">
+        <v>780</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D16, settings!B$2:B$53, 0))</f>
+        <v>SRT</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>97959</v>
+      </c>
+      <c r="B17" t="s">
+        <v>782</v>
+      </c>
+      <c r="C17" t="s">
+        <v>782</v>
+      </c>
+      <c r="D17" t="s">
+        <v>782</v>
+      </c>
+      <c r="E17" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D17, settings!B$2:B$53, 0))</f>
+        <v>TaskSwitching</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>99990</v>
+      </c>
+      <c r="B18" t="s">
+        <v>773</v>
+      </c>
+      <c r="C18" t="s">
+        <v>773</v>
+      </c>
+      <c r="D18" t="s">
+        <v>773</v>
+      </c>
+      <c r="E18" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D18, settings!B$2:B$53, 0))</f>
+        <v>TaskSwitching</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>100001</v>
+      </c>
+      <c r="B19" t="s">
+        <v>764</v>
+      </c>
+      <c r="C19" t="s">
+        <v>764</v>
+      </c>
+      <c r="D19" t="s">
+        <v>764</v>
+      </c>
+      <c r="E19" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D19, settings!B$2:B$53, 0))</f>
+        <v>Flanker</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>97956</v>
+      </c>
+      <c r="B20" t="s">
+        <v>846</v>
+      </c>
+      <c r="C20" t="s">
+        <v>764</v>
+      </c>
+      <c r="D20" t="s">
+        <v>764</v>
+      </c>
+      <c r="E20" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D20, settings!B$2:B$53, 0))</f>
+        <v>Flanker</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>99998</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D21, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>100019</v>
+      </c>
+      <c r="B22" t="s">
+        <v>790</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D22, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>99996</v>
+      </c>
+      <c r="B23" t="s">
+        <v>789</v>
+      </c>
+      <c r="C23" t="s">
+        <v>849</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D23, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>99995</v>
+      </c>
+      <c r="B24" t="s">
+        <v>788</v>
+      </c>
+      <c r="C24" t="s">
+        <v>849</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D24, settings!B$2:B$53, 0))</f>
+        <v>DRT</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>100010</v>
+      </c>
+      <c r="B25" t="s">
+        <v>786</v>
+      </c>
+      <c r="C25" t="s">
+        <v>786</v>
+      </c>
+      <c r="D25" t="s">
+        <v>786</v>
+      </c>
+      <c r="E25" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D25, settings!B$2:B$53, 0))</f>
+        <v>DivAtten1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>100018</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D26, settings!B$2:B$53, 0))</f>
+        <v>DivAtten2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>97976</v>
+      </c>
+      <c r="B27" t="s">
+        <v>787</v>
+      </c>
+      <c r="C27" t="s">
+        <v>786</v>
+      </c>
+      <c r="D27" t="s">
+        <v>786</v>
+      </c>
+      <c r="E27" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D27, settings!B$2:B$53, 0))</f>
+        <v>DivAtten1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>97991</v>
+      </c>
+      <c r="B28" t="s">
+        <v>758</v>
+      </c>
+      <c r="C28" t="s">
+        <v>758</v>
+      </c>
+      <c r="D28" t="s">
+        <v>758</v>
+      </c>
+      <c r="E28" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D28, settings!B$2:B$53, 0))</f>
+        <v>SymbolMemory</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>99979</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D29, settings!B$2:B$53, 0))</f>
+        <v>Symbol</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>97972</v>
+      </c>
+      <c r="B30" t="s">
+        <v>759</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D30, settings!B$2:B$53, 0))</f>
+        <v>Symbol</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>97966</v>
+      </c>
+      <c r="B31" t="s">
+        <v>757</v>
+      </c>
+      <c r="C31" t="s">
+        <v>843</v>
+      </c>
+      <c r="D31" t="s">
+        <v>843</v>
+      </c>
+      <c r="E31" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D31, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>97987</v>
+      </c>
+      <c r="B32" t="s">
+        <v>753</v>
+      </c>
+      <c r="C32" t="s">
+        <v>844</v>
+      </c>
+      <c r="D32" t="s">
+        <v>844</v>
+      </c>
+      <c r="E32" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D32, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>97986</v>
+      </c>
+      <c r="B33" t="s">
+        <v>835</v>
+      </c>
+      <c r="C33" t="s">
+        <v>835</v>
+      </c>
+      <c r="D33" t="s">
+        <v>835</v>
+      </c>
+      <c r="E33" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D33, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>97993</v>
+      </c>
+      <c r="B34" t="s">
+        <v>836</v>
+      </c>
+      <c r="C34" t="s">
+        <v>836</v>
+      </c>
+      <c r="D34" t="s">
+        <v>836</v>
+      </c>
+      <c r="E34" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D34, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailWord</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>97992</v>
+      </c>
+      <c r="B35" t="s">
+        <v>679</v>
+      </c>
+      <c r="C35" t="s">
+        <v>679</v>
+      </c>
+      <c r="D35" t="s">
+        <v>679</v>
+      </c>
+      <c r="E35" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D35, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailLocation</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>97997</v>
+      </c>
+      <c r="B36" t="s">
+        <v>750</v>
+      </c>
+      <c r="C36" t="s">
+        <v>750</v>
+      </c>
+      <c r="D36" t="s">
+        <v>750</v>
+      </c>
+      <c r="E36" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D36, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailDigit</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>97994</v>
+      </c>
+      <c r="B37" t="s">
+        <v>751</v>
+      </c>
+      <c r="C37" t="s">
+        <v>751</v>
+      </c>
+      <c r="D37" t="s">
+        <v>751</v>
+      </c>
+      <c r="E37" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D37, settings!B$2:B$53, 0))</f>
+        <v>MemoryTailLetter</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>97990</v>
+      </c>
+      <c r="B38" t="s">
+        <v>783</v>
+      </c>
+      <c r="C38" t="s">
+        <v>783</v>
+      </c>
+      <c r="D38" t="s">
+        <v>783</v>
+      </c>
+      <c r="E38" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D38, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>97955</v>
+      </c>
+      <c r="B39" t="s">
+        <v>837</v>
+      </c>
+      <c r="C39" t="s">
+        <v>837</v>
+      </c>
+      <c r="D39" t="s">
+        <v>837</v>
+      </c>
+      <c r="E39" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D39, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>97998</v>
+      </c>
+      <c r="B40" t="s">
+        <v>774</v>
+      </c>
+      <c r="C40" t="s">
+        <v>774</v>
+      </c>
+      <c r="D40" t="s">
+        <v>774</v>
+      </c>
+      <c r="E40" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D40, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>97985</v>
+      </c>
+      <c r="B41" t="s">
+        <v>740</v>
+      </c>
+      <c r="C41" t="s">
+        <v>740</v>
+      </c>
+      <c r="D41" t="s">
+        <v>740</v>
+      </c>
+      <c r="E41" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D41, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>99991</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D42, settings!B$2:B$53, 0))</f>
+        <v>AssocMemory</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>97967</v>
+      </c>
+      <c r="B43" t="s">
+        <v>756</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D43, settings!B$2:B$53, 0))</f>
+        <v>AssocMemory</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>97989</v>
+      </c>
+      <c r="B44" t="s">
+        <v>755</v>
+      </c>
+      <c r="C44" t="s">
+        <v>845</v>
+      </c>
+      <c r="D44" t="s">
+        <v>845</v>
+      </c>
+      <c r="E44" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D44, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>100021</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D45, settings!B$2:B$53, 0))</f>
+        <v>SRTBread</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>99975</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D46, settings!B$2:B$53, 0))</f>
+        <v>Pinyin</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>97965</v>
+      </c>
+      <c r="B47" t="s">
+        <v>772</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D47, settings!B$2:B$53, 0))</f>
+        <v>Pinyin</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>99992</v>
+      </c>
+      <c r="B48" t="s">
+        <v>838</v>
+      </c>
+      <c r="C48" t="s">
+        <v>848</v>
+      </c>
+      <c r="D48" t="s">
+        <v>848</v>
+      </c>
+      <c r="E48" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D48, settings!B$2:B$53, 0))</f>
+        <v>GNGLure</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>99977</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D49, settings!B$2:B$53, 0))</f>
+        <v>Tone</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>97970</v>
+      </c>
+      <c r="B50" t="s">
+        <v>776</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D50, settings!B$2:B$53, 0))</f>
+        <v>Tone</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>97961</v>
+      </c>
+      <c r="B51" t="s">
+        <v>839</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E51" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D51, settings!B$2:B$53, 0))</f>
+        <v>Anticipation</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>97995</v>
+      </c>
+      <c r="B52" t="s">
+        <v>752</v>
+      </c>
+      <c r="C52" t="s">
+        <v>752</v>
+      </c>
+      <c r="D52" t="s">
+        <v>752</v>
+      </c>
+      <c r="E52" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D52, settings!B$2:B$53, 0))</f>
+        <v>VisualSearch</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>99971</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D53, settings!B$2:B$53, 0))</f>
+        <v>Subitizing</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>99970</v>
+      </c>
+      <c r="B54" t="s">
+        <v>768</v>
+      </c>
+      <c r="C54" t="s">
+        <v>768</v>
+      </c>
+      <c r="D54" t="s">
+        <v>768</v>
+      </c>
+      <c r="E54" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D54, settings!B$2:B$53, 0))</f>
+        <v>DigitCmp</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>99973</v>
+      </c>
+      <c r="B55" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" t="s">
+        <v>122</v>
+      </c>
+      <c r="E55" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D55, settings!B$2:B$53, 0))</f>
+        <v>NumStroop</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>100016</v>
+      </c>
+      <c r="B56" t="s">
+        <v>763</v>
+      </c>
+      <c r="C56" t="s">
+        <v>763</v>
+      </c>
+      <c r="D56" t="s">
+        <v>763</v>
+      </c>
+      <c r="E56" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D56, settings!B$2:B$53, 0))</f>
+        <v>GNGFruit</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>97982</v>
+      </c>
+      <c r="B57" t="s">
+        <v>762</v>
+      </c>
+      <c r="C57" t="s">
+        <v>763</v>
+      </c>
+      <c r="D57" t="s">
+        <v>763</v>
+      </c>
+      <c r="E57" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D57, settings!B$2:B$53, 0))</f>
+        <v>GNGFruit</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>97963</v>
+      </c>
+      <c r="B58" t="s">
+        <v>761</v>
+      </c>
+      <c r="C58" t="s">
+        <v>763</v>
+      </c>
+      <c r="D58" t="s">
+        <v>763</v>
+      </c>
+      <c r="E58" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D58, settings!B$2:B$53, 0))</f>
+        <v>GNGFruit</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>100002</v>
+      </c>
+      <c r="B59" t="s">
+        <v>734</v>
+      </c>
+      <c r="C59" t="s">
+        <v>734</v>
+      </c>
+      <c r="D59" t="s">
+        <v>734</v>
+      </c>
+      <c r="E59" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D59, settings!B$2:B$53, 0))</f>
+        <v>ForSpan</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>97975</v>
+      </c>
+      <c r="B60" t="s">
+        <v>733</v>
+      </c>
+      <c r="C60" t="s">
+        <v>734</v>
+      </c>
+      <c r="D60" t="s">
+        <v>734</v>
+      </c>
+      <c r="E60" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D60, settings!B$2:B$53, 0))</f>
+        <v>ForSpan</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>100011</v>
+      </c>
+      <c r="B61" t="s">
+        <v>737</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D61, settings!B$2:B$53, 0))</f>
+        <v>SpeedAdd</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>97981</v>
+      </c>
+      <c r="B62" t="s">
+        <v>736</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D62, settings!B$2:B$53, 0))</f>
+        <v>SpeedAdd</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>99989</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D63, settings!B$2:B$53, 0))</f>
+        <v>SpeedSubtract</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>97951</v>
+      </c>
+      <c r="B64" t="s">
+        <v>840</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" t="s">
+        <v>31</v>
+      </c>
+      <c r="E64" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D64, settings!B$2:B$53, 0))</f>
+        <v>SpeedSubtract</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>99983</v>
+      </c>
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D65, settings!B$2:B$53, 0))</f>
+        <v>Homonym</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>99988</v>
+      </c>
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D66, settings!B$2:B$53, 0))</f>
+        <v>PicMemory</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>97968</v>
+      </c>
+      <c r="B67" t="s">
+        <v>777</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D67, settings!B$2:B$53, 0))</f>
+        <v>PicMemory</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>97996</v>
+      </c>
+      <c r="B68" t="s">
+        <v>841</v>
+      </c>
+      <c r="C68" t="s">
+        <v>841</v>
+      </c>
+      <c r="D68" t="s">
+        <v>841</v>
+      </c>
+      <c r="E68" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D68, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>100023</v>
+      </c>
+      <c r="B69" t="s">
+        <v>793</v>
+      </c>
+      <c r="C69" t="s">
+        <v>793</v>
+      </c>
+      <c r="D69" t="s">
+        <v>793</v>
+      </c>
+      <c r="E69" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D69, settings!B$2:B$53, 0))</f>
         <v>SpatialSpan</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>813</v>
-      </c>
-      <c r="B3" t="s">
-        <v>812</v>
-      </c>
-      <c r="C3" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B3, settings!B$2:B$53, 0))</f>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>97980</v>
+      </c>
+      <c r="B70" t="s">
+        <v>792</v>
+      </c>
+      <c r="C70" t="s">
+        <v>793</v>
+      </c>
+      <c r="D70" t="s">
+        <v>793</v>
+      </c>
+      <c r="E70" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D70, settings!B$2:B$53, 0))</f>
         <v>SpatialSpan</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>811</v>
-      </c>
-      <c r="B4" t="s">
-        <v>811</v>
-      </c>
-      <c r="C4" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B4, settings!B$2:B$53, 0))</f>
-        <v>BackSpan</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>807</v>
-      </c>
-      <c r="C5" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B5, settings!B$2:B$53, 0))</f>
-        <v>DRT</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>810</v>
-      </c>
-      <c r="B6" t="s">
-        <v>807</v>
-      </c>
-      <c r="C6" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B6, settings!B$2:B$53, 0))</f>
-        <v>DRT</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>809</v>
-      </c>
-      <c r="B7" t="s">
-        <v>807</v>
-      </c>
-      <c r="C7" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B7, settings!B$2:B$53, 0))</f>
-        <v>DRT</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>808</v>
-      </c>
-      <c r="B8" t="s">
-        <v>807</v>
-      </c>
-      <c r="C8" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B8, settings!B$2:B$53, 0))</f>
-        <v>DRT</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B9, settings!B$2:B$53, 0))</f>
-        <v>DivAtten2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>805</v>
-      </c>
-      <c r="B10" t="s">
-        <v>805</v>
-      </c>
-      <c r="C10" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B10, settings!B$2:B$53, 0))</f>
-        <v>DivAtten1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>806</v>
-      </c>
-      <c r="B11" t="s">
-        <v>805</v>
-      </c>
-      <c r="C11" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B11, settings!B$2:B$53, 0))</f>
-        <v>DivAtten1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>804</v>
-      </c>
-      <c r="B12" t="s">
-        <v>804</v>
-      </c>
-      <c r="C12" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B12, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>803</v>
-      </c>
-      <c r="B13" t="s">
-        <v>803</v>
-      </c>
-      <c r="C13" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B13, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>802</v>
-      </c>
-      <c r="B14" t="s">
-        <v>802</v>
-      </c>
-      <c r="C14" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B14, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>801</v>
-      </c>
-      <c r="B15" t="s">
-        <v>801</v>
-      </c>
-      <c r="C15" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B15, settings!B$2:B$53, 0))</f>
-        <v>TaskSwitching</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>800</v>
-      </c>
-      <c r="B16" t="s">
-        <v>797</v>
-      </c>
-      <c r="C16" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B16, settings!B$2:B$53, 0))</f>
-        <v>SRT</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>799</v>
-      </c>
-      <c r="B17" t="s">
-        <v>797</v>
-      </c>
-      <c r="C17" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B17, settings!B$2:B$53, 0))</f>
-        <v>SRT</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>797</v>
-      </c>
-      <c r="C18" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B18, settings!B$2:B$53, 0))</f>
-        <v>SRT</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>798</v>
-      </c>
-      <c r="B19" t="s">
-        <v>797</v>
-      </c>
-      <c r="C19" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B19, settings!B$2:B$53, 0))</f>
-        <v>SRT</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>796</v>
-      </c>
-      <c r="C20" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B20, settings!B$2:B$53, 0))</f>
-        <v>Homonym</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B21, settings!B$2:B$53, 0))</f>
-        <v>BART</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>795</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B22, settings!B$2:B$53, 0))</f>
-        <v>BART</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B23, settings!B$2:B$53, 0))</f>
-        <v>PicMemory</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>794</v>
-      </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B24, settings!B$2:B$53, 0))</f>
-        <v>PicMemory</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B25, settings!B$2:B$53, 0))</f>
-        <v>Tone</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>793</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B26, settings!B$2:B$53, 0))</f>
-        <v>Tone</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B27, settings!B$2:B$53, 0))</f>
-        <v>Orthograph</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>792</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B28, settings!B$2:B$53, 0))</f>
-        <v>Orthograph</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>791</v>
-      </c>
-      <c r="B29" t="s">
-        <v>791</v>
-      </c>
-      <c r="C29" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B29, settings!B$2:B$53, 0))</f>
-        <v>Anticipation</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>790</v>
-      </c>
-      <c r="B30" t="s">
-        <v>790</v>
-      </c>
-      <c r="C30" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B30, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>789</v>
-      </c>
-      <c r="B31" t="s">
-        <v>789</v>
-      </c>
-      <c r="C31" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B31, settings!B$2:B$53, 0))</f>
-        <v>TaskSwitching</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B32, settings!B$2:B$53, 0))</f>
-        <v>GNGLure</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B33, settings!B$2:B$53, 0))</f>
-        <v>Pinyin</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>788</v>
-      </c>
-      <c r="B34" t="s">
-        <v>787</v>
-      </c>
-      <c r="C34" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B34, settings!B$2:B$53, 0))</f>
-        <v>Pinyin</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>786</v>
-      </c>
-      <c r="B35" t="s">
-        <v>786</v>
-      </c>
-      <c r="C35" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B35, settings!B$2:B$53, 0))</f>
-        <v>CPT1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>151</v>
-      </c>
-      <c r="B36" t="s">
-        <v>151</v>
-      </c>
-      <c r="C36" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B36, settings!B$2:B$53, 0))</f>
-        <v>CPT2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>785</v>
-      </c>
-      <c r="B37" t="s">
-        <v>784</v>
-      </c>
-      <c r="C37" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B37, settings!B$2:B$53, 0))</f>
-        <v>CPT2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>783</v>
-      </c>
-      <c r="B38" t="s">
-        <v>782</v>
-      </c>
-      <c r="C38" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B38, settings!B$2:B$53, 0))</f>
-        <v>CPT1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>781</v>
-      </c>
-      <c r="B39" t="s">
-        <v>781</v>
-      </c>
-      <c r="C39" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B39, settings!B$2:B$53, 0))</f>
-        <v>DigitCmp</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B40, settings!B$2:B$53, 0))</f>
-        <v>NumStroop</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>780</v>
-      </c>
-      <c r="B41" t="s">
-        <v>780</v>
-      </c>
-      <c r="C41" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B41, settings!B$2:B$53, 0))</f>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>100004</v>
+      </c>
+      <c r="B71" t="s">
+        <v>766</v>
+      </c>
+      <c r="C71" t="s">
+        <v>766</v>
+      </c>
+      <c r="D71" t="s">
+        <v>766</v>
+      </c>
+      <c r="E71" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D71, settings!B$2:B$53, 0))</f>
+        <v>Nback1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>100005</v>
+      </c>
+      <c r="B72" t="s">
+        <v>767</v>
+      </c>
+      <c r="C72" t="s">
+        <v>767</v>
+      </c>
+      <c r="D72" t="s">
+        <v>767</v>
+      </c>
+      <c r="E72" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D72, settings!B$2:B$53, 0))</f>
         <v>Nback2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>779</v>
-      </c>
-      <c r="B42" t="s">
-        <v>779</v>
-      </c>
-      <c r="C42" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B42, settings!B$2:B$53, 0))</f>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>97977</v>
+      </c>
+      <c r="B73" t="s">
+        <v>765</v>
+      </c>
+      <c r="C73" t="s">
+        <v>766</v>
+      </c>
+      <c r="D73" t="s">
+        <v>766</v>
+      </c>
+      <c r="E73" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D73, settings!B$2:B$53, 0))</f>
         <v>Nback1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>778</v>
-      </c>
-      <c r="B43" t="s">
-        <v>777</v>
-      </c>
-      <c r="C43" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B43, settings!B$2:B$53, 0))</f>
-        <v>Nback1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B44, settings!B$2:B$53, 0))</f>
-        <v>Subitizing</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>776</v>
-      </c>
-      <c r="B45" t="s">
-        <v>776</v>
-      </c>
-      <c r="C45" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B45, settings!B$2:B$53, 0))</f>
-        <v>Flanker</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>775</v>
-      </c>
-      <c r="B46" t="s">
-        <v>775</v>
-      </c>
-      <c r="C46" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B46, settings!B$2:B$53, 0))</f>
-        <v>GNGFruit</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>774</v>
-      </c>
-      <c r="B47" t="s">
-        <v>773</v>
-      </c>
-      <c r="C47" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B47, settings!B$2:B$53, 0))</f>
-        <v>GNGFruit</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>772</v>
-      </c>
-      <c r="B48" t="s">
-        <v>771</v>
-      </c>
-      <c r="C48" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B48, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B49, settings!B$2:B$53, 0))</f>
-        <v>AttenSearch</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>770</v>
-      </c>
-      <c r="B50" t="s">
-        <v>770</v>
-      </c>
-      <c r="C50" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B50, settings!B$2:B$53, 0))</f>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>97960</v>
+      </c>
+      <c r="B74" t="s">
+        <v>760</v>
+      </c>
+      <c r="C74" t="s">
+        <v>760</v>
+      </c>
+      <c r="D74" t="s">
+        <v>760</v>
+      </c>
+      <c r="E74" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D74, settings!B$2:B$53, 0))</f>
         <v>TempDiscounting</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B51, settings!B$2:B$53, 0))</f>
-        <v>Symbol</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>769</v>
-      </c>
-      <c r="B52" t="s">
-        <v>768</v>
-      </c>
-      <c r="C52" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B52, settings!B$2:B$53, 0))</f>
-        <v>Symbol</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>767</v>
-      </c>
-      <c r="B53" t="s">
-        <v>767</v>
-      </c>
-      <c r="C53" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B53, settings!B$2:B$53, 0))</f>
-        <v>SymbolMemory</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>766</v>
-      </c>
-      <c r="B54" t="s">
-        <v>766</v>
-      </c>
-      <c r="C54" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B54, settings!B$2:B$53, 0))</f>
-        <v>StopSignal</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B55, settings!B$2:B$53, 0))</f>
-        <v>AssocMemory</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>765</v>
-      </c>
-      <c r="B56" t="s">
-        <v>764</v>
-      </c>
-      <c r="C56" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B56, settings!B$2:B$53, 0))</f>
-        <v>AssocMemory</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>763</v>
-      </c>
-      <c r="B57" t="s">
-        <v>763</v>
-      </c>
-      <c r="C57" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B57, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B58, settings!B$2:B$53, 0))</f>
-        <v>Jigsaw2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>762</v>
-      </c>
-      <c r="B59" t="s">
-        <v>762</v>
-      </c>
-      <c r="C59" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B59, settings!B$2:B$53, 0))</f>
-        <v>Jigsaw1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>761</v>
-      </c>
-      <c r="B60" t="s">
-        <v>761</v>
-      </c>
-      <c r="C60" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B60, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>760</v>
-      </c>
-      <c r="B61" t="s">
-        <v>760</v>
-      </c>
-      <c r="C61" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B61, settings!B$2:B$53, 0))</f>
-        <v>VisualSearch</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B62, settings!B$2:B$53, 0))</f>
-        <v>WordMemory</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>759</v>
-      </c>
-      <c r="B63" t="s">
-        <v>759</v>
-      </c>
-      <c r="C63" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B63, settings!B$2:B$53, 0))</f>
-        <v>MemoryTailLetter</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>758</v>
-      </c>
-      <c r="B64" t="s">
-        <v>758</v>
-      </c>
-      <c r="C64" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B64, settings!B$2:B$53, 0))</f>
-        <v>MemoryTailDigit</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>679</v>
-      </c>
-      <c r="B65" t="s">
-        <v>679</v>
-      </c>
-      <c r="C65" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B65, settings!B$2:B$53, 0))</f>
-        <v>MemoryTailLocation</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B66" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B66, settings!B$2:B$53, 0))</f>
-        <v>Lexic</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>757</v>
-      </c>
-      <c r="B67" t="s">
-        <v>756</v>
-      </c>
-      <c r="C67" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B67, settings!B$2:B$53, 0))</f>
-        <v>Lexic</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>755</v>
-      </c>
-      <c r="B68" t="s">
-        <v>755</v>
-      </c>
-      <c r="C68" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B68, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>754</v>
-      </c>
-      <c r="B69" t="s">
-        <v>754</v>
-      </c>
-      <c r="C69" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B69, settings!B$2:B$53, 0))</f>
-        <v>Semantic</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>753</v>
-      </c>
-      <c r="B70" t="s">
-        <v>752</v>
-      </c>
-      <c r="C70" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B70, settings!B$2:B$53, 0))</f>
-        <v>Semantic</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>751</v>
-      </c>
-      <c r="B71" t="s">
-        <v>751</v>
-      </c>
-      <c r="C71" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B71, settings!B$2:B$53, 0))</f>
-        <v>SemanticMemory</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>750</v>
-      </c>
-      <c r="B72" t="s">
-        <v>750</v>
-      </c>
-      <c r="C72" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B72, settings!B$2:B$53, 0))</f>
-        <v>SRTWatch</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>749</v>
-      </c>
-      <c r="B73" t="s">
-        <v>748</v>
-      </c>
-      <c r="C73" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B73, settings!B$2:B$53, 0))</f>
-        <v>SRTWatch</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>747</v>
-      </c>
-      <c r="B74" t="s">
-        <v>747</v>
-      </c>
-      <c r="C74" t="e">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B74, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>7</v>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>100007</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
       </c>
-      <c r="C75" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B75, settings!B$2:B$53, 0))</f>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D75, settings!B$2:B$53, 0))</f>
         <v>CRT</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>99997</v>
+      </c>
+      <c r="B76" t="s">
+        <v>738</v>
+      </c>
+      <c r="C76" t="s">
+        <v>850</v>
+      </c>
+      <c r="D76" t="s">
+        <v>847</v>
+      </c>
+      <c r="E76" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D76, settings!B$2:B$53, 0))</f>
+        <v>CRT</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>97964</v>
+      </c>
+      <c r="B77" t="s">
+        <v>739</v>
+      </c>
+      <c r="C77" t="s">
+        <v>847</v>
+      </c>
+      <c r="D77" t="s">
+        <v>847</v>
+      </c>
+      <c r="E77" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D77, settings!B$2:B$53, 0))</f>
+        <v>CRT</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>99987</v>
+      </c>
+      <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D78, settings!B$2:B$53, 0))</f>
+        <v>WordMemory</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>100029</v>
+      </c>
+      <c r="B79" t="s">
+        <v>732</v>
+      </c>
+      <c r="C79" t="s">
+        <v>732</v>
+      </c>
+      <c r="D79" t="s">
+        <v>732</v>
+      </c>
+      <c r="E79" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D79, settings!B$2:B$53, 0))</f>
+        <v>Stroop1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>99999</v>
+      </c>
+      <c r="B80" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D80, settings!B$2:B$53, 0))</f>
+        <v>Stroop2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>99986</v>
+      </c>
+      <c r="B81" t="s">
+        <v>744</v>
+      </c>
+      <c r="C81" t="s">
+        <v>744</v>
+      </c>
+      <c r="D81" t="s">
+        <v>744</v>
+      </c>
+      <c r="E81" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D81, settings!B$2:B$53, 0))</f>
+        <v>SemanticMemory</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>99982</v>
+      </c>
+      <c r="B82" t="s">
+        <v>747</v>
+      </c>
+      <c r="C82" t="s">
+        <v>747</v>
+      </c>
+      <c r="D82" t="s">
+        <v>747</v>
+      </c>
+      <c r="E82" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D82, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>97974</v>
+      </c>
+      <c r="B83" t="s">
+        <v>745</v>
+      </c>
+      <c r="C83" t="s">
+        <v>747</v>
+      </c>
+      <c r="D83" t="s">
+        <v>747</v>
+      </c>
+      <c r="E83" t="e">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D83, settings!B$2:B$53, 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>99980</v>
+      </c>
+      <c r="B84" t="s">
         <v>746</v>
       </c>
-      <c r="B76" t="s">
-        <v>744</v>
-      </c>
-      <c r="C76" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B76, settings!B$2:B$53, 0))</f>
-        <v>CRT</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>745</v>
-      </c>
-      <c r="B77" t="s">
-        <v>744</v>
-      </c>
-      <c r="C77" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B77, settings!B$2:B$53, 0))</f>
-        <v>CRT</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>31</v>
-      </c>
-      <c r="B78" t="s">
-        <v>31</v>
-      </c>
-      <c r="C78" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B78, settings!B$2:B$53, 0))</f>
-        <v>SpeedSubtract</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>743</v>
-      </c>
-      <c r="B79" t="s">
-        <v>743</v>
-      </c>
-      <c r="C79" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B79, settings!B$2:B$53, 0))</f>
-        <v>SpeedAdd</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>742</v>
-      </c>
-      <c r="B80" t="s">
-        <v>741</v>
-      </c>
-      <c r="C80" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B80, settings!B$2:B$53, 0))</f>
-        <v>SpeedAdd</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="C84" t="s">
+        <v>746</v>
+      </c>
+      <c r="D84" t="s">
+        <v>746</v>
+      </c>
+      <c r="E84" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D84, settings!B$2:B$53, 0))</f>
+        <v>Semantic</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>99972</v>
+      </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D85, settings!B$2:B$53, 0))</f>
+        <v>AttenSearch</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>99981</v>
+      </c>
+      <c r="B86" t="s">
         <v>10</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C86" t="s">
         <v>10</v>
       </c>
-      <c r="C81" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B81, settings!B$2:B$53, 0))</f>
+      <c r="D86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D86, settings!B$2:B$53, 0))</f>
         <v>SusAtten</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>740</v>
-      </c>
-      <c r="B82" t="s">
-        <v>739</v>
-      </c>
-      <c r="C82" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B82, settings!B$2:B$53, 0))</f>
-        <v>SusAtten</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>8</v>
-      </c>
-      <c r="B83" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B83, settings!B$2:B$53, 0))</f>
-        <v>SRTBread</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>738</v>
-      </c>
-      <c r="B84" t="s">
-        <v>738</v>
-      </c>
-      <c r="C84" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B84, settings!B$2:B$53, 0))</f>
-        <v>ForSpan</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>737</v>
-      </c>
-      <c r="B85" t="s">
-        <v>736</v>
-      </c>
-      <c r="C85" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B85, settings!B$2:B$53, 0))</f>
-        <v>ForSpan</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>35</v>
-      </c>
-      <c r="B86" t="s">
-        <v>35</v>
-      </c>
-      <c r="C86" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B86, settings!B$2:B$53, 0))</f>
-        <v>Stroop2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>735</v>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>97978</v>
       </c>
       <c r="B87" t="s">
         <v>735</v>
       </c>
-      <c r="C87" t="str">
-        <f>INDEX(settings!C$2:C$53, MATCH(taskname!B87, settings!B$2:B$53, 0))</f>
-        <v>Stroop1</v>
+      <c r="C87" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D87, settings!B$2:B$53, 0))</f>
+        <v>SusAtten</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>100008</v>
+      </c>
+      <c r="B88" t="s">
+        <v>771</v>
+      </c>
+      <c r="C88" t="s">
+        <v>771</v>
+      </c>
+      <c r="D88" t="s">
+        <v>771</v>
+      </c>
+      <c r="E88" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D88, settings!B$2:B$53, 0))</f>
+        <v>CPT1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>97969</v>
+      </c>
+      <c r="B89" t="s">
+        <v>769</v>
+      </c>
+      <c r="C89" t="s">
+        <v>771</v>
+      </c>
+      <c r="D89" t="s">
+        <v>771</v>
+      </c>
+      <c r="E89" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D89, settings!B$2:B$53, 0))</f>
+        <v>CPT1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>99974</v>
+      </c>
+      <c r="B90" t="s">
+        <v>151</v>
+      </c>
+      <c r="C90" t="s">
+        <v>151</v>
+      </c>
+      <c r="D90" t="s">
+        <v>151</v>
+      </c>
+      <c r="E90" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D90, settings!B$2:B$53, 0))</f>
+        <v>CPT2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>97957</v>
+      </c>
+      <c r="B91" t="s">
+        <v>770</v>
+      </c>
+      <c r="C91" t="s">
+        <v>151</v>
+      </c>
+      <c r="D91" t="s">
+        <v>151</v>
+      </c>
+      <c r="E91" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D91, settings!B$2:B$53, 0))</f>
+        <v>CPT2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>99985</v>
+      </c>
+      <c r="B92" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92" t="s">
+        <v>39</v>
+      </c>
+      <c r="D92" t="s">
+        <v>39</v>
+      </c>
+      <c r="E92" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D92, settings!B$2:B$53, 0))</f>
+        <v>Jigsaw2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>99984</v>
+      </c>
+      <c r="B93" t="s">
+        <v>754</v>
+      </c>
+      <c r="C93" t="s">
+        <v>754</v>
+      </c>
+      <c r="D93" t="s">
+        <v>754</v>
+      </c>
+      <c r="E93" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D93, settings!B$2:B$53, 0))</f>
+        <v>Jigsaw1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>99978</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D94, settings!B$2:B$53, 0))</f>
+        <v>Orthograph</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>97973</v>
+      </c>
+      <c r="B95" t="s">
+        <v>775</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1</v>
+      </c>
+      <c r="E95" t="str">
+        <f>INDEX(settings!C$2:C$53, MATCH(taskname!D95, settings!B$2:B$53, 0))</f>
+        <v>Orthograph</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B2:D87">
+    <sortCondition ref="B2:B87"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10564,10 +11288,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -10594,7 +11318,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f t="shared" ref="A2:A26" si="0">ROW()-1</f>
+        <f t="shared" ref="A2:A42" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -10659,13 +11383,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C6" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D6" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -10674,13 +11398,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C7" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -10689,13 +11413,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C8" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D8" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -10704,13 +11428,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D9" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -10719,13 +11443,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D10" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -10734,13 +11458,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D11" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -10749,13 +11473,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>687</v>
+        <v>812</v>
       </c>
       <c r="C12" t="s">
-        <v>688</v>
+        <v>812</v>
       </c>
       <c r="D12" t="s">
-        <v>689</v>
+        <v>828</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -10764,13 +11488,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>717</v>
+        <v>813</v>
       </c>
       <c r="C13" t="s">
-        <v>717</v>
+        <v>813</v>
       </c>
       <c r="D13" t="s">
-        <v>689</v>
+        <v>828</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -10779,13 +11503,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>724</v>
+        <v>814</v>
       </c>
       <c r="C14" t="s">
-        <v>724</v>
+        <v>814</v>
       </c>
       <c r="D14" t="s">
-        <v>733</v>
+        <v>828</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -10794,13 +11518,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>690</v>
+        <v>815</v>
       </c>
       <c r="C15" t="s">
-        <v>690</v>
+        <v>815</v>
       </c>
       <c r="D15" t="s">
-        <v>691</v>
+        <v>828</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -10809,13 +11533,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>719</v>
+        <v>821</v>
       </c>
       <c r="C16" t="s">
-        <v>719</v>
+        <v>821</v>
       </c>
       <c r="D16" t="s">
-        <v>728</v>
+        <v>831</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -10824,13 +11548,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>816</v>
       </c>
       <c r="C17" t="s">
-        <v>201</v>
+        <v>816</v>
       </c>
       <c r="D17" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -10839,13 +11563,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>193</v>
+        <v>817</v>
       </c>
       <c r="C18" t="s">
-        <v>202</v>
+        <v>817</v>
       </c>
       <c r="D18" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -10854,13 +11578,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>818</v>
       </c>
       <c r="C19" t="s">
-        <v>200</v>
+        <v>818</v>
       </c>
       <c r="D19" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -10869,13 +11593,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>819</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>819</v>
       </c>
       <c r="D20" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -10884,13 +11608,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>198</v>
+        <v>820</v>
       </c>
       <c r="C21" t="s">
-        <v>198</v>
+        <v>820</v>
       </c>
       <c r="D21" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -10899,13 +11623,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>637</v>
+        <v>823</v>
       </c>
       <c r="C22" t="s">
-        <v>637</v>
+        <v>823</v>
       </c>
       <c r="D22" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -10914,13 +11638,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>685</v>
+        <v>824</v>
       </c>
       <c r="C23" t="s">
-        <v>686</v>
+        <v>824</v>
       </c>
       <c r="D23" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -10929,13 +11653,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>714</v>
+        <v>825</v>
       </c>
       <c r="C24" t="s">
-        <v>686</v>
+        <v>825</v>
       </c>
       <c r="D24" t="s">
-        <v>683</v>
+        <v>829</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -10944,13 +11668,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>721</v>
+        <v>826</v>
       </c>
       <c r="C25" t="s">
-        <v>721</v>
+        <v>826</v>
       </c>
       <c r="D25" t="s">
-        <v>729</v>
+        <v>829</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -10959,18 +11683,258 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>723</v>
+        <v>827</v>
       </c>
       <c r="C26" t="s">
-        <v>731</v>
+        <v>827</v>
       </c>
       <c r="D26" t="s">
-        <v>732</v>
+        <v>829</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>689</v>
+      </c>
+      <c r="C27" t="s">
+        <v>689</v>
+      </c>
+      <c r="D27" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>687</v>
+      </c>
+      <c r="C28" t="s">
+        <v>688</v>
+      </c>
+      <c r="D28" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>715</v>
+      </c>
+      <c r="C29" t="s">
+        <v>715</v>
+      </c>
+      <c r="D29" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>722</v>
+      </c>
+      <c r="C30" t="s">
+        <v>722</v>
+      </c>
+      <c r="D30" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>717</v>
+      </c>
+      <c r="C31" t="s">
+        <v>717</v>
+      </c>
+      <c r="D31" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" t="s">
+        <v>196</v>
+      </c>
+      <c r="D35" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>637</v>
+      </c>
+      <c r="C37" t="s">
+        <v>637</v>
+      </c>
+      <c r="D37" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>685</v>
+      </c>
+      <c r="C38" t="s">
+        <v>686</v>
+      </c>
+      <c r="D38" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>712</v>
+      </c>
+      <c r="C39" t="s">
+        <v>686</v>
+      </c>
+      <c r="D39" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>719</v>
+      </c>
+      <c r="C40" t="s">
+        <v>719</v>
+      </c>
+      <c r="D40" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>721</v>
+      </c>
+      <c r="C41" t="s">
+        <v>729</v>
+      </c>
+      <c r="D41" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>822</v>
+      </c>
+      <c r="C42" t="s">
+        <v>822</v>
+      </c>
+      <c r="D42" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D26">
-    <sortCondition ref="D2:D26"/>
+  <sortState ref="A2:D42">
+    <sortCondition ref="D2:D42"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}">
@@ -11162,18 +12126,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>825</v>
+        <v>803</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>825</v>
+        <v>803</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>826</v>
+        <v>804</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>826</v>
+        <v>804</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
FIX BUG: minor bug fixes in Merges and Proc. 1. Fix metadata variables specification. 2. Handle task names better.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -4021,11 +4021,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9556,7 +9556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ADD FEATURE:Better handling of preprocessing.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -339,6 +339,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张亮:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Use '|' to separate different variable names.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E26" authorId="0" shapeId="0">
       <text>
         <r>
@@ -370,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="876">
   <si>
     <t>符号判断</t>
   </si>
@@ -2921,10 +2945,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>枣庄市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>重庆市</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3344,6 +3364,98 @@
   </si>
   <si>
     <t>TaskName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红绿灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SchoolNameEn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NoteEn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BJ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山东省</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DongZB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BeiF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShiL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HuaiB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DongJMX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiuLHZX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DouDZX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HuiWDY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QingHFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShouDYK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PreSpVar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alltime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RECORD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3351,7 +3463,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3532,6 +3644,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3584,7 +3709,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3730,6 +3855,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4021,11 +4155,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4035,7 +4169,7 @@
     <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1328125" style="21" customWidth="1"/>
     <col min="5" max="5" width="16.1328125" customWidth="1"/>
-    <col min="6" max="6" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12.73046875" customWidth="1"/>
     <col min="11" max="11" width="15" style="21" bestFit="1" customWidth="1"/>
@@ -4068,7 +4202,7 @@
       <c r="E1" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="20" t="s">
         <v>147</v>
       </c>
       <c r="G1" s="20" t="s">
@@ -4135,10 +4269,10 @@
         <v>80</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E2" s="13"/>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G2" s="20" t="s">
@@ -4195,10 +4329,10 @@
         <v>81</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E3" s="14"/>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G3" s="20" t="s">
@@ -4255,10 +4389,10 @@
         <v>82</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E4" s="14"/>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G4" s="20" t="s">
@@ -4315,10 +4449,10 @@
         <v>83</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G5" s="20" t="s">
@@ -4375,10 +4509,10 @@
         <v>84</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E6" s="14"/>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G6" s="20" t="s">
@@ -4435,10 +4569,10 @@
         <v>85</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E7" s="14"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G7" s="20" t="s">
@@ -4495,10 +4629,10 @@
         <v>219</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="20" t="s">
         <v>224</v>
       </c>
       <c r="G8" s="20"/>
@@ -4539,10 +4673,10 @@
         <v>113</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E9" s="13"/>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="20" t="s">
         <v>126</v>
       </c>
       <c r="G9" s="29" t="s">
@@ -4600,10 +4734,10 @@
         <v>114</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E10" s="14"/>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="20" t="s">
         <v>126</v>
       </c>
       <c r="G10" s="27" t="s">
@@ -4661,10 +4795,10 @@
         <v>89</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E11" s="14"/>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="20" t="s">
         <v>130</v>
       </c>
       <c r="G11" s="27" t="s">
@@ -4721,10 +4855,10 @@
         <v>526</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="20" t="s">
         <v>131</v>
       </c>
       <c r="G12" s="27" t="s">
@@ -4780,10 +4914,10 @@
         <v>104</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="20" t="s">
         <v>142</v>
       </c>
       <c r="G13" s="20" t="s">
@@ -4848,10 +4982,10 @@
         <v>86</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E14" s="14"/>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="20" t="s">
         <v>127</v>
       </c>
       <c r="G14" s="20" t="s">
@@ -4910,10 +5044,10 @@
         <v>87</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E15" s="14"/>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="20" t="s">
         <v>127</v>
       </c>
       <c r="G15" s="20" t="s">
@@ -4976,10 +5110,10 @@
         <v>88</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E16" s="14"/>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="20" t="s">
         <v>127</v>
       </c>
       <c r="G16" s="20" t="s">
@@ -5042,10 +5176,10 @@
         <v>117</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E17" s="14"/>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="20" t="s">
         <v>128</v>
       </c>
       <c r="G17" s="20" t="s">
@@ -5104,10 +5238,10 @@
         <v>118</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E18" s="14"/>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="20" t="s">
         <v>129</v>
       </c>
       <c r="G18" s="20" t="s">
@@ -5166,10 +5300,10 @@
         <v>94</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="20" t="s">
         <v>132</v>
       </c>
       <c r="G19" s="20" t="s">
@@ -5224,10 +5358,10 @@
         <v>90</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E20" s="15"/>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="20" t="s">
         <v>208</v>
       </c>
       <c r="G20" s="20" t="s">
@@ -5283,10 +5417,10 @@
         <v>91</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E21" s="15"/>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="20" t="s">
         <v>91</v>
       </c>
       <c r="G21" s="20" t="s">
@@ -5341,10 +5475,10 @@
         <v>92</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E22" s="13"/>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="20" t="s">
         <v>134</v>
       </c>
       <c r="G22" s="20" t="s">
@@ -5407,10 +5541,10 @@
         <v>93</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="20" t="s">
         <v>134</v>
       </c>
       <c r="G23" s="20" t="s">
@@ -5473,10 +5607,10 @@
         <v>116</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E24" s="13"/>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="20" t="s">
         <v>139</v>
       </c>
       <c r="G24" s="20" t="s">
@@ -5534,10 +5668,10 @@
         <v>119</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E25" s="14"/>
-      <c r="F25" s="23" t="s">
+      <c r="F25" s="20" t="s">
         <v>139</v>
       </c>
       <c r="G25" s="20" t="s">
@@ -5595,10 +5729,10 @@
         <v>101</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E26" s="14"/>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="20" t="s">
         <v>140</v>
       </c>
       <c r="G26" s="20" t="s">
@@ -5662,10 +5796,10 @@
         <v>102</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E27" s="14"/>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="20" t="s">
         <v>141</v>
       </c>
       <c r="G27" s="20" t="s">
@@ -5729,10 +5863,10 @@
         <v>103</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E28" s="14"/>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="20" t="s">
         <v>141</v>
       </c>
       <c r="G28" s="20" t="s">
@@ -5794,10 +5928,10 @@
         <v>106</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E29" s="13"/>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="20" t="s">
         <v>144</v>
       </c>
       <c r="G29" s="20" t="s">
@@ -5856,10 +5990,10 @@
         <v>106</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E30" s="13"/>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="20" t="s">
         <v>693</v>
       </c>
       <c r="G30" s="20" t="s">
@@ -5918,10 +6052,10 @@
         <v>154</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E31" s="13"/>
-      <c r="F31" s="23" t="s">
+      <c r="F31" s="20" t="s">
         <v>143</v>
       </c>
       <c r="G31" s="28" t="s">
@@ -5976,10 +6110,10 @@
         <v>105</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E32" s="13"/>
-      <c r="F32" s="23" t="s">
+      <c r="F32" s="20" t="s">
         <v>143</v>
       </c>
       <c r="G32" s="30" t="s">
@@ -6034,10 +6168,10 @@
         <v>95</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="23" t="s">
+      <c r="F33" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G33" s="20" t="s">
@@ -6088,10 +6222,10 @@
         <v>96</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E34" s="7"/>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G34" s="20" t="s">
@@ -6142,10 +6276,10 @@
         <v>110</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G35" s="20" t="s">
@@ -6196,10 +6330,10 @@
         <v>97</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E36" s="13"/>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="20" t="s">
         <v>136</v>
       </c>
       <c r="G36" s="20" t="s">
@@ -6256,10 +6390,10 @@
         <v>98</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E37" s="14"/>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="20" t="s">
         <v>137</v>
       </c>
       <c r="G37" s="20" t="s">
@@ -6321,10 +6455,10 @@
         <v>99</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E38" s="14"/>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="20" t="s">
         <v>137</v>
       </c>
       <c r="G38" s="20" t="s">
@@ -6380,20 +6514,20 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>799</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="D39" s="29" t="s">
+        <v>810</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="20" t="s">
         <v>800</v>
       </c>
-      <c r="D39" s="29" t="s">
-        <v>811</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="23" t="s">
+      <c r="G39" s="20" t="s">
         <v>801</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>802</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>529</v>
@@ -6451,10 +6585,10 @@
         <v>100</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E40" s="7"/>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="20" t="s">
         <v>138</v>
       </c>
       <c r="G40" s="20" t="s">
@@ -6511,10 +6645,10 @@
         <v>107</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="23" t="s">
+      <c r="F41" s="20" t="s">
         <v>145</v>
       </c>
       <c r="G41" s="20"/>
@@ -6541,10 +6675,10 @@
         <v>108</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E42" s="13"/>
-      <c r="F42" s="23" t="s">
+      <c r="F42" s="20" t="s">
         <v>145</v>
       </c>
       <c r="G42" s="20"/>
@@ -6572,7 +6706,7 @@
       </c>
       <c r="D43" s="43"/>
       <c r="E43" s="11"/>
-      <c r="F43" s="23" t="s">
+      <c r="F43" s="20" t="s">
         <v>146</v>
       </c>
       <c r="G43" s="20" t="s">
@@ -6609,7 +6743,7 @@
       </c>
       <c r="D44" s="44"/>
       <c r="E44" s="12"/>
-      <c r="F44" s="23" t="s">
+      <c r="F44" s="20" t="s">
         <v>148</v>
       </c>
       <c r="G44" s="20"/>
@@ -6635,7 +6769,7 @@
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="10"/>
-      <c r="F45" s="23" t="s">
+      <c r="F45" s="20" t="s">
         <v>149</v>
       </c>
       <c r="G45" s="20"/>
@@ -6659,7 +6793,7 @@
       <c r="C46" s="10" t="s">
         <v>662</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="F46" s="20" t="s">
         <v>663</v>
       </c>
     </row>
@@ -6676,7 +6810,7 @@
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="20" t="s">
         <v>668</v>
       </c>
     </row>
@@ -6692,7 +6826,7 @@
         <v>675</v>
       </c>
       <c r="E48" s="5"/>
-      <c r="F48" s="23" t="s">
+      <c r="F48" s="20" t="s">
         <v>676</v>
       </c>
     </row>
@@ -6708,7 +6842,7 @@
         <v>695</v>
       </c>
       <c r="E49" s="5"/>
-      <c r="F49" s="23" t="s">
+      <c r="F49" s="20" t="s">
         <v>680</v>
       </c>
     </row>
@@ -6724,7 +6858,7 @@
         <v>699</v>
       </c>
       <c r="E50" s="5"/>
-      <c r="F50" s="23" t="s">
+      <c r="F50" s="20" t="s">
         <v>680</v>
       </c>
     </row>
@@ -6740,7 +6874,7 @@
         <v>700</v>
       </c>
       <c r="E51" s="5"/>
-      <c r="F51" s="23" t="s">
+      <c r="F51" s="20" t="s">
         <v>680</v>
       </c>
     </row>
@@ -6755,7 +6889,7 @@
       <c r="C52" t="s">
         <v>701</v>
       </c>
-      <c r="F52" s="23" t="s">
+      <c r="F52" s="20" t="s">
         <v>680</v>
       </c>
     </row>
@@ -6770,12 +6904,12 @@
       <c r="C53" t="s">
         <v>707</v>
       </c>
-      <c r="F53" s="24" t="s">
+      <c r="F53" s="21" t="s">
         <v>708</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AC51">
+  <sortState ref="A2:AD51">
     <sortCondition ref="V2:V51"/>
   </sortState>
   <customSheetViews>
@@ -8830,10 +8964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -8841,13 +8975,15 @@
     <col min="1" max="1" width="3.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.06640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>533</v>
       </c>
@@ -8857,7 +8993,7 @@
       <c r="C1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="21" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -8872,8 +9008,17 @@
       <c r="H1" s="5" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="49" t="s">
+        <v>872</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f>ROW() - 1</f>
         <v>1</v>
@@ -8884,7 +9029,7 @@
       <c r="C2" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="21" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -8894,8 +9039,17 @@
         <v>1</v>
       </c>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>874</v>
+      </c>
+      <c r="K2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f>ROW() - 1</f>
         <v>2</v>
@@ -8906,7 +9060,7 @@
       <c r="C3" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="21" t="s">
         <v>222</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -8916,8 +9070,9 @@
         <v>2</v>
       </c>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A32" si="0">ROW() - 1</f>
         <v>3</v>
@@ -8928,7 +9083,7 @@
       <c r="C4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="21" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -8938,8 +9093,12 @@
         <v>1</v>
       </c>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="50"/>
+      <c r="J4" s="29" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8950,7 +9109,7 @@
       <c r="C5" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -8960,8 +9119,9 @@
         <v>0</v>
       </c>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8972,7 +9132,7 @@
       <c r="C6" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="21" t="s">
         <v>55</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -8982,8 +9142,9 @@
         <v>0</v>
       </c>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="50"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8994,7 +9155,7 @@
       <c r="C7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="21" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -9004,8 +9165,9 @@
         <v>0</v>
       </c>
       <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="50"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -9016,7 +9178,7 @@
       <c r="C8" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="21" t="s">
         <v>57</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -9026,8 +9188,9 @@
         <v>0</v>
       </c>
       <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -9038,7 +9201,7 @@
       <c r="C9" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="21" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -9048,8 +9211,9 @@
         <v>0</v>
       </c>
       <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -9060,7 +9224,7 @@
       <c r="C10" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -9070,8 +9234,9 @@
         <v>0</v>
       </c>
       <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -9082,7 +9247,7 @@
       <c r="C11" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="20" t="s">
         <v>209</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -9092,8 +9257,9 @@
         <v>0</v>
       </c>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -9104,18 +9270,19 @@
       <c r="C12" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="20" t="s">
         <v>57</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -9126,7 +9293,7 @@
       <c r="C13" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="20" t="s">
         <v>115</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -9138,8 +9305,9 @@
       <c r="G13" s="5" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -9150,7 +9318,7 @@
       <c r="C14" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="20" t="s">
         <v>52</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -9160,8 +9328,9 @@
         <v>216</v>
       </c>
       <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -9172,7 +9341,7 @@
       <c r="C15" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="21" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -9184,19 +9353,20 @@
       <c r="H15" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="51" t="s">
         <v>52</v>
       </c>
       <c r="E16" s="46" t="s">
@@ -9206,8 +9376,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="5"/>
+      <c r="J16" s="51"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -9218,7 +9390,7 @@
       <c r="C17" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="21" t="s">
         <v>121</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -9228,10 +9400,11 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>794</v>
+      </c>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -9242,7 +9415,7 @@
       <c r="C18" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="21" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -9252,8 +9425,9 @@
         <v>0</v>
       </c>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -9264,7 +9438,7 @@
       <c r="C19" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="21" t="s">
         <v>57</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -9274,8 +9448,9 @@
         <v>0</v>
       </c>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -9286,7 +9461,7 @@
       <c r="C20" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -9296,8 +9471,9 @@
         <v>0</v>
       </c>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -9308,7 +9484,7 @@
       <c r="C21" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="20" t="s">
         <v>124</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -9318,8 +9494,9 @@
         <v>0</v>
       </c>
       <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -9330,7 +9507,7 @@
       <c r="C22" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="21" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -9340,8 +9517,9 @@
         <v>0</v>
       </c>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -9352,7 +9530,7 @@
       <c r="C23" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -9362,8 +9540,9 @@
         <v>0</v>
       </c>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -9374,7 +9553,7 @@
       <c r="C24" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="21" t="s">
         <v>72</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -9386,8 +9565,9 @@
       <c r="H24" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -9398,7 +9578,7 @@
       <c r="C25" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="21" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -9408,8 +9588,9 @@
         <v>0</v>
       </c>
       <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -9420,7 +9601,7 @@
       <c r="C26" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="20" t="s">
         <v>665</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -9429,8 +9610,9 @@
       <c r="F26" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -9441,14 +9623,15 @@
       <c r="C27" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="20" t="s">
         <v>671</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -9459,14 +9642,15 @@
       <c r="C28" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="20" t="s">
         <v>677</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -9477,7 +9661,7 @@
       <c r="C29" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="20" t="s">
         <v>702</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -9486,8 +9670,9 @@
       <c r="F29">
         <v>124</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -9498,12 +9683,12 @@
       <c r="C30" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -9514,12 +9699,12 @@
       <c r="C31" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -9530,12 +9715,73 @@
       <c r="C32" s="5" t="s">
         <v>705</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="20" t="s">
         <v>710</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>711</v>
       </c>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -9557,7 +9803,7 @@
   <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9569,19 +9815,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C1" t="s">
+        <v>851</v>
+      </c>
+      <c r="D1" t="s">
         <v>852</v>
       </c>
-      <c r="D1" t="s">
-        <v>853</v>
-      </c>
       <c r="E1" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -9589,13 +9835,13 @@
         <v>97954</v>
       </c>
       <c r="B2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E2" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D2, settings!B$2:B$53, 0))</f>
@@ -9607,13 +9853,13 @@
         <v>100020</v>
       </c>
       <c r="B3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E3" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D3, settings!B$2:B$53, 0))</f>
@@ -9625,13 +9871,13 @@
         <v>97979</v>
       </c>
       <c r="B4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E4" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D4, settings!B$2:B$53, 0))</f>
@@ -9661,13 +9907,13 @@
         <v>97962</v>
       </c>
       <c r="B6" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C6" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D6" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E6" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D6, settings!B$2:B$53, 0))</f>
@@ -9697,13 +9943,13 @@
         <v>97971</v>
       </c>
       <c r="B8" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C8" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D8" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E8" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D8, settings!B$2:B$53, 0))</f>
@@ -9715,13 +9961,13 @@
         <v>100003</v>
       </c>
       <c r="B9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E9" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D9, settings!B$2:B$53, 0))</f>
@@ -9733,13 +9979,13 @@
         <v>97950</v>
       </c>
       <c r="B10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E10" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D10, settings!B$2:B$53, 0))</f>
@@ -9751,13 +9997,13 @@
         <v>97988</v>
       </c>
       <c r="B11" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C11" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D11" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E11" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D11, settings!B$2:B$53, 0))</f>
@@ -9769,13 +10015,13 @@
         <v>97983</v>
       </c>
       <c r="B12" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C12" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D12" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E12" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D12, settings!B$2:B$53, 0))</f>
@@ -9805,10 +10051,10 @@
         <v>100000</v>
       </c>
       <c r="B14" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C14" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -9823,10 +10069,10 @@
         <v>99994</v>
       </c>
       <c r="B15" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C15" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -9841,7 +10087,7 @@
         <v>99993</v>
       </c>
       <c r="B16" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -9859,13 +10105,13 @@
         <v>97959</v>
       </c>
       <c r="B17" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C17" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D17" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E17" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D17, settings!B$2:B$53, 0))</f>
@@ -9877,13 +10123,13 @@
         <v>99990</v>
       </c>
       <c r="B18" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C18" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D18" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E18" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D18, settings!B$2:B$53, 0))</f>
@@ -9895,13 +10141,13 @@
         <v>100001</v>
       </c>
       <c r="B19" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C19" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D19" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E19" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D19, settings!B$2:B$53, 0))</f>
@@ -9913,13 +10159,13 @@
         <v>97956</v>
       </c>
       <c r="B20" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C20" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D20" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E20" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D20, settings!B$2:B$53, 0))</f>
@@ -9949,7 +10195,7 @@
         <v>100019</v>
       </c>
       <c r="B22" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -9967,10 +10213,10 @@
         <v>99996</v>
       </c>
       <c r="B23" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C23" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -9985,10 +10231,10 @@
         <v>99995</v>
       </c>
       <c r="B24" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C24" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -10003,13 +10249,13 @@
         <v>100010</v>
       </c>
       <c r="B25" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C25" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D25" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E25" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D25, settings!B$2:B$53, 0))</f>
@@ -10039,13 +10285,13 @@
         <v>97976</v>
       </c>
       <c r="B27" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C27" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D27" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E27" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D27, settings!B$2:B$53, 0))</f>
@@ -10057,13 +10303,13 @@
         <v>97991</v>
       </c>
       <c r="B28" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C28" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D28" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E28" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D28, settings!B$2:B$53, 0))</f>
@@ -10093,7 +10339,7 @@
         <v>97972</v>
       </c>
       <c r="B30" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -10111,17 +10357,17 @@
         <v>97966</v>
       </c>
       <c r="B31" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D31" t="s">
-        <v>843</v>
-      </c>
-      <c r="E31" t="e">
+        <v>853</v>
+      </c>
+      <c r="E31" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D31, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
+        <v>StopSignal</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -10129,13 +10375,13 @@
         <v>97987</v>
       </c>
       <c r="B32" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C32" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D32" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E32" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D32, settings!B$2:B$53, 0))</f>
@@ -10147,13 +10393,13 @@
         <v>97986</v>
       </c>
       <c r="B33" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C33" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D33" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E33" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D33, settings!B$2:B$53, 0))</f>
@@ -10165,13 +10411,13 @@
         <v>97993</v>
       </c>
       <c r="B34" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C34" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D34" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E34" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D34, settings!B$2:B$53, 0))</f>
@@ -10201,13 +10447,13 @@
         <v>97997</v>
       </c>
       <c r="B36" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C36" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D36" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E36" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D36, settings!B$2:B$53, 0))</f>
@@ -10219,13 +10465,13 @@
         <v>97994</v>
       </c>
       <c r="B37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D37" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E37" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D37, settings!B$2:B$53, 0))</f>
@@ -10237,13 +10483,13 @@
         <v>97990</v>
       </c>
       <c r="B38" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C38" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D38" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E38" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D38, settings!B$2:B$53, 0))</f>
@@ -10255,13 +10501,13 @@
         <v>97955</v>
       </c>
       <c r="B39" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C39" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D39" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E39" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D39, settings!B$2:B$53, 0))</f>
@@ -10273,13 +10519,13 @@
         <v>97998</v>
       </c>
       <c r="B40" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C40" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D40" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E40" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D40, settings!B$2:B$53, 0))</f>
@@ -10291,13 +10537,13 @@
         <v>97985</v>
       </c>
       <c r="B41" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C41" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D41" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E41" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D41, settings!B$2:B$53, 0))</f>
@@ -10327,7 +10573,7 @@
         <v>97967</v>
       </c>
       <c r="B43" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -10345,13 +10591,13 @@
         <v>97989</v>
       </c>
       <c r="B44" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C44" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D44" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E44" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D44, settings!B$2:B$53, 0))</f>
@@ -10399,7 +10645,7 @@
         <v>97965</v>
       </c>
       <c r="B47" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -10417,13 +10663,13 @@
         <v>99992</v>
       </c>
       <c r="B48" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C48" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D48" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E48" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D48, settings!B$2:B$53, 0))</f>
@@ -10453,7 +10699,7 @@
         <v>97970</v>
       </c>
       <c r="B50" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -10471,7 +10717,7 @@
         <v>97961</v>
       </c>
       <c r="B51" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>666</v>
@@ -10489,13 +10735,13 @@
         <v>97995</v>
       </c>
       <c r="B52" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C52" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D52" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E52" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D52, settings!B$2:B$53, 0))</f>
@@ -10525,13 +10771,13 @@
         <v>99970</v>
       </c>
       <c r="B54" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C54" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D54" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E54" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D54, settings!B$2:B$53, 0))</f>
@@ -10561,13 +10807,13 @@
         <v>100016</v>
       </c>
       <c r="B56" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C56" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D56" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E56" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D56, settings!B$2:B$53, 0))</f>
@@ -10579,13 +10825,13 @@
         <v>97982</v>
       </c>
       <c r="B57" t="s">
+        <v>761</v>
+      </c>
+      <c r="C57" t="s">
         <v>762</v>
       </c>
-      <c r="C57" t="s">
-        <v>763</v>
-      </c>
       <c r="D57" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E57" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D57, settings!B$2:B$53, 0))</f>
@@ -10597,13 +10843,13 @@
         <v>97963</v>
       </c>
       <c r="B58" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C58" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D58" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E58" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D58, settings!B$2:B$53, 0))</f>
@@ -10615,13 +10861,13 @@
         <v>100002</v>
       </c>
       <c r="B59" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C59" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D59" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E59" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D59, settings!B$2:B$53, 0))</f>
@@ -10633,13 +10879,13 @@
         <v>97975</v>
       </c>
       <c r="B60" t="s">
+        <v>732</v>
+      </c>
+      <c r="C60" t="s">
         <v>733</v>
       </c>
-      <c r="C60" t="s">
-        <v>734</v>
-      </c>
       <c r="D60" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E60" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D60, settings!B$2:B$53, 0))</f>
@@ -10651,7 +10897,7 @@
         <v>100011</v>
       </c>
       <c r="B61" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>32</v>
@@ -10669,7 +10915,7 @@
         <v>97981</v>
       </c>
       <c r="B62" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>32</v>
@@ -10705,7 +10951,7 @@
         <v>97951</v>
       </c>
       <c r="B64" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C64" t="s">
         <v>31</v>
@@ -10759,7 +11005,7 @@
         <v>97968</v>
       </c>
       <c r="B67" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -10777,13 +11023,13 @@
         <v>97996</v>
       </c>
       <c r="B68" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C68" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D68" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E68" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D68, settings!B$2:B$53, 0))</f>
@@ -10795,13 +11041,13 @@
         <v>100023</v>
       </c>
       <c r="B69" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C69" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D69" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E69" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D69, settings!B$2:B$53, 0))</f>
@@ -10813,13 +11059,13 @@
         <v>97980</v>
       </c>
       <c r="B70" t="s">
+        <v>791</v>
+      </c>
+      <c r="C70" t="s">
         <v>792</v>
       </c>
-      <c r="C70" t="s">
-        <v>793</v>
-      </c>
       <c r="D70" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E70" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D70, settings!B$2:B$53, 0))</f>
@@ -10831,13 +11077,13 @@
         <v>100004</v>
       </c>
       <c r="B71" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C71" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D71" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E71" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D71, settings!B$2:B$53, 0))</f>
@@ -10849,13 +11095,13 @@
         <v>100005</v>
       </c>
       <c r="B72" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C72" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D72" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E72" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D72, settings!B$2:B$53, 0))</f>
@@ -10867,13 +11113,13 @@
         <v>97977</v>
       </c>
       <c r="B73" t="s">
+        <v>764</v>
+      </c>
+      <c r="C73" t="s">
         <v>765</v>
       </c>
-      <c r="C73" t="s">
-        <v>766</v>
-      </c>
       <c r="D73" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E73" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D73, settings!B$2:B$53, 0))</f>
@@ -10885,13 +11131,13 @@
         <v>97960</v>
       </c>
       <c r="B74" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C74" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D74" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E74" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D74, settings!B$2:B$53, 0))</f>
@@ -10921,13 +11167,13 @@
         <v>99997</v>
       </c>
       <c r="B76" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C76" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D76" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E76" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D76, settings!B$2:B$53, 0))</f>
@@ -10939,13 +11185,13 @@
         <v>97964</v>
       </c>
       <c r="B77" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C77" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D77" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E77" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D77, settings!B$2:B$53, 0))</f>
@@ -10975,13 +11221,13 @@
         <v>100029</v>
       </c>
       <c r="B79" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C79" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D79" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E79" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D79, settings!B$2:B$53, 0))</f>
@@ -11011,13 +11257,13 @@
         <v>99986</v>
       </c>
       <c r="B81" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C81" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D81" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E81" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D81, settings!B$2:B$53, 0))</f>
@@ -11029,13 +11275,13 @@
         <v>99982</v>
       </c>
       <c r="B82" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C82" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D82" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E82" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D82, settings!B$2:B$53, 0))</f>
@@ -11047,13 +11293,13 @@
         <v>97974</v>
       </c>
       <c r="B83" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C83" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D83" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E83" t="e">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D83, settings!B$2:B$53, 0))</f>
@@ -11065,13 +11311,13 @@
         <v>99980</v>
       </c>
       <c r="B84" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C84" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D84" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E84" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D84, settings!B$2:B$53, 0))</f>
@@ -11119,7 +11365,7 @@
         <v>97978</v>
       </c>
       <c r="B87" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
@@ -11137,13 +11383,13 @@
         <v>100008</v>
       </c>
       <c r="B88" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C88" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D88" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E88" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D88, settings!B$2:B$53, 0))</f>
@@ -11155,13 +11401,13 @@
         <v>97969</v>
       </c>
       <c r="B89" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C89" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D89" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E89" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D89, settings!B$2:B$53, 0))</f>
@@ -11191,7 +11437,7 @@
         <v>97957</v>
       </c>
       <c r="B91" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C91" t="s">
         <v>151</v>
@@ -11227,13 +11473,13 @@
         <v>99984</v>
       </c>
       <c r="B93" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C93" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D93" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E93" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D93, settings!B$2:B$53, 0))</f>
@@ -11263,7 +11509,7 @@
         <v>97973</v>
       </c>
       <c r="B95" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -11288,21 +11534,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>189</v>
       </c>
@@ -11313,10 +11560,16 @@
         <v>191</v>
       </c>
       <c r="D1" t="s">
+        <v>854</v>
+      </c>
+      <c r="E1" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <f t="shared" ref="A2:A42" si="0">ROW()-1</f>
         <v>1</v>
@@ -11328,10 +11581,16 @@
         <v>195</v>
       </c>
       <c r="D2" t="s">
+        <v>862</v>
+      </c>
+      <c r="E2" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -11343,11 +11602,17 @@
         <v>194</v>
       </c>
       <c r="D3" t="s">
+        <v>863</v>
+      </c>
+      <c r="E3" t="s">
         <v>684</v>
       </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>856</v>
+      </c>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -11359,10 +11624,16 @@
         <v>199</v>
       </c>
       <c r="D4" t="s">
+        <v>864</v>
+      </c>
+      <c r="E4" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -11374,10 +11645,16 @@
         <v>636</v>
       </c>
       <c r="D5" t="s">
+        <v>865</v>
+      </c>
+      <c r="E5" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -11389,10 +11666,16 @@
         <v>713</v>
       </c>
       <c r="D6" t="s">
+        <v>866</v>
+      </c>
+      <c r="E6" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -11404,10 +11687,16 @@
         <v>714</v>
       </c>
       <c r="D7" t="s">
+        <v>867</v>
+      </c>
+      <c r="E7" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -11419,10 +11708,16 @@
         <v>716</v>
       </c>
       <c r="D8" t="s">
+        <v>868</v>
+      </c>
+      <c r="E8" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -11434,10 +11729,16 @@
         <v>718</v>
       </c>
       <c r="D9" t="s">
+        <v>869</v>
+      </c>
+      <c r="E9" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -11449,10 +11750,16 @@
         <v>720</v>
       </c>
       <c r="D10" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>870</v>
+      </c>
+      <c r="E10" t="s">
+        <v>727</v>
+      </c>
+      <c r="F10" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -11464,235 +11771,286 @@
         <v>723</v>
       </c>
       <c r="D11" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>871</v>
+      </c>
+      <c r="E11" t="s">
+        <v>730</v>
+      </c>
+      <c r="F11" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C12" t="s">
-        <v>812</v>
-      </c>
-      <c r="D12" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>811</v>
+      </c>
+      <c r="E12" t="s">
+        <v>827</v>
+      </c>
+      <c r="F12" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C13" t="s">
-        <v>813</v>
-      </c>
-      <c r="D13" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>812</v>
+      </c>
+      <c r="E13" t="s">
+        <v>827</v>
+      </c>
+      <c r="F13" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C14" t="s">
-        <v>814</v>
-      </c>
-      <c r="D14" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>813</v>
+      </c>
+      <c r="E14" t="s">
+        <v>827</v>
+      </c>
+      <c r="F14" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C15" t="s">
-        <v>815</v>
-      </c>
-      <c r="D15" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>814</v>
+      </c>
+      <c r="E15" t="s">
+        <v>827</v>
+      </c>
+      <c r="F15" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C16" t="s">
-        <v>821</v>
-      </c>
-      <c r="D16" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>820</v>
+      </c>
+      <c r="E16" t="s">
+        <v>830</v>
+      </c>
+      <c r="F16" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C17" t="s">
-        <v>816</v>
-      </c>
-      <c r="D17" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>815</v>
+      </c>
+      <c r="E17" t="s">
+        <v>828</v>
+      </c>
+      <c r="F17" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C18" t="s">
-        <v>817</v>
-      </c>
-      <c r="D18" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>816</v>
+      </c>
+      <c r="E18" t="s">
+        <v>828</v>
+      </c>
+      <c r="F18" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C19" t="s">
-        <v>818</v>
-      </c>
-      <c r="D19" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>817</v>
+      </c>
+      <c r="E19" t="s">
+        <v>828</v>
+      </c>
+      <c r="F19" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C20" t="s">
-        <v>819</v>
-      </c>
-      <c r="D20" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>818</v>
+      </c>
+      <c r="E20" t="s">
+        <v>828</v>
+      </c>
+      <c r="F20" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C21" t="s">
-        <v>820</v>
-      </c>
-      <c r="D21" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>819</v>
+      </c>
+      <c r="E21" t="s">
+        <v>828</v>
+      </c>
+      <c r="F21" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C22" t="s">
-        <v>823</v>
-      </c>
-      <c r="D22" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>822</v>
+      </c>
+      <c r="E22" t="s">
+        <v>828</v>
+      </c>
+      <c r="F22" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C23" t="s">
-        <v>824</v>
-      </c>
-      <c r="D23" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>823</v>
+      </c>
+      <c r="E23" t="s">
+        <v>828</v>
+      </c>
+      <c r="F23" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C24" t="s">
-        <v>825</v>
-      </c>
-      <c r="D24" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>824</v>
+      </c>
+      <c r="E24" t="s">
+        <v>828</v>
+      </c>
+      <c r="F24" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C25" t="s">
-        <v>826</v>
-      </c>
-      <c r="D25" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>825</v>
+      </c>
+      <c r="E25" t="s">
+        <v>828</v>
+      </c>
+      <c r="F25" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C26" t="s">
-        <v>827</v>
-      </c>
-      <c r="D26" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>826</v>
+      </c>
+      <c r="E26" t="s">
+        <v>828</v>
+      </c>
+      <c r="F26" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -11703,11 +12061,14 @@
       <c r="C27" t="s">
         <v>689</v>
       </c>
-      <c r="D27" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>828</v>
+      </c>
+      <c r="F27" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -11718,11 +12079,14 @@
       <c r="C28" t="s">
         <v>688</v>
       </c>
-      <c r="D28" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>829</v>
+      </c>
+      <c r="F28" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -11733,11 +12097,14 @@
       <c r="C29" t="s">
         <v>715</v>
       </c>
-      <c r="D29" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>829</v>
+      </c>
+      <c r="F29" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -11748,11 +12115,14 @@
       <c r="C30" t="s">
         <v>722</v>
       </c>
-      <c r="D30" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>829</v>
+      </c>
+      <c r="F30" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -11763,11 +12133,14 @@
       <c r="C31" t="s">
         <v>717</v>
       </c>
-      <c r="D31" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>859</v>
+      </c>
+      <c r="F31" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -11778,11 +12151,14 @@
       <c r="C32" t="s">
         <v>201</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -11793,11 +12169,14 @@
       <c r="C33" t="s">
         <v>202</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -11808,11 +12187,14 @@
       <c r="C34" t="s">
         <v>200</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -11823,11 +12205,14 @@
       <c r="C35" t="s">
         <v>196</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -11838,11 +12223,14 @@
       <c r="C36" t="s">
         <v>198</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -11853,11 +12241,14 @@
       <c r="C37" t="s">
         <v>637</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -11868,11 +12259,14 @@
       <c r="C38" t="s">
         <v>686</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -11883,11 +12277,14 @@
       <c r="C39" t="s">
         <v>686</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -11898,11 +12295,14 @@
       <c r="C40" t="s">
         <v>719</v>
       </c>
-      <c r="D40" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>726</v>
+      </c>
+      <c r="F40" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -11911,30 +12311,36 @@
         <v>721</v>
       </c>
       <c r="C41" t="s">
+        <v>728</v>
+      </c>
+      <c r="E41" t="s">
         <v>729</v>
       </c>
-      <c r="D41" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C42" t="s">
-        <v>822</v>
-      </c>
-      <c r="D42" t="s">
-        <v>832</v>
+        <v>821</v>
+      </c>
+      <c r="E42" t="s">
+        <v>831</v>
+      </c>
+      <c r="F42" t="s">
+        <v>861</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D42">
-    <sortCondition ref="D2:D42"/>
+  <sortState ref="A2:E42">
+    <sortCondition ref="E2:E42"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}">
@@ -12126,18 +12532,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
FIX BUG: for preprocessing.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张亮:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Use '|' to separate different variable names.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -339,30 +363,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>张亮:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-Use '|' to separate different variable names.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E26" authorId="0" shapeId="0">
       <text>
         <r>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="874">
   <si>
     <t>符号判断</t>
   </si>
@@ -3448,14 +3448,6 @@
   </si>
   <si>
     <t>alltime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NSN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RECORD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4153,13 +4145,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4170,23 +4162,24 @@
     <col min="4" max="4" width="16.1328125" style="21" customWidth="1"/>
     <col min="5" max="5" width="16.1328125" customWidth="1"/>
     <col min="6" max="6" width="15" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.73046875" customWidth="1"/>
-    <col min="11" max="11" width="15" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.265625" customWidth="1"/>
-    <col min="13" max="13" width="14.73046875" customWidth="1"/>
-    <col min="14" max="14" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.73046875" customWidth="1"/>
-    <col min="16" max="16" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.46484375" style="21" customWidth="1"/>
-    <col min="19" max="19" width="57.1328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.73046875" customWidth="1"/>
+    <col min="12" max="12" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.265625" customWidth="1"/>
+    <col min="14" max="14" width="14.73046875" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.73046875" customWidth="1"/>
+    <col min="17" max="17" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.46484375" style="21" customWidth="1"/>
+    <col min="20" max="20" width="57.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -4205,59 +4198,62 @@
       <c r="F1" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="49" t="s">
+        <v>872</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>576</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>616</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -4275,49 +4271,52 @@
       <c r="F2" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2">
         <v>0.5</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="2"/>
+      <c r="O2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="S2" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>602</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4335,49 +4334,52 @@
       <c r="F3" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="H3" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
         <v>0.5</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="2"/>
+      <c r="O3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="Q3" s="24" t="s">
+      <c r="R3" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="S3" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>602</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4395,49 +4397,52 @@
       <c r="F4" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
         <v>0.5</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="L4" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="R4" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="S4" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>602</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4455,49 +4460,52 @@
       <c r="F5" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
         <v>0.5</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="L5" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="2"/>
+      <c r="O5" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="R5" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="S5" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>602</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4515,49 +4523,52 @@
       <c r="F6" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
         <v>0.5</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="L6" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="2"/>
+      <c r="O6" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="R6" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="S6" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>602</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4575,49 +4586,52 @@
       <c r="F7" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="50" t="s">
+        <v>873</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2">
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
         <v>0.5</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="L7" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="Q7" s="24" t="s">
+      <c r="R7" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="S7" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>602</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4635,33 +4649,34 @@
       <c r="F8" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="2"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="20"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" t="s">
         <v>578</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="R8" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4679,50 +4694,51 @@
       <c r="F9" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="29" t="s">
         <v>535</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>3000</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>0.5</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="L9" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
-      <c r="O9" t="s">
+      <c r="O9" s="8"/>
+      <c r="P9" t="s">
         <v>524</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="R9" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="R9" s="21" t="s">
+      <c r="S9" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>603</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>599</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="V9" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="V9">
-        <v>2</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="W9">
+        <v>2</v>
+      </c>
+      <c r="X9" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4740,50 +4756,51 @@
       <c r="F10" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="27" t="s">
         <v>535</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>3000</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>0.5</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="L10" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
-      <c r="O10" t="s">
+      <c r="O10" s="8"/>
+      <c r="P10" t="s">
         <v>524</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="R10" s="24" t="s">
         <v>581</v>
       </c>
-      <c r="R10" s="21" t="s">
+      <c r="S10" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>603</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>599</v>
       </c>
-      <c r="U10" s="8" t="s">
+      <c r="V10" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="V10">
-        <v>2</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="W10">
+        <v>2</v>
+      </c>
+      <c r="X10" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4801,49 +4818,50 @@
       <c r="F11" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="27" t="s">
         <v>575</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I11" s="8">
+      <c r="J11" s="8">
         <v>2000</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>0.5</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="L11" s="27" t="s">
         <v>605</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="M11" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="39"/>
+      <c r="P11" s="8"/>
       <c r="Q11" s="39"/>
-      <c r="R11" s="21" t="s">
+      <c r="R11" s="39"/>
+      <c r="S11" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>606</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>599</v>
       </c>
-      <c r="U11" s="8" t="s">
+      <c r="V11" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="V11">
-        <v>2</v>
-      </c>
-      <c r="W11" t="s">
+      <c r="W11">
+        <v>2</v>
+      </c>
+      <c r="X11" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4861,48 +4879,49 @@
       <c r="F12" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="27" t="s">
         <v>575</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I12" s="8">
+      <c r="J12" s="8">
         <v>3000</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>0.5</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="L12" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="M12" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="P12" s="39"/>
+      <c r="O12" s="8"/>
       <c r="Q12" s="39"/>
-      <c r="R12" s="21" t="s">
+      <c r="R12" s="39"/>
+      <c r="S12" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>607</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>600</v>
       </c>
-      <c r="U12" s="8" t="s">
+      <c r="V12" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="V12">
-        <v>2</v>
-      </c>
-      <c r="W12" t="s">
+      <c r="W12">
+        <v>2</v>
+      </c>
+      <c r="X12" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4920,57 +4939,58 @@
       <c r="F13" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I13" s="10">
+      <c r="J13" s="10">
         <v>2000</v>
       </c>
-      <c r="J13" s="8">
+      <c r="K13" s="8">
         <v>0.5</v>
       </c>
-      <c r="K13" s="28" t="s">
+      <c r="L13" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="O13" s="18" t="s">
+      <c r="P13" s="18" t="s">
         <v>658</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="40"/>
+      <c r="R13" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="R13" s="22" t="s">
+      <c r="S13" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>642</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>3000</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="V13" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="V13">
-        <v>2</v>
-      </c>
-      <c r="W13" t="s">
+      <c r="W13">
+        <v>2</v>
+      </c>
+      <c r="X13" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4988,51 +5008,52 @@
       <c r="F14" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>3000</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="2"/>
+      <c r="L14" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="2"/>
+      <c r="P14" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="17" t="s">
+      <c r="Q14" s="39"/>
+      <c r="R14" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="S14" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>609</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>610</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>3</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5050,55 +5071,56 @@
       <c r="F15" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="5"/>
+      <c r="H15" s="20" t="s">
         <v>487</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>3000</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>0.5</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="L15" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2" t="s">
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O15" s="17" t="s">
+      <c r="P15" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="17" t="s">
+      <c r="Q15" s="39"/>
+      <c r="R15" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="R15" s="21" t="s">
+      <c r="S15" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="S15" s="31" t="s">
+      <c r="T15" s="31" t="s">
         <v>614</v>
       </c>
-      <c r="T15" s="32" t="s">
+      <c r="U15" s="32" t="s">
         <v>611</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="V15" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>3</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5116,55 +5138,56 @@
       <c r="F16" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="20" t="s">
         <v>535</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>3000</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>0.5</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="L16" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2" t="s">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O16" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="O16" s="17" t="s">
+      <c r="P16" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="17" t="s">
+      <c r="Q16" s="39"/>
+      <c r="R16" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="R16" s="21" t="s">
+      <c r="S16" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>609</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>612</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="V16" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>3</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5182,51 +5205,52 @@
       <c r="F17" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="5"/>
+      <c r="H17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>3000</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="2"/>
+      <c r="L17" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="17" t="s">
+      <c r="O17" s="2"/>
+      <c r="P17" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="17" t="s">
+      <c r="Q17" s="39"/>
+      <c r="R17" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="R17" s="21" t="s">
+      <c r="S17" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>609</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>613</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>3</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5244,51 +5268,52 @@
       <c r="F18" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>1000</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="2"/>
+      <c r="L18" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2" t="s">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="17" t="s">
+      <c r="O18" s="2"/>
+      <c r="P18" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="17" t="s">
+      <c r="Q18" s="39"/>
+      <c r="R18" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="R18" s="21" t="s">
+      <c r="S18" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>609</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>599</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="V18" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>3</v>
       </c>
-      <c r="W18" t="s">
+      <c r="X18" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5306,47 +5331,48 @@
       <c r="F19" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="5"/>
+      <c r="H19" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="28" t="s">
+      <c r="K19" s="5"/>
+      <c r="L19" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="2"/>
+      <c r="O19" s="5" t="s">
         <v>621</v>
       </c>
-      <c r="O19" s="19"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39" t="s">
+      <c r="P19" s="19"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39" t="s">
         <v>579</v>
       </c>
-      <c r="R19" s="21" t="s">
+      <c r="S19" s="21" t="s">
         <v>590</v>
       </c>
-      <c r="S19" s="5" t="s">
+      <c r="T19" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>600</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="V19" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>4</v>
       </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5364,48 +5390,49 @@
       <c r="F20" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="5"/>
+      <c r="H20" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I20" s="5">
+      <c r="J20" s="5">
         <v>1000</v>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="20" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2" t="s">
+      <c r="N20" s="2"/>
+      <c r="O20" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39" t="s">
+      <c r="P20" s="19"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39" t="s">
         <v>646</v>
       </c>
-      <c r="R20" s="21" t="s">
+      <c r="S20" s="21" t="s">
         <v>591</v>
       </c>
-      <c r="S20" s="5" t="s">
+      <c r="T20" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="V20" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>4</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5423,47 +5450,48 @@
       <c r="F21" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="5"/>
+      <c r="H21" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I21" s="5">
+      <c r="J21" s="5">
         <v>500</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="20" t="s">
+      <c r="K21" s="5"/>
+      <c r="L21" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="18" t="s">
+      <c r="N21" s="10"/>
+      <c r="O21" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="O21" s="10"/>
-      <c r="Q21" s="25" t="s">
+      <c r="P21" s="10"/>
+      <c r="R21" s="25" t="s">
         <v>580</v>
       </c>
-      <c r="R21" s="21" t="s">
+      <c r="S21" s="21" t="s">
         <v>591</v>
       </c>
-      <c r="S21" s="5" t="s">
+      <c r="T21" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="V21" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>4</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5481,55 +5509,56 @@
       <c r="F22" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="5"/>
+      <c r="H22" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>1000</v>
       </c>
-      <c r="J22" s="5">
+      <c r="K22" s="5">
         <v>0.5</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="L22" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O22" s="19"/>
-      <c r="P22" t="s">
+      <c r="P22" s="19"/>
+      <c r="Q22" t="s">
         <v>498</v>
       </c>
-      <c r="Q22" s="26" t="s">
+      <c r="R22" s="26" t="s">
         <v>632</v>
       </c>
-      <c r="R22" s="22" t="s">
+      <c r="S22" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="S22" s="17" t="s">
+      <c r="T22" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="T22" s="17" t="s">
+      <c r="U22" s="17" t="s">
         <v>618</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="V22" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>4</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5547,55 +5576,56 @@
       <c r="F23" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="I23" s="5">
+      <c r="J23" s="5">
         <v>1000</v>
       </c>
-      <c r="J23" s="5">
+      <c r="K23" s="5">
         <v>0.5</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="L23" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="2"/>
+      <c r="O23" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="O23" s="19"/>
-      <c r="P23" t="s">
+      <c r="P23" s="19"/>
+      <c r="Q23" t="s">
         <v>498</v>
       </c>
-      <c r="Q23" s="26" t="s">
+      <c r="R23" s="26" t="s">
         <v>632</v>
       </c>
-      <c r="R23" s="22" t="s">
+      <c r="S23" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="S23" s="17" t="s">
+      <c r="T23" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="T23" s="17" t="s">
+      <c r="U23" s="17" t="s">
         <v>619</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="V23" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>4</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5613,50 +5643,51 @@
       <c r="F24" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="5"/>
+      <c r="H24" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>2000</v>
       </c>
-      <c r="J24" s="2">
+      <c r="K24" s="2">
         <v>0.5</v>
       </c>
-      <c r="K24" s="20" t="s">
+      <c r="L24" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="2"/>
+      <c r="O24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O24" s="19"/>
-      <c r="Q24" s="26" t="s">
+      <c r="P24" s="19"/>
+      <c r="R24" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="R24" s="22" t="s">
+      <c r="S24" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="S24" s="5" t="s">
+      <c r="T24" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="T24" s="17"/>
-      <c r="U24" s="2" t="s">
+      <c r="U24" s="17"/>
+      <c r="V24" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>5</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5674,50 +5705,51 @@
       <c r="F25" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="5"/>
+      <c r="H25" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>0</v>
       </c>
-      <c r="J25" s="2">
+      <c r="K25" s="2">
         <v>0.5</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="L25" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2" t="s">
+      <c r="N25" s="2"/>
+      <c r="O25" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="O25" s="19"/>
-      <c r="Q25" s="26" t="s">
+      <c r="P25" s="19"/>
+      <c r="R25" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="R25" s="22" t="s">
+      <c r="S25" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="S25" s="5" t="s">
+      <c r="T25" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="T25" s="17"/>
-      <c r="U25" s="2" t="s">
+      <c r="U25" s="17"/>
+      <c r="V25" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>5</v>
       </c>
-      <c r="W25" t="s">
+      <c r="X25" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5735,56 +5767,57 @@
       <c r="F26" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="5"/>
+      <c r="H26" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>3000</v>
       </c>
-      <c r="J26" s="2">
+      <c r="K26" s="2">
         <v>0.5</v>
       </c>
-      <c r="K26" s="28" t="s">
+      <c r="L26" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="N26" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="O26" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>660</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>658</v>
       </c>
-      <c r="R26" s="22" t="s">
+      <c r="S26" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>642</v>
       </c>
-      <c r="T26" s="17">
+      <c r="U26" s="17">
         <v>2000</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="V26" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>5</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5802,56 +5835,57 @@
       <c r="F27" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="5"/>
+      <c r="H27" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>3000</v>
       </c>
-      <c r="J27" s="2">
+      <c r="K27" s="2">
         <v>0.25</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="L27" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="M27" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="N27" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="O27" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>660</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>658</v>
       </c>
-      <c r="R27" s="22" t="s">
+      <c r="S27" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>642</v>
       </c>
-      <c r="T27" s="17">
+      <c r="U27" s="17">
         <v>3000</v>
       </c>
-      <c r="U27" s="2" t="s">
+      <c r="V27" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>5</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5869,54 +5903,55 @@
       <c r="F28" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2">
+      <c r="J28" s="2"/>
+      <c r="K28" s="2">
         <v>0.25</v>
       </c>
-      <c r="K28" s="28" t="s">
+      <c r="L28" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="M28" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="M28" s="5" t="s">
+      <c r="N28" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="O28" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>660</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>658</v>
       </c>
-      <c r="R28" s="22" t="s">
+      <c r="S28" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>642</v>
       </c>
-      <c r="T28" s="17">
+      <c r="U28" s="17">
         <v>3000</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="V28" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>5</v>
       </c>
-      <c r="W28" t="s">
+      <c r="X28" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5934,51 +5969,52 @@
       <c r="F29" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="5"/>
+      <c r="H29" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>3000</v>
       </c>
-      <c r="J29" s="2">
+      <c r="K29" s="2">
         <v>0.5</v>
       </c>
-      <c r="K29" s="28" t="s">
+      <c r="L29" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="N29" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="O29" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>660</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>658</v>
       </c>
-      <c r="R29" s="22"/>
-      <c r="T29" s="17">
+      <c r="S29" s="22"/>
+      <c r="U29" s="17">
         <v>3000</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="V29" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>5</v>
       </c>
-      <c r="W29" t="s">
+      <c r="X29" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5996,51 +6032,52 @@
       <c r="F30" s="20" t="s">
         <v>693</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="5"/>
+      <c r="H30" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>3000</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>0.5</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="L30" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="N30" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="O30" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>660</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>658</v>
       </c>
-      <c r="R30" s="22"/>
-      <c r="T30" s="17">
+      <c r="S30" s="22"/>
+      <c r="U30" s="17">
         <v>3000</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="V30" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>5</v>
       </c>
-      <c r="W30" t="s">
+      <c r="X30" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6058,47 +6095,48 @@
       <c r="F31" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G31" s="28" t="s">
+      <c r="G31" s="5"/>
+      <c r="H31" s="28" t="s">
         <v>535</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>2000</v>
       </c>
-      <c r="J31" s="2">
+      <c r="K31" s="2">
         <v>0.5</v>
       </c>
-      <c r="K31" s="20" t="s">
+      <c r="L31" s="20" t="s">
         <v>570</v>
       </c>
-      <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="Q31" s="24" t="s">
+      <c r="O31" s="2"/>
+      <c r="R31" s="24" t="s">
         <v>582</v>
       </c>
-      <c r="R31" s="22" t="s">
+      <c r="S31" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>609</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>620</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="V31" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>5</v>
       </c>
-      <c r="W31" t="s">
+      <c r="X31" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -6116,47 +6154,48 @@
       <c r="F32" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G32" s="30" t="s">
+      <c r="G32" s="5"/>
+      <c r="H32" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>2000</v>
       </c>
-      <c r="J32" s="2">
+      <c r="K32" s="2">
         <v>0.5</v>
       </c>
-      <c r="K32" s="20" t="s">
+      <c r="L32" s="20" t="s">
         <v>571</v>
       </c>
-      <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="Q32" s="24" t="s">
+      <c r="O32" s="2"/>
+      <c r="R32" s="24" t="s">
         <v>583</v>
       </c>
-      <c r="R32" s="22" t="s">
+      <c r="S32" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>609</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>620</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="V32" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>5</v>
       </c>
-      <c r="W32" t="s">
+      <c r="X32" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -6174,43 +6213,44 @@
       <c r="F33" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="5"/>
+      <c r="H33" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="28" t="s">
+      <c r="K33" s="5"/>
+      <c r="L33" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="Q33" s="24" t="s">
+      <c r="O33" s="2"/>
+      <c r="R33" s="24" t="s">
         <v>584</v>
       </c>
-      <c r="R33" s="22" t="s">
+      <c r="S33" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="S33" s="5" t="s">
+      <c r="T33" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="T33" s="17">
+      <c r="U33" s="17">
         <v>400</v>
       </c>
-      <c r="U33" s="2" t="s">
+      <c r="V33" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>6</v>
       </c>
-      <c r="W33" t="s">
+      <c r="X33" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A53" si="1">ROW() - 1</f>
         <v>33</v>
@@ -6228,43 +6268,44 @@
       <c r="F34" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="5"/>
+      <c r="H34" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I34" s="5"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="28" t="s">
+      <c r="K34" s="5"/>
+      <c r="L34" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="Q34" s="24" t="s">
+      <c r="O34" s="2"/>
+      <c r="R34" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="R34" s="22" t="s">
+      <c r="S34" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="S34" s="5" t="s">
+      <c r="T34" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="T34" s="17">
+      <c r="U34" s="17">
         <v>500</v>
       </c>
-      <c r="U34" s="2" t="s">
+      <c r="V34" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>6</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -6282,43 +6323,44 @@
       <c r="F35" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="5"/>
+      <c r="H35" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="28" t="s">
+      <c r="K35" s="5"/>
+      <c r="L35" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="Q35" s="24" t="s">
+      <c r="O35" s="2"/>
+      <c r="R35" s="24" t="s">
         <v>586</v>
       </c>
-      <c r="R35" s="22" t="s">
+      <c r="S35" s="22" t="s">
         <v>596</v>
       </c>
-      <c r="S35" s="5" t="s">
+      <c r="T35" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="T35" s="17">
+      <c r="U35" s="17">
         <v>600</v>
       </c>
-      <c r="U35" s="2" t="s">
+      <c r="V35" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>6</v>
       </c>
-      <c r="W35" t="s">
+      <c r="X35" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6336,49 +6378,50 @@
       <c r="F36" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="5"/>
+      <c r="H36" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>2000</v>
       </c>
-      <c r="J36" s="2">
+      <c r="K36" s="2">
         <v>0.25</v>
       </c>
-      <c r="K36" s="20" t="s">
+      <c r="L36" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="L36" s="3" t="s">
+      <c r="M36" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="Q36" s="24" t="s">
+      <c r="O36" s="2"/>
+      <c r="R36" s="24" t="s">
         <v>631</v>
       </c>
-      <c r="R36" s="22" t="s">
+      <c r="S36" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="S36" s="17" t="s">
+      <c r="T36" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="T36" s="17" t="s">
+      <c r="U36" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="U36" s="2" t="s">
+      <c r="V36" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>6</v>
       </c>
-      <c r="W36" t="s">
+      <c r="X36" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -6396,54 +6439,55 @@
       <c r="F37" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="5"/>
+      <c r="H37" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>2000</v>
       </c>
-      <c r="J37" s="2">
+      <c r="K37" s="2">
         <v>0.5</v>
       </c>
-      <c r="K37" s="28" t="s">
+      <c r="L37" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="M37" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="5" t="s">
+      <c r="N37" s="2"/>
+      <c r="O37" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="O37" s="5" t="s">
+      <c r="P37" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="Q37" s="24" t="s">
+      <c r="R37" s="24" t="s">
         <v>647</v>
       </c>
-      <c r="R37" s="22" t="s">
+      <c r="S37" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="S37" s="17" t="s">
+      <c r="T37" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="T37" s="17" t="s">
+      <c r="U37" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="V37" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>6</v>
       </c>
-      <c r="W37" t="s">
+      <c r="X37" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -6461,54 +6505,55 @@
       <c r="F38" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="5"/>
+      <c r="H38" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>2000</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>0.5</v>
       </c>
-      <c r="K38" s="28" t="s">
+      <c r="L38" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="5" t="s">
+      <c r="N38" s="2"/>
+      <c r="O38" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="O38" s="5" t="s">
+      <c r="P38" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="Q38" s="24" t="s">
+      <c r="R38" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="R38" s="22" t="s">
+      <c r="S38" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="S38" s="17" t="s">
+      <c r="T38" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="T38" s="17" t="s">
+      <c r="U38" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="U38" s="2" t="s">
+      <c r="V38" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>6</v>
       </c>
-      <c r="W38" t="s">
+      <c r="X38" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -6526,54 +6571,55 @@
       <c r="F39" s="20" t="s">
         <v>800</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="5"/>
+      <c r="H39" s="20" t="s">
         <v>801</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>2000</v>
       </c>
-      <c r="J39" s="2">
+      <c r="K39" s="2">
         <v>0.5</v>
       </c>
-      <c r="K39" s="28" t="s">
+      <c r="L39" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="5" t="s">
+      <c r="N39" s="2"/>
+      <c r="O39" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="P39" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="Q39" s="24" t="s">
+      <c r="R39" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="R39" s="22" t="s">
+      <c r="S39" s="22" t="s">
         <v>597</v>
       </c>
-      <c r="S39" s="17" t="s">
+      <c r="T39" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="T39" s="17" t="s">
+      <c r="U39" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="U39" s="2" t="s">
+      <c r="V39" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>6</v>
       </c>
-      <c r="W39" t="s">
+      <c r="X39" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -6591,49 +6637,50 @@
       <c r="F40" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="5"/>
+      <c r="H40" s="20" t="s">
         <v>653</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>2000</v>
       </c>
-      <c r="J40" s="2">
+      <c r="K40" s="2">
         <v>0.5</v>
       </c>
-      <c r="K40" s="20" t="s">
+      <c r="L40" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="M40" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2" t="s">
+      <c r="N40" s="2"/>
+      <c r="O40" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="Q40" s="24" t="s">
+      <c r="R40" s="24" t="s">
         <v>654</v>
       </c>
-      <c r="R40" s="22"/>
-      <c r="S40" s="17" t="s">
+      <c r="S40" s="22"/>
+      <c r="T40" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="T40" s="17" t="s">
+      <c r="U40" s="17" t="s">
         <v>628</v>
       </c>
-      <c r="U40" s="2" t="s">
+      <c r="V40" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>6</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -6651,19 +6698,20 @@
       <c r="F41" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="2" t="s">
+      <c r="G41" s="5"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="20"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
-      <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O41" s="2"/>
+      <c r="V41" s="2"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -6681,19 +6729,20 @@
       <c r="F42" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="2" t="s">
+      <c r="G42" s="5"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I42" s="2"/>
       <c r="J42" s="2"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="20"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
-      <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O42" s="2"/>
+      <c r="V42" s="2"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -6709,28 +6758,29 @@
       <c r="F43" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="5"/>
+      <c r="H43" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="20" t="s">
+      <c r="K43" s="2"/>
+      <c r="L43" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
-      <c r="Q43" s="20" t="s">
+      <c r="O43" s="2"/>
+      <c r="R43" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="U43" s="2" t="s">
+      <c r="V43" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6746,17 +6796,18 @@
       <c r="F44" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="2"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="20"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="20"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
-      <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O44" s="2"/>
+      <c r="V44" s="2"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -6772,17 +6823,18 @@
       <c r="F45" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="2"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="20"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="20"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
-      <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="O45" s="2"/>
+      <c r="V45" s="2"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -6796,8 +6848,9 @@
       <c r="F46" s="20" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -6813,8 +6866,9 @@
       <c r="F47" s="20" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -6829,8 +6883,9 @@
       <c r="F48" s="20" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -6845,8 +6900,9 @@
       <c r="F49" s="20" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -6861,8 +6917,9 @@
       <c r="F50" s="20" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -6877,8 +6934,9 @@
       <c r="F51" s="20" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -6892,8 +6950,9 @@
       <c r="F52" s="20" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -6909,8 +6968,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AD51">
-    <sortCondition ref="V2:V51"/>
+  <sortState ref="A2:AE51">
+    <sortCondition ref="W2:W51"/>
   </sortState>
   <customSheetViews>
     <customSheetView guid="{EA03B590-7847-4E8E-A1B2-851363113915}" topLeftCell="A11">
@@ -8964,10 +9023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -8979,11 +9038,9 @@
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.06640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>533</v>
       </c>
@@ -9008,17 +9065,8 @@
       <c r="H1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="I1" s="49" t="s">
-        <v>872</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f>ROW() - 1</f>
         <v>1</v>
@@ -9039,17 +9087,8 @@
         <v>1</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="I2" s="50" t="s">
-        <v>873</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>874</v>
-      </c>
-      <c r="K2" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f>ROW() - 1</f>
         <v>2</v>
@@ -9070,11 +9109,10 @@
         <v>2</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="I3" s="50"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A32" si="0">ROW() - 1</f>
+        <f>ROW() - 1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -9093,14 +9131,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="29" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -9119,11 +9153,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="I5" s="50"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -9142,11 +9175,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="I6" s="50"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -9165,11 +9197,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="I7" s="50"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -9188,11 +9219,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -9211,11 +9241,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -9234,11 +9263,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -9257,11 +9285,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -9280,11 +9307,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -9305,11 +9331,10 @@
       <c r="G13" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -9328,11 +9353,10 @@
         <v>216</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -9353,11 +9377,10 @@
       <c r="H15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>15</v>
       </c>
       <c r="B16" s="46" t="s">
@@ -9376,12 +9399,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="46"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="51"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -9402,11 +9423,10 @@
       <c r="G17" s="5" t="s">
         <v>794</v>
       </c>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -9425,11 +9445,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -9448,11 +9467,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -9471,11 +9489,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -9494,11 +9511,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -9517,11 +9533,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -9540,11 +9555,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -9565,11 +9579,10 @@
       <c r="H24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -9588,11 +9601,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -9610,11 +9622,10 @@
       <c r="F26" s="5">
         <v>0</v>
       </c>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -9629,11 +9640,10 @@
       <c r="E27" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -9648,11 +9658,10 @@
       <c r="E28" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -9670,11 +9679,10 @@
       <c r="F29">
         <v>124</v>
       </c>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -9686,11 +9694,10 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -9702,11 +9709,10 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <f t="shared" si="0"/>
+        <f>ROW() - 1</f>
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -9721,67 +9727,6 @@
       <c r="E32" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I44" s="5"/>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I47" s="5"/>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>

</xml_diff>

<commit_message>
ADD FEATURE: Add support for alltime property. Notice: there might be further compatibility problem in the future version.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-Use '|' to separate different variable names.</t>
+Use space (' ') to separate different variable names.</t>
         </r>
       </text>
     </comment>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="876">
   <si>
     <t>符号判断</t>
   </si>
@@ -3448,6 +3448,14 @@
   </si>
   <si>
     <t>alltime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语义判断(高级)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语义判断(高级)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4147,11 +4155,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9068,7 +9076,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" ref="A2:A32" si="0">ROW() - 1</f>
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -9090,7 +9098,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -9112,7 +9120,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -9134,7 +9142,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -9156,7 +9164,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -9178,7 +9186,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -9200,7 +9208,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -9222,7 +9230,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -9244,7 +9252,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -9266,7 +9274,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -9288,7 +9296,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -9310,7 +9318,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -9334,7 +9342,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -9356,7 +9364,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -9380,7 +9388,7 @@
     </row>
     <row r="16" spans="1:8" s="48" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="45">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="46" t="s">
@@ -9402,7 +9410,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -9426,7 +9434,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -9448,7 +9456,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -9470,7 +9478,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -9492,7 +9500,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -9514,7 +9522,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -9536,7 +9544,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -9558,7 +9566,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -9582,7 +9590,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -9604,7 +9612,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -9625,7 +9633,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -9643,7 +9651,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -9661,7 +9669,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -9682,7 +9690,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -9697,7 +9705,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -9712,7 +9720,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <f>ROW() - 1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -9747,8 +9755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -11244,11 +11252,11 @@
         <v>746</v>
       </c>
       <c r="D83" t="s">
-        <v>746</v>
-      </c>
-      <c r="E83" t="e">
+        <v>875</v>
+      </c>
+      <c r="E83" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D83, settings!B$2:B$53, 0))</f>
-        <v>#N/A</v>
+        <v>Semantic</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -11262,7 +11270,7 @@
         <v>745</v>
       </c>
       <c r="D84" t="s">
-        <v>745</v>
+        <v>874</v>
       </c>
       <c r="E84" t="str">
         <f>INDEX(settings!C$2:C$53, MATCH(taskname!D84, settings!B$2:B$53, 0))</f>

</xml_diff>

<commit_message>
FIX BUG: Compatibility consideration better now. Support for more flexible meta vars.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -2756,10 +2756,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>H1 R1 H2 R2 Delay Resp RT CurUtility TotalUtility</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>记忆尾巴（空间位置）</t>
   </si>
   <si>
@@ -3494,6 +3490,10 @@
   </si>
   <si>
     <t>angACC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H1 R1 H2 R2 Delay Resp RT CurUtility TotalUtility\X1 X2 Delay H1 R1 H2 R2 Resp RT CurUtility TotalUtility</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4177,8 +4177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
@@ -4220,16 +4220,16 @@
         <v>79</v>
       </c>
       <c r="D1" s="40" t="s">
+        <v>686</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>687</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>688</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>147</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>27</v>
@@ -4295,7 +4295,7 @@
         <v>94</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="20" t="s">
@@ -4354,7 +4354,7 @@
         <v>90</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="20" t="s">
@@ -4414,7 +4414,7 @@
         <v>91</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="20" t="s">
@@ -4473,7 +4473,7 @@
         <v>92</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="20" t="s">
@@ -4540,7 +4540,7 @@
         <v>93</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="20" t="s">
@@ -4607,7 +4607,7 @@
         <v>104</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="20" t="s">
@@ -4676,7 +4676,7 @@
         <v>116</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="20" t="s">
@@ -4738,7 +4738,7 @@
         <v>119</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="20" t="s">
@@ -4800,7 +4800,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="20" t="s">
@@ -4868,7 +4868,7 @@
         <v>102</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="20" t="s">
@@ -4937,7 +4937,7 @@
         <v>103</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="20" t="s">
@@ -5004,7 +5004,7 @@
         <v>154</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="20" t="s">
@@ -5030,11 +5030,11 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="Q13" s="39"/>
       <c r="R13" s="4" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="S13" s="22" t="s">
         <v>590</v>
@@ -5067,7 +5067,7 @@
         <v>105</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="20" t="s">
@@ -5093,11 +5093,11 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="Q14" s="39"/>
       <c r="R14" s="4" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="S14" s="22" t="s">
         <v>593</v>
@@ -5130,17 +5130,17 @@
         <v>659</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>660</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="21" t="s">
+        <v>873</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>874</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>875</v>
       </c>
       <c r="J15">
         <v>1000</v>
@@ -5149,11 +5149,11 @@
         <v>0.5</v>
       </c>
       <c r="P15" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Q15" s="39"/>
       <c r="R15" s="5" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="W15">
         <v>5</v>
@@ -5174,7 +5174,7 @@
         <v>113</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="20" t="s">
@@ -5237,7 +5237,7 @@
         <v>114</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="20" t="s">
@@ -5300,7 +5300,7 @@
         <v>89</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="20" t="s">
@@ -5328,11 +5328,11 @@
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Q18" s="39"/>
       <c r="R18" s="5" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="S18" s="21" t="s">
         <v>586</v>
@@ -5365,7 +5365,7 @@
         <v>526</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="20" t="s">
@@ -5425,7 +5425,7 @@
         <v>95</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="20" t="s">
@@ -5481,7 +5481,7 @@
         <v>96</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="20" t="s">
@@ -5536,7 +5536,7 @@
         <v>110</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="20" t="s">
@@ -5591,7 +5591,7 @@
         <v>97</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="20" t="s">
@@ -5619,10 +5619,10 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="R23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="S23" s="22" t="s">
         <v>595</v>
@@ -5655,7 +5655,7 @@
         <v>98</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="20" t="s">
@@ -5721,7 +5721,7 @@
         <v>99</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="20" t="s">
@@ -5781,21 +5781,21 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>795</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>796</v>
-      </c>
       <c r="D26" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="20" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="20" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>529</v>
@@ -5853,7 +5853,7 @@
         <v>100</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="20" t="s">
@@ -5914,14 +5914,14 @@
         <v>80</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G28" s="49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H28" s="20" t="s">
         <v>203</v>
@@ -5977,14 +5977,14 @@
         <v>81</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H29" s="20" t="s">
         <v>203</v>
@@ -6040,14 +6040,14 @@
         <v>82</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G30" s="49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H30" s="20" t="s">
         <v>203</v>
@@ -6103,14 +6103,14 @@
         <v>83</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G31" s="49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H31" s="20" t="s">
         <v>203</v>
@@ -6166,14 +6166,14 @@
         <v>84</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G32" s="49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H32" s="20" t="s">
         <v>203</v>
@@ -6229,14 +6229,14 @@
         <v>85</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G33" s="49" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H33" s="20" t="s">
         <v>203</v>
@@ -6292,7 +6292,7 @@
         <v>219</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="20" t="s">
@@ -6337,7 +6337,7 @@
         <v>86</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="20" t="s">
@@ -6400,7 +6400,7 @@
         <v>87</v>
       </c>
       <c r="D36" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="20" t="s">
@@ -6467,7 +6467,7 @@
         <v>88</v>
       </c>
       <c r="D37" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="20" t="s">
@@ -6534,7 +6534,7 @@
         <v>117</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="20" t="s">
@@ -6597,7 +6597,7 @@
         <v>118</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="20" t="s">
@@ -6660,7 +6660,7 @@
         <v>106</v>
       </c>
       <c r="D40" s="41" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E40" s="13"/>
       <c r="F40" s="20" t="s">
@@ -6717,17 +6717,17 @@
         <v>40</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E41" s="13"/>
       <c r="F41" s="20" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="20" t="s">
@@ -6786,7 +6786,7 @@
         <v>107</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="20" t="s">
@@ -6817,7 +6817,7 @@
         <v>108</v>
       </c>
       <c r="D43" s="41" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E43" s="13"/>
       <c r="F43" s="20" t="s">
@@ -6959,7 +6959,7 @@
         <v>672</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="20" t="s">
@@ -6973,17 +6973,17 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C49" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="20" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G49" s="5"/>
     </row>
@@ -6993,17 +6993,17 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C50" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="20" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G50" s="5"/>
     </row>
@@ -7013,17 +7013,17 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C51" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="20" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G51" s="5"/>
     </row>
@@ -7033,16 +7033,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C52" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G52" s="5"/>
     </row>
@@ -7052,13 +7052,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>702</v>
+      </c>
+      <c r="C53" t="s">
         <v>703</v>
       </c>
-      <c r="C53" t="s">
+      <c r="F53" s="21" t="s">
         <v>704</v>
-      </c>
-      <c r="F53" s="21" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -7067,13 +7067,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C54" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -7082,13 +7082,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C55" t="s">
+        <v>878</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>879</v>
-      </c>
-      <c r="D55" s="21" t="s">
-        <v>880</v>
       </c>
     </row>
   </sheetData>
@@ -9149,8 +9149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -9159,7 +9159,7 @@
     <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.59765625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="5" max="5" width="111.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
@@ -9425,7 +9425,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -9508,7 +9508,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="45" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C16" s="46" t="s">
         <v>137</v>
@@ -9545,7 +9545,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -9664,7 +9664,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>144</v>
@@ -9764,6 +9764,9 @@
       <c r="E27" s="5" t="s">
         <v>670</v>
       </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -9780,7 +9783,10 @@
         <v>674</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>675</v>
+        <v>884</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -9789,16 +9795,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>700</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>678</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>699</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>701</v>
       </c>
       <c r="F29">
         <v>124</v>
@@ -9840,16 +9846,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>706</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>702</v>
-      </c>
-      <c r="D32" s="20" t="s">
+      <c r="E32" s="5" t="s">
         <v>707</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -9884,19 +9890,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C1" t="s">
+        <v>847</v>
+      </c>
+      <c r="D1" t="s">
         <v>848</v>
       </c>
-      <c r="D1" t="s">
-        <v>849</v>
-      </c>
       <c r="E1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -9904,13 +9910,13 @@
         <v>97954</v>
       </c>
       <c r="B2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E2" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D2, settings!B$2:B$1048576, 0))</f>
@@ -9922,13 +9928,13 @@
         <v>100020</v>
       </c>
       <c r="B3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D3" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E3" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D3, settings!B$2:B$1048576, 0))</f>
@@ -9940,13 +9946,13 @@
         <v>97979</v>
       </c>
       <c r="B4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E4" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D4, settings!B$2:B$1048576, 0))</f>
@@ -9976,13 +9982,13 @@
         <v>97962</v>
       </c>
       <c r="B6" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C6" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D6" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E6" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D6, settings!B$2:B$1048576, 0))</f>
@@ -10012,13 +10018,13 @@
         <v>97971</v>
       </c>
       <c r="B8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C8" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D8" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E8" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D8, settings!B$2:B$1048576, 0))</f>
@@ -10030,13 +10036,13 @@
         <v>100003</v>
       </c>
       <c r="B9" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C9" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D9" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E9" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D9, settings!B$2:B$1048576, 0))</f>
@@ -10048,13 +10054,13 @@
         <v>97950</v>
       </c>
       <c r="B10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E10" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D10, settings!B$2:B$1048576, 0))</f>
@@ -10066,13 +10072,13 @@
         <v>97988</v>
       </c>
       <c r="B11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E11" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D11, settings!B$2:B$1048576, 0))</f>
@@ -10084,13 +10090,13 @@
         <v>97983</v>
       </c>
       <c r="B12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E12" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D12, settings!B$2:B$1048576, 0))</f>
@@ -10120,10 +10126,10 @@
         <v>100000</v>
       </c>
       <c r="B14" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C14" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -10138,10 +10144,10 @@
         <v>99994</v>
       </c>
       <c r="B15" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C15" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -10156,7 +10162,7 @@
         <v>99993</v>
       </c>
       <c r="B16" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -10174,13 +10180,13 @@
         <v>97959</v>
       </c>
       <c r="B17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E17" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D17, settings!B$2:B$1048576, 0))</f>
@@ -10192,13 +10198,13 @@
         <v>99990</v>
       </c>
       <c r="B18" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C18" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D18" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E18" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D18, settings!B$2:B$1048576, 0))</f>
@@ -10210,13 +10216,13 @@
         <v>100001</v>
       </c>
       <c r="B19" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C19" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D19" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E19" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D19, settings!B$2:B$1048576, 0))</f>
@@ -10228,13 +10234,13 @@
         <v>97956</v>
       </c>
       <c r="B20" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C20" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D20" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E20" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D20, settings!B$2:B$1048576, 0))</f>
@@ -10264,7 +10270,7 @@
         <v>100019</v>
       </c>
       <c r="B22" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -10282,10 +10288,10 @@
         <v>99996</v>
       </c>
       <c r="B23" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C23" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -10300,10 +10306,10 @@
         <v>99995</v>
       </c>
       <c r="B24" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C24" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -10318,13 +10324,13 @@
         <v>100010</v>
       </c>
       <c r="B25" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C25" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D25" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E25" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D25, settings!B$2:B$1048576, 0))</f>
@@ -10354,13 +10360,13 @@
         <v>97976</v>
       </c>
       <c r="B27" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C27" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D27" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E27" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D27, settings!B$2:B$1048576, 0))</f>
@@ -10372,13 +10378,13 @@
         <v>97991</v>
       </c>
       <c r="B28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E28" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D28, settings!B$2:B$1048576, 0))</f>
@@ -10408,7 +10414,7 @@
         <v>97972</v>
       </c>
       <c r="B30" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -10426,13 +10432,13 @@
         <v>97966</v>
       </c>
       <c r="B31" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C31" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E31" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D31, settings!B$2:B$1048576, 0))</f>
@@ -10444,13 +10450,13 @@
         <v>97987</v>
       </c>
       <c r="B32" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C32" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D32" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E32" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D32, settings!B$2:B$1048576, 0))</f>
@@ -10462,13 +10468,13 @@
         <v>97986</v>
       </c>
       <c r="B33" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C33" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D33" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E33" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D33, settings!B$2:B$1048576, 0))</f>
@@ -10480,13 +10486,13 @@
         <v>97993</v>
       </c>
       <c r="B34" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C34" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D34" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E34" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D34, settings!B$2:B$1048576, 0))</f>
@@ -10498,13 +10504,13 @@
         <v>97992</v>
       </c>
       <c r="B35" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C35" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D35" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E35" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D35, settings!B$2:B$1048576, 0))</f>
@@ -10516,13 +10522,13 @@
         <v>97997</v>
       </c>
       <c r="B36" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C36" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D36" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E36" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D36, settings!B$2:B$1048576, 0))</f>
@@ -10534,13 +10540,13 @@
         <v>97994</v>
       </c>
       <c r="B37" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C37" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D37" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E37" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D37, settings!B$2:B$1048576, 0))</f>
@@ -10552,13 +10558,13 @@
         <v>97990</v>
       </c>
       <c r="B38" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C38" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D38" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E38" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D38, settings!B$2:B$1048576, 0))</f>
@@ -10570,13 +10576,13 @@
         <v>97955</v>
       </c>
       <c r="B39" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C39" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D39" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E39" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D39, settings!B$2:B$1048576, 0))</f>
@@ -10588,13 +10594,13 @@
         <v>97998</v>
       </c>
       <c r="B40" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C40" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D40" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E40" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D40, settings!B$2:B$1048576, 0))</f>
@@ -10606,13 +10612,13 @@
         <v>97985</v>
       </c>
       <c r="B41" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C41" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D41" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E41" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D41, settings!B$2:B$1048576, 0))</f>
@@ -10642,7 +10648,7 @@
         <v>97967</v>
       </c>
       <c r="B43" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
@@ -10660,13 +10666,13 @@
         <v>97989</v>
       </c>
       <c r="B44" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C44" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D44" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E44" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D44, settings!B$2:B$1048576, 0))</f>
@@ -10714,7 +10720,7 @@
         <v>97965</v>
       </c>
       <c r="B47" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -10732,13 +10738,13 @@
         <v>99992</v>
       </c>
       <c r="B48" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C48" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D48" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E48" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D48, settings!B$2:B$1048576, 0))</f>
@@ -10768,7 +10774,7 @@
         <v>97970</v>
       </c>
       <c r="B50" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -10786,7 +10792,7 @@
         <v>97961</v>
       </c>
       <c r="B51" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>663</v>
@@ -10804,13 +10810,13 @@
         <v>97995</v>
       </c>
       <c r="B52" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C52" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D52" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E52" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D52, settings!B$2:B$1048576, 0))</f>
@@ -10840,13 +10846,13 @@
         <v>99970</v>
       </c>
       <c r="B54" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C54" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D54" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E54" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D54, settings!B$2:B$1048576, 0))</f>
@@ -10876,13 +10882,13 @@
         <v>100016</v>
       </c>
       <c r="B56" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C56" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D56" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E56" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D56, settings!B$2:B$1048576, 0))</f>
@@ -10894,13 +10900,13 @@
         <v>97982</v>
       </c>
       <c r="B57" t="s">
+        <v>757</v>
+      </c>
+      <c r="C57" t="s">
         <v>758</v>
       </c>
-      <c r="C57" t="s">
-        <v>759</v>
-      </c>
       <c r="D57" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E57" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D57, settings!B$2:B$1048576, 0))</f>
@@ -10912,13 +10918,13 @@
         <v>97963</v>
       </c>
       <c r="B58" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C58" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D58" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E58" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D58, settings!B$2:B$1048576, 0))</f>
@@ -10930,13 +10936,13 @@
         <v>100002</v>
       </c>
       <c r="B59" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C59" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D59" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E59" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D59, settings!B$2:B$1048576, 0))</f>
@@ -10948,13 +10954,13 @@
         <v>97975</v>
       </c>
       <c r="B60" t="s">
+        <v>728</v>
+      </c>
+      <c r="C60" t="s">
         <v>729</v>
       </c>
-      <c r="C60" t="s">
-        <v>730</v>
-      </c>
       <c r="D60" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E60" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D60, settings!B$2:B$1048576, 0))</f>
@@ -10966,7 +10972,7 @@
         <v>100011</v>
       </c>
       <c r="B61" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>32</v>
@@ -10984,7 +10990,7 @@
         <v>97981</v>
       </c>
       <c r="B62" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>32</v>
@@ -11020,7 +11026,7 @@
         <v>97951</v>
       </c>
       <c r="B64" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C64" t="s">
         <v>31</v>
@@ -11074,7 +11080,7 @@
         <v>97968</v>
       </c>
       <c r="B67" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
@@ -11092,13 +11098,13 @@
         <v>97996</v>
       </c>
       <c r="B68" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C68" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D68" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E68" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D68, settings!B$2:B$1048576, 0))</f>
@@ -11110,13 +11116,13 @@
         <v>100023</v>
       </c>
       <c r="B69" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C69" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D69" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E69" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D69, settings!B$2:B$1048576, 0))</f>
@@ -11128,13 +11134,13 @@
         <v>97980</v>
       </c>
       <c r="B70" t="s">
+        <v>787</v>
+      </c>
+      <c r="C70" t="s">
         <v>788</v>
       </c>
-      <c r="C70" t="s">
-        <v>789</v>
-      </c>
       <c r="D70" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E70" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D70, settings!B$2:B$1048576, 0))</f>
@@ -11146,13 +11152,13 @@
         <v>100004</v>
       </c>
       <c r="B71" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C71" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D71" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E71" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D71, settings!B$2:B$1048576, 0))</f>
@@ -11164,13 +11170,13 @@
         <v>100005</v>
       </c>
       <c r="B72" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C72" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D72" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E72" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D72, settings!B$2:B$1048576, 0))</f>
@@ -11182,13 +11188,13 @@
         <v>97977</v>
       </c>
       <c r="B73" t="s">
+        <v>760</v>
+      </c>
+      <c r="C73" t="s">
         <v>761</v>
       </c>
-      <c r="C73" t="s">
-        <v>762</v>
-      </c>
       <c r="D73" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E73" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D73, settings!B$2:B$1048576, 0))</f>
@@ -11200,13 +11206,13 @@
         <v>97960</v>
       </c>
       <c r="B74" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C74" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D74" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E74" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D74, settings!B$2:B$1048576, 0))</f>
@@ -11236,13 +11242,13 @@
         <v>99997</v>
       </c>
       <c r="B76" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C76" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D76" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E76" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D76, settings!B$2:B$1048576, 0))</f>
@@ -11254,13 +11260,13 @@
         <v>97964</v>
       </c>
       <c r="B77" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C77" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D77" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E77" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D77, settings!B$2:B$1048576, 0))</f>
@@ -11290,13 +11296,13 @@
         <v>100029</v>
       </c>
       <c r="B79" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C79" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D79" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E79" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D79, settings!B$2:B$1048576, 0))</f>
@@ -11326,13 +11332,13 @@
         <v>99986</v>
       </c>
       <c r="B81" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C81" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D81" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E81" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D81, settings!B$2:B$1048576, 0))</f>
@@ -11344,13 +11350,13 @@
         <v>99982</v>
       </c>
       <c r="B82" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C82" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D82" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E82" t="e">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D82, settings!B$2:B$1048576, 0))</f>
@@ -11362,13 +11368,13 @@
         <v>97974</v>
       </c>
       <c r="B83" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C83" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D83" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E83" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D83, settings!B$2:B$1048576, 0))</f>
@@ -11380,13 +11386,13 @@
         <v>99980</v>
       </c>
       <c r="B84" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C84" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D84" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E84" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D84, settings!B$2:B$1048576, 0))</f>
@@ -11434,7 +11440,7 @@
         <v>97978</v>
       </c>
       <c r="B87" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
@@ -11452,13 +11458,13 @@
         <v>100008</v>
       </c>
       <c r="B88" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C88" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D88" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E88" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D88, settings!B$2:B$1048576, 0))</f>
@@ -11470,13 +11476,13 @@
         <v>97969</v>
       </c>
       <c r="B89" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C89" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D89" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E89" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D89, settings!B$2:B$1048576, 0))</f>
@@ -11506,7 +11512,7 @@
         <v>97957</v>
       </c>
       <c r="B91" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C91" t="s">
         <v>151</v>
@@ -11542,13 +11548,13 @@
         <v>99984</v>
       </c>
       <c r="B93" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C93" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D93" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E93" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D93, settings!B$2:B$1048576, 0))</f>
@@ -11578,7 +11584,7 @@
         <v>97973</v>
       </c>
       <c r="B95" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -11629,13 +11635,13 @@
         <v>191</v>
       </c>
       <c r="D1" t="s">
+        <v>850</v>
+      </c>
+      <c r="E1" t="s">
+        <v>678</v>
+      </c>
+      <c r="F1" t="s">
         <v>851</v>
-      </c>
-      <c r="E1" t="s">
-        <v>679</v>
-      </c>
-      <c r="F1" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -11650,13 +11656,13 @@
         <v>195</v>
       </c>
       <c r="D2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -11671,13 +11677,13 @@
         <v>194</v>
       </c>
       <c r="D3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="J3"/>
     </row>
@@ -11693,13 +11699,13 @@
         <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F4" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -11714,13 +11720,13 @@
         <v>633</v>
       </c>
       <c r="D5" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F5" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -11729,19 +11735,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D6" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -11750,19 +11756,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C7" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D7" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F7" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -11771,19 +11777,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C8" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D8" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F8" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -11792,19 +11798,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C9" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E9" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F9" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -11813,19 +11819,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D10" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E10" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F10" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -11834,19 +11840,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C11" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D11" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -11855,16 +11861,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E12" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F12" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -11873,16 +11879,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C13" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E13" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F13" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -11891,16 +11897,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E14" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F14" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -11909,16 +11915,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C15" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E15" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F15" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -11927,16 +11933,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E16" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F16" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -11945,16 +11951,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C17" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E17" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -11963,16 +11969,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C18" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E18" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F18" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -11981,16 +11987,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E19" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F19" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -11999,16 +12005,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C20" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E20" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -12017,16 +12023,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C21" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E21" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F21" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -12035,16 +12041,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E22" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F22" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -12053,16 +12059,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C23" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E23" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F23" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -12071,16 +12077,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C24" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E24" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F24" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -12089,16 +12095,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E25" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F25" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -12107,16 +12113,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C26" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E26" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F26" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -12125,16 +12131,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E27" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F27" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -12143,16 +12149,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>683</v>
+      </c>
+      <c r="C28" t="s">
         <v>684</v>
       </c>
-      <c r="C28" t="s">
-        <v>685</v>
-      </c>
       <c r="E28" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F28" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -12161,16 +12167,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C29" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E29" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F29" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -12179,16 +12185,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C30" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E30" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F30" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -12197,16 +12203,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C31" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E31" t="s">
+        <v>855</v>
+      </c>
+      <c r="F31" t="s">
         <v>856</v>
-      </c>
-      <c r="F31" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -12221,10 +12227,10 @@
         <v>201</v>
       </c>
       <c r="E32" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F32" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -12239,10 +12245,10 @@
         <v>202</v>
       </c>
       <c r="E33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F33" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -12257,10 +12263,10 @@
         <v>200</v>
       </c>
       <c r="E34" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F34" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -12275,10 +12281,10 @@
         <v>196</v>
       </c>
       <c r="E35" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F35" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -12293,10 +12299,10 @@
         <v>198</v>
       </c>
       <c r="E36" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F36" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -12311,10 +12317,10 @@
         <v>634</v>
       </c>
       <c r="E37" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F37" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -12323,16 +12329,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>681</v>
+      </c>
+      <c r="C38" t="s">
         <v>682</v>
       </c>
-      <c r="C38" t="s">
-        <v>683</v>
-      </c>
       <c r="E38" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F38" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -12341,16 +12347,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C39" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E39" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F39" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -12359,16 +12365,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C40" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E40" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="F40" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -12377,16 +12383,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C41" t="s">
+        <v>724</v>
+      </c>
+      <c r="E41" t="s">
         <v>725</v>
       </c>
-      <c r="E41" t="s">
-        <v>726</v>
-      </c>
       <c r="F41" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -12395,16 +12401,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C42" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E42" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F42" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
   </sheetData>
@@ -12601,18 +12607,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
FIX BUG: Add one setting parameter to denote whether the task needs response for each trial.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\CCDPro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CCDPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,35 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张亮:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Response required:
+TRUE = every trial needs a response.
+FALSE = not every trial needs a response.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="886">
   <si>
     <t>符号判断</t>
   </si>
@@ -3494,6 +3522,10 @@
   </si>
   <si>
     <t>H1 R1 H2 R2 Delay Resp RT CurUtility TotalUtility\X1 X2 Delay H1 R1 H2 R2 Resp RT CurUtility TotalUtility</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RespRequired</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4175,13 +4207,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X55"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomRight" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4194,22 +4226,22 @@
     <col min="6" max="6" width="15" style="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="4" customWidth="1"/>
     <col min="8" max="8" width="12.73046875" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.73046875" customWidth="1"/>
-    <col min="12" max="12" width="15" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.265625" customWidth="1"/>
-    <col min="14" max="14" width="14.73046875" customWidth="1"/>
-    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.73046875" customWidth="1"/>
-    <col min="17" max="17" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" style="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.46484375" style="21" customWidth="1"/>
-    <col min="20" max="20" width="57.1328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12.73046875" customWidth="1"/>
+    <col min="13" max="13" width="15" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.265625" customWidth="1"/>
+    <col min="15" max="15" width="14.73046875" customWidth="1"/>
+    <col min="16" max="16" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.73046875" customWidth="1"/>
+    <col min="18" max="18" width="10.46484375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.46484375" style="21" customWidth="1"/>
+    <col min="21" max="21" width="57.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -4237,53 +4269,56 @@
       <c r="I1" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>576</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <f t="shared" ref="A2:A33" si="0">ROW() - 1</f>
         <v>1</v>
@@ -4308,41 +4343,44 @@
       <c r="I2" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K2" s="5"/>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="2"/>
+      <c r="P2" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="24" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="T2" s="21" t="s">
         <v>588</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>600</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>4</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4367,42 +4405,45 @@
       <c r="I3" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
         <v>1000</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="2"/>
+      <c r="P3" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="24" t="s">
+      <c r="Q3" s="19"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="24" t="s">
         <v>643</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="T3" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>4</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4427,41 +4468,44 @@
       <c r="I4" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
         <v>500</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="10"/>
+      <c r="P4" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="R4" s="25" t="s">
+      <c r="Q4" s="10"/>
+      <c r="S4" s="25" t="s">
         <v>580</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="T4" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>4</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4486,49 +4530,52 @@
       <c r="I5" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
         <v>1000</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>0.5</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="M5" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2" t="s">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P5" s="19"/>
-      <c r="Q5" t="s">
+      <c r="Q5" s="19"/>
+      <c r="R5" t="s">
         <v>498</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="S5" s="26" t="s">
         <v>629</v>
       </c>
-      <c r="S5" s="22" t="s">
+      <c r="T5" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="U5" s="17" t="s">
         <v>615</v>
       </c>
-      <c r="U5" s="17" t="s">
+      <c r="V5" s="17" t="s">
         <v>616</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>4</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4553,49 +4600,52 @@
       <c r="I6" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
         <v>1000</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>0.5</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="M6" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2" t="s">
+      <c r="O6" s="2"/>
+      <c r="P6" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" t="s">
+      <c r="Q6" s="19"/>
+      <c r="R6" t="s">
         <v>498</v>
       </c>
-      <c r="R6" s="26" t="s">
+      <c r="S6" s="26" t="s">
         <v>629</v>
       </c>
-      <c r="S6" s="22" t="s">
+      <c r="T6" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="T6" s="17" t="s">
+      <c r="U6" s="17" t="s">
         <v>615</v>
       </c>
-      <c r="U6" s="17" t="s">
+      <c r="V6" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>4</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4620,51 +4670,54 @@
       <c r="I7" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10">
         <v>2000</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>0.5</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="M7" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="P7" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="P7" s="18" t="s">
+      <c r="Q7" s="18" t="s">
         <v>655</v>
       </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="5"/>
+      <c r="S7" s="23" t="s">
         <v>656</v>
       </c>
-      <c r="S7" s="22" t="s">
+      <c r="T7" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>639</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>3000</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="W7">
-        <v>2</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4689,44 +4742,47 @@
       <c r="I8" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
         <v>2000</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>0.5</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="M8" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2" t="s">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P8" s="19"/>
-      <c r="R8" s="26" t="s">
+      <c r="Q8" s="19"/>
+      <c r="S8" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="S8" s="22" t="s">
+      <c r="T8" s="22" t="s">
         <v>591</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="U8" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="U8" s="17"/>
-      <c r="V8" s="2" t="s">
+      <c r="V8" s="17"/>
+      <c r="W8" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>5</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4751,44 +4807,47 @@
       <c r="I9" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
         <v>0.5</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="M9" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P9" s="19"/>
-      <c r="R9" s="26" t="s">
+      <c r="Q9" s="19"/>
+      <c r="S9" s="26" t="s">
         <v>580</v>
       </c>
-      <c r="S9" s="22" t="s">
+      <c r="T9" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="U9" s="5" t="s">
         <v>613</v>
       </c>
-      <c r="U9" s="17"/>
-      <c r="V9" s="2" t="s">
+      <c r="V9" s="17"/>
+      <c r="W9" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>5</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4813,50 +4872,53 @@
       <c r="I10" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
         <v>3000</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>0.5</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="M10" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>657</v>
       </c>
-      <c r="R10" s="24" t="s">
+      <c r="S10" s="24" t="s">
         <v>655</v>
       </c>
-      <c r="S10" s="22" t="s">
+      <c r="T10" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>639</v>
       </c>
-      <c r="U10" s="17">
+      <c r="V10" s="17">
         <v>2000</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>5</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4881,51 +4943,54 @@
       <c r="I11" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
         <v>3000</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>0.25</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="M11" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>657</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39" t="s">
+      <c r="R11" s="39"/>
+      <c r="S11" s="39" t="s">
         <v>655</v>
       </c>
-      <c r="S11" s="22" t="s">
+      <c r="T11" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>639</v>
       </c>
-      <c r="U11" s="17">
+      <c r="V11" s="17">
         <v>3000</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="W11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>5</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4950,49 +5015,52 @@
       <c r="I12" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2">
+      <c r="J12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2">
         <v>0.25</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="M12" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>657</v>
       </c>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39" t="s">
+      <c r="R12" s="39"/>
+      <c r="S12" s="39" t="s">
         <v>655</v>
       </c>
-      <c r="S12" s="22" t="s">
+      <c r="T12" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>639</v>
       </c>
-      <c r="U12" s="17">
+      <c r="V12" s="17">
         <v>3000</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="W12" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>5</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5017,45 +5085,48 @@
       <c r="I13" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
         <v>2000</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>0.5</v>
       </c>
-      <c r="L13" s="20" t="s">
+      <c r="M13" s="20" t="s">
         <v>570</v>
       </c>
-      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" t="s">
+      <c r="P13" s="2"/>
+      <c r="Q13" t="s">
         <v>882</v>
       </c>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="4" t="s">
+      <c r="R13" s="39"/>
+      <c r="S13" s="4" t="s">
         <v>883</v>
       </c>
-      <c r="S13" s="22" t="s">
+      <c r="T13" s="22" t="s">
         <v>590</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>607</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>618</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="W13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>5</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5080,45 +5151,48 @@
       <c r="I14" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
         <v>2000</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>0.5</v>
       </c>
-      <c r="L14" s="20" t="s">
+      <c r="M14" s="20" t="s">
         <v>571</v>
       </c>
-      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" t="s">
+      <c r="P14" s="2"/>
+      <c r="Q14" t="s">
         <v>882</v>
       </c>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="4" t="s">
+      <c r="R14" s="39"/>
+      <c r="S14" s="4" t="s">
         <v>883</v>
       </c>
-      <c r="S14" s="22" t="s">
+      <c r="T14" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>607</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>618</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>5</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5142,27 +5216,30 @@
       <c r="I15" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>1000</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.5</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>876</v>
       </c>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="5" t="s">
+      <c r="R15" s="39"/>
+      <c r="S15" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>5</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5187,45 +5264,48 @@
       <c r="I16" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7">
         <v>3000</v>
       </c>
-      <c r="K16" s="8">
+      <c r="L16" s="8">
         <v>0.5</v>
       </c>
-      <c r="L16" s="27" t="s">
+      <c r="M16" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-      <c r="P16" t="s">
+      <c r="P16" s="8"/>
+      <c r="Q16" t="s">
         <v>524</v>
       </c>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="39"/>
+      <c r="S16" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="S16" s="21" t="s">
+      <c r="T16" s="21" t="s">
         <v>586</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>601</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>597</v>
       </c>
-      <c r="V16" s="8" t="s">
+      <c r="W16" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="W16">
-        <v>2</v>
-      </c>
-      <c r="X16" t="s">
+      <c r="X16">
+        <v>2</v>
+      </c>
+      <c r="Y16" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5250,45 +5330,48 @@
       <c r="I17" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="7">
         <v>3000</v>
       </c>
-      <c r="K17" s="8">
+      <c r="L17" s="8">
         <v>0.5</v>
       </c>
-      <c r="L17" s="27" t="s">
+      <c r="M17" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-      <c r="P17" t="s">
+      <c r="P17" s="8"/>
+      <c r="Q17" t="s">
         <v>524</v>
       </c>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="4" t="s">
+      <c r="R17" s="39"/>
+      <c r="S17" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="S17" s="21" t="s">
+      <c r="T17" s="21" t="s">
         <v>586</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>601</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>597</v>
       </c>
-      <c r="V17" s="8" t="s">
+      <c r="W17" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="W17">
-        <v>2</v>
-      </c>
-      <c r="X17" t="s">
+      <c r="X17">
+        <v>2</v>
+      </c>
+      <c r="Y17" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5313,47 +5396,50 @@
       <c r="I18" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="8">
         <v>2000</v>
       </c>
-      <c r="K18" s="8">
+      <c r="L18" s="8">
         <v>0.5</v>
       </c>
-      <c r="L18" s="27" t="s">
+      <c r="M18" s="27" t="s">
         <v>603</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="N18" s="8" t="s">
         <v>602</v>
       </c>
-      <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="8" t="s">
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8" t="s">
         <v>880</v>
       </c>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="39"/>
+      <c r="S18" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="S18" s="21" t="s">
+      <c r="T18" s="21" t="s">
         <v>586</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>604</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>597</v>
       </c>
-      <c r="V18" s="8" t="s">
+      <c r="W18" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="W18">
-        <v>2</v>
-      </c>
-      <c r="X18" t="s">
+      <c r="X18">
+        <v>2</v>
+      </c>
+      <c r="Y18" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5378,42 +5464,45 @@
       <c r="I19" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8">
         <v>3000</v>
       </c>
-      <c r="K19" s="8">
+      <c r="L19" s="8">
         <v>0.5</v>
       </c>
-      <c r="L19" s="27" t="s">
+      <c r="M19" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="N19" s="8" t="s">
         <v>606</v>
       </c>
-      <c r="N19" s="8"/>
       <c r="O19" s="8"/>
-      <c r="Q19" s="39"/>
+      <c r="P19" s="8"/>
       <c r="R19" s="39"/>
-      <c r="S19" s="21" t="s">
+      <c r="S19" s="39"/>
+      <c r="T19" s="21" t="s">
         <v>586</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>605</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>598</v>
       </c>
-      <c r="V19" s="8" t="s">
+      <c r="W19" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="W19">
-        <v>2</v>
-      </c>
-      <c r="X19" t="s">
+      <c r="X19">
+        <v>2</v>
+      </c>
+      <c r="Y19" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5438,38 +5527,41 @@
       <c r="I20" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="J20" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="28" t="s">
+      <c r="L20" s="5"/>
+      <c r="M20" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39" t="s">
+      <c r="P20" s="2"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39" t="s">
         <v>582</v>
       </c>
-      <c r="S20" s="22" t="s">
+      <c r="T20" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="T20" s="5" t="s">
+      <c r="U20" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="U20" s="17">
+      <c r="V20" s="17">
         <v>400</v>
       </c>
-      <c r="V20" s="2" t="s">
+      <c r="W20" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>6</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5494,37 +5586,40 @@
       <c r="I21" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="J21" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K21" s="5"/>
-      <c r="L21" s="28" t="s">
+      <c r="L21" s="5"/>
+      <c r="M21" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="R21" s="24" t="s">
+      <c r="P21" s="2"/>
+      <c r="S21" s="24" t="s">
         <v>583</v>
       </c>
-      <c r="S21" s="22" t="s">
+      <c r="T21" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="T21" s="5" t="s">
+      <c r="U21" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="U21" s="17">
+      <c r="V21" s="17">
         <v>500</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="W21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>6</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5549,37 +5644,40 @@
       <c r="I22" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J22" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K22" s="5"/>
-      <c r="L22" s="28" t="s">
+      <c r="L22" s="5"/>
+      <c r="M22" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="R22" s="24" t="s">
+      <c r="P22" s="2"/>
+      <c r="S22" s="24" t="s">
         <v>584</v>
       </c>
-      <c r="S22" s="22" t="s">
+      <c r="T22" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="T22" s="5" t="s">
+      <c r="U22" s="5" t="s">
         <v>620</v>
       </c>
-      <c r="U22" s="17">
+      <c r="V22" s="17">
         <v>600</v>
       </c>
-      <c r="V22" s="2" t="s">
+      <c r="W22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>6</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5604,46 +5702,49 @@
       <c r="I23" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
         <v>2000</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>0.25</v>
       </c>
-      <c r="L23" s="20" t="s">
+      <c r="M23" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" t="s">
+      <c r="P23" s="2"/>
+      <c r="Q23" t="s">
         <v>882</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>882</v>
       </c>
-      <c r="S23" s="22" t="s">
+      <c r="T23" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="T23" s="17" t="s">
+      <c r="U23" s="17" t="s">
         <v>621</v>
       </c>
-      <c r="U23" s="17" t="s">
+      <c r="V23" s="17" t="s">
         <v>622</v>
       </c>
-      <c r="V23" s="2" t="s">
+      <c r="W23" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>6</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5668,48 +5769,51 @@
       <c r="I24" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
         <v>2000</v>
       </c>
-      <c r="K24" s="2">
+      <c r="L24" s="2">
         <v>0.5</v>
       </c>
-      <c r="L24" s="28" t="s">
+      <c r="M24" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="5" t="s">
+      <c r="O24" s="2"/>
+      <c r="P24" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="P24" s="5" t="s">
+      <c r="Q24" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="R24" s="24" t="s">
+      <c r="S24" s="24" t="s">
         <v>644</v>
       </c>
-      <c r="S24" s="22" t="s">
+      <c r="T24" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="T24" s="17" t="s">
+      <c r="U24" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="U24" s="17" t="s">
+      <c r="V24" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="W24" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>6</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5734,48 +5838,51 @@
       <c r="I25" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
         <v>2000</v>
       </c>
-      <c r="K25" s="2">
+      <c r="L25" s="2">
         <v>0.5</v>
       </c>
-      <c r="L25" s="28" t="s">
+      <c r="M25" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="N25" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="N25" s="2"/>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="2"/>
+      <c r="P25" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="P25" s="5" t="s">
+      <c r="Q25" s="5" t="s">
         <v>647</v>
       </c>
-      <c r="R25" s="24" t="s">
+      <c r="S25" s="24" t="s">
         <v>645</v>
       </c>
-      <c r="S25" s="22" t="s">
+      <c r="T25" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="T25" s="17" t="s">
+      <c r="U25" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="U25" s="17" t="s">
+      <c r="V25" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="V25" s="2" t="s">
+      <c r="W25" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>6</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5800,48 +5907,51 @@
       <c r="I26" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
         <v>2000</v>
       </c>
-      <c r="K26" s="2">
+      <c r="L26" s="2">
         <v>0.5</v>
       </c>
-      <c r="L26" s="28" t="s">
+      <c r="M26" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="5" t="s">
+      <c r="O26" s="2"/>
+      <c r="P26" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="P26" s="5" t="s">
+      <c r="Q26" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="S26" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="S26" s="22" t="s">
+      <c r="T26" s="22" t="s">
         <v>595</v>
       </c>
-      <c r="T26" s="17" t="s">
+      <c r="U26" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="U26" s="17" t="s">
+      <c r="V26" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="V26" s="2" t="s">
+      <c r="W26" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>6</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5866,43 +5976,46 @@
       <c r="I27" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
         <v>2000</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
         <v>0.5</v>
       </c>
-      <c r="L27" s="20" t="s">
+      <c r="M27" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2" t="s">
+      <c r="O27" s="2"/>
+      <c r="P27" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="S27" s="22"/>
-      <c r="T27" s="17" t="s">
+      <c r="T27" s="22"/>
+      <c r="U27" s="17" t="s">
         <v>621</v>
       </c>
-      <c r="U27" s="17" t="s">
+      <c r="V27" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="V27" s="2" t="s">
+      <c r="W27" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>6</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5929,43 +6042,46 @@
       <c r="I28" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2">
+      <c r="J28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2">
         <v>0.5</v>
       </c>
-      <c r="L28" s="20" t="s">
+      <c r="M28" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2" t="s">
+      <c r="O28" s="2"/>
+      <c r="P28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P28" s="2" t="s">
+      <c r="Q28" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="R28" s="4" t="s">
+      <c r="S28" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="S28" s="21" t="s">
+      <c r="T28" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>600</v>
       </c>
-      <c r="V28" s="2" t="s">
+      <c r="W28" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W28">
-        <v>1</v>
-      </c>
-      <c r="X28" t="s">
+      <c r="X28">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5992,43 +6108,46 @@
       <c r="I29" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2">
+      <c r="J29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2">
         <v>0.5</v>
       </c>
-      <c r="L29" s="20" t="s">
+      <c r="M29" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2" t="s">
+      <c r="O29" s="2"/>
+      <c r="P29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P29" s="2" t="s">
+      <c r="Q29" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="R29" s="4" t="s">
+      <c r="S29" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="S29" s="21" t="s">
+      <c r="T29" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>600</v>
       </c>
-      <c r="V29" s="2" t="s">
+      <c r="W29" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W29">
-        <v>1</v>
-      </c>
-      <c r="X29" t="s">
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6055,43 +6174,46 @@
       <c r="I30" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2">
+      <c r="J30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2">
         <v>0.5</v>
       </c>
-      <c r="L30" s="20" t="s">
+      <c r="M30" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2" t="s">
+      <c r="O30" s="2"/>
+      <c r="P30" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P30" s="2" t="s">
+      <c r="Q30" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="R30" s="4" t="s">
+      <c r="S30" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="S30" s="21" t="s">
+      <c r="T30" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>600</v>
       </c>
-      <c r="V30" s="2" t="s">
+      <c r="W30" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W30">
-        <v>1</v>
-      </c>
-      <c r="X30" t="s">
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6118,43 +6240,46 @@
       <c r="I31" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2">
+      <c r="J31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2">
         <v>0.5</v>
       </c>
-      <c r="L31" s="20" t="s">
+      <c r="M31" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2" t="s">
+      <c r="O31" s="2"/>
+      <c r="P31" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P31" s="2" t="s">
+      <c r="Q31" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="R31" s="24" t="s">
+      <c r="S31" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="S31" s="21" t="s">
+      <c r="T31" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>600</v>
       </c>
-      <c r="V31" s="2" t="s">
+      <c r="W31" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W31">
-        <v>1</v>
-      </c>
-      <c r="X31" t="s">
+      <c r="X31">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -6181,43 +6306,46 @@
       <c r="I32" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2">
+      <c r="J32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2">
         <v>0.5</v>
       </c>
-      <c r="L32" s="20" t="s">
+      <c r="M32" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2" t="s">
+      <c r="O32" s="2"/>
+      <c r="P32" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P32" s="2" t="s">
+      <c r="Q32" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="R32" s="24" t="s">
+      <c r="S32" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="S32" s="21" t="s">
+      <c r="T32" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>600</v>
       </c>
-      <c r="V32" s="2" t="s">
+      <c r="W32" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W32">
-        <v>1</v>
-      </c>
-      <c r="X32" t="s">
+      <c r="X32">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -6244,43 +6372,46 @@
       <c r="I33" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2">
+      <c r="J33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2">
         <v>0.5</v>
       </c>
-      <c r="L33" s="20" t="s">
+      <c r="M33" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2" t="s">
+      <c r="O33" s="2"/>
+      <c r="P33" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P33" s="2" t="s">
+      <c r="Q33" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="R33" s="24" t="s">
+      <c r="S33" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="S33" s="21" t="s">
+      <c r="T33" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>600</v>
       </c>
-      <c r="V33" s="2" t="s">
+      <c r="W33" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W33">
-        <v>1</v>
-      </c>
-      <c r="X33" t="s">
+      <c r="X33">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" ref="A34:A55" si="1">ROW() - 1</f>
         <v>33</v>
@@ -6303,29 +6434,32 @@
       <c r="I34" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="J34" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K34" s="5"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="2"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="20"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" t="s">
+      <c r="P34" s="2"/>
+      <c r="Q34" t="s">
         <v>578</v>
       </c>
-      <c r="R34" s="24" t="s">
+      <c r="S34" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="V34" s="2" t="s">
+      <c r="W34" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="W34">
-        <v>1</v>
-      </c>
-      <c r="X34" t="s">
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="Y34" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -6350,45 +6484,48 @@
       <c r="I35" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" s="2">
         <v>3000</v>
       </c>
-      <c r="K35" s="2"/>
-      <c r="L35" s="20" t="s">
+      <c r="L35" s="2"/>
+      <c r="M35" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2" t="s">
+      <c r="N35" s="2"/>
+      <c r="O35" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="O35" s="2"/>
-      <c r="P35" s="17" t="s">
+      <c r="P35" s="2"/>
+      <c r="Q35" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="26" t="s">
+      <c r="R35" s="4"/>
+      <c r="S35" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="S35" s="21" t="s">
+      <c r="T35" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>607</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>608</v>
       </c>
-      <c r="V35" s="2" t="s">
+      <c r="W35" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>3</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -6413,49 +6550,52 @@
       <c r="I36" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
         <v>3000</v>
       </c>
-      <c r="K36" s="2">
+      <c r="L36" s="2">
         <v>0.5</v>
       </c>
-      <c r="L36" s="20" t="s">
+      <c r="M36" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2" t="s">
+      <c r="O36" s="2"/>
+      <c r="P36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="P36" s="17" t="s">
+      <c r="Q36" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="26" t="s">
+      <c r="R36" s="4"/>
+      <c r="S36" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="S36" s="21" t="s">
+      <c r="T36" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="T36" s="31" t="s">
+      <c r="U36" s="31" t="s">
         <v>612</v>
       </c>
-      <c r="U36" s="32" t="s">
+      <c r="V36" s="32" t="s">
         <v>609</v>
       </c>
-      <c r="V36" s="2" t="s">
+      <c r="W36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="W36">
+      <c r="X36">
         <v>3</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -6480,49 +6620,52 @@
       <c r="I37" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" s="2">
         <v>3000</v>
       </c>
-      <c r="K37" s="2">
+      <c r="L37" s="2">
         <v>0.5</v>
       </c>
-      <c r="L37" s="20" t="s">
+      <c r="M37" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2" t="s">
+      <c r="N37" s="2"/>
+      <c r="O37" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="P37" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="P37" s="17" t="s">
+      <c r="Q37" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="26" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="S37" s="21" t="s">
+      <c r="T37" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>607</v>
       </c>
-      <c r="U37" t="s">
+      <c r="V37" t="s">
         <v>610</v>
       </c>
-      <c r="V37" s="2" t="s">
+      <c r="W37" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="W37">
+      <c r="X37">
         <v>3</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -6547,45 +6690,48 @@
       <c r="I38" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" s="2">
         <v>3000</v>
       </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="20" t="s">
+      <c r="L38" s="2"/>
+      <c r="M38" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2" t="s">
+      <c r="N38" s="2"/>
+      <c r="O38" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="O38" s="2"/>
-      <c r="P38" s="17" t="s">
+      <c r="P38" s="2"/>
+      <c r="Q38" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="26" t="s">
+      <c r="R38" s="4"/>
+      <c r="S38" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="S38" s="21" t="s">
+      <c r="T38" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
         <v>607</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>611</v>
       </c>
-      <c r="V38" s="2" t="s">
+      <c r="W38" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="W38">
+      <c r="X38">
         <v>3</v>
       </c>
-      <c r="X38" t="s">
+      <c r="Y38" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -6610,45 +6756,48 @@
       <c r="I39" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" s="2">
         <v>1000</v>
       </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="20" t="s">
+      <c r="L39" s="2"/>
+      <c r="M39" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2" t="s">
+      <c r="N39" s="2"/>
+      <c r="O39" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="O39" s="2"/>
-      <c r="P39" s="17" t="s">
+      <c r="P39" s="2"/>
+      <c r="Q39" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="26" t="s">
+      <c r="R39" s="4"/>
+      <c r="S39" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="S39" s="21" t="s">
+      <c r="T39" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>607</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>597</v>
       </c>
-      <c r="V39" s="2" t="s">
+      <c r="W39" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="W39">
+      <c r="X39">
         <v>3</v>
       </c>
-      <c r="X39" t="s">
+      <c r="Y39" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -6673,45 +6822,48 @@
       <c r="I40" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" s="2">
         <v>3000</v>
       </c>
-      <c r="K40" s="2">
+      <c r="L40" s="2">
         <v>0.5</v>
       </c>
-      <c r="L40" s="28" t="s">
+      <c r="M40" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="O40" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="O40" s="5" t="s">
+      <c r="P40" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>657</v>
       </c>
-      <c r="R40" s="24" t="s">
+      <c r="S40" s="24" t="s">
         <v>655</v>
       </c>
-      <c r="S40" s="22"/>
-      <c r="U40" s="17">
+      <c r="T40" s="22"/>
+      <c r="V40" s="17">
         <v>3000</v>
       </c>
-      <c r="V40" s="2" t="s">
+      <c r="W40" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="W40">
+      <c r="X40">
         <v>5</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -6736,45 +6888,48 @@
       <c r="I41" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" s="2">
         <v>3000</v>
       </c>
-      <c r="K41" s="2">
+      <c r="L41" s="2">
         <v>0.5</v>
       </c>
-      <c r="L41" s="28" t="s">
+      <c r="M41" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="N41" s="5" t="s">
+      <c r="O41" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="O41" s="5" t="s">
+      <c r="P41" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>657</v>
       </c>
-      <c r="R41" s="24" t="s">
+      <c r="S41" s="24" t="s">
         <v>655</v>
       </c>
-      <c r="S41" s="22"/>
-      <c r="U41" s="17">
+      <c r="T41" s="22"/>
+      <c r="V41" s="17">
         <v>3000</v>
       </c>
-      <c r="V41" s="2" t="s">
+      <c r="W41" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="W41">
+      <c r="X41">
         <v>5</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -6797,15 +6952,18 @@
       <c r="I42" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J42" s="2"/>
+      <c r="J42" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K42" s="2"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="20"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="V42" s="2"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P42" s="2"/>
+      <c r="W42" s="2"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -6828,16 +6986,19 @@
       <c r="I43" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J43" s="2"/>
+      <c r="J43" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K43" s="2"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="20"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-      <c r="R43" s="21"/>
-      <c r="V43" s="2"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P43" s="2"/>
+      <c r="S43" s="21"/>
+      <c r="W43" s="2"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -6860,22 +7021,25 @@
       <c r="I44" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="J44" s="2"/>
+      <c r="J44" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K44" s="2"/>
-      <c r="L44" s="20" t="s">
+      <c r="L44" s="2"/>
+      <c r="M44" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="R44" s="23" t="s">
+      <c r="P44" s="2"/>
+      <c r="S44" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="V44" s="2" t="s">
+      <c r="W44" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -6896,13 +7060,14 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="20"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-      <c r="V45" s="2"/>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P45" s="2"/>
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -6923,13 +7088,14 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="20"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-      <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="P46" s="2"/>
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -6947,7 +7113,7 @@
       </c>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -9149,7 +9315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
UPDATE FUNCTIONS: newer calculation of digit comparison task. New calculation; better handle displaying when merging.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="898">
   <si>
     <t>符号判断</t>
   </si>
@@ -3526,6 +3526,54 @@
   </si>
   <si>
     <t>RespRequired</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十四</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>十五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4209,7 +4257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12852,10 +12900,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -12946,122 +12994,170 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>521</v>
+      <c r="A12" t="s">
+        <v>886</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>521</v>
+        <v>888</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>522</v>
+      <c r="A13" t="s">
+        <v>887</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>522</v>
+        <v>889</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>434</v>
+      <c r="A14" t="s">
+        <v>890</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>434</v>
+        <v>891</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>435</v>
+      <c r="A15" t="s">
+        <v>892</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>435</v>
+        <v>893</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>436</v>
+      <c r="A16" t="s">
+        <v>894</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>436</v>
+        <v>895</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>437</v>
+      <c r="A17" t="s">
+        <v>896</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>437</v>
+        <v>897</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>438</v>
+        <v>521</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>438</v>
+        <v>521</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>439</v>
+        <v>522</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>439</v>
+        <v>522</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>446</v>
       </c>
     </row>

</xml_diff>

<commit_message>
POLISH: Better handle accuracy rate for stop signal task.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9338"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="899">
   <si>
     <t>符号判断</t>
   </si>
@@ -3574,6 +3574,10 @@
   </si>
   <si>
     <t>15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4257,11 +4261,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H44" sqref="H44"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5272,6 +5276,9 @@
       </c>
       <c r="L15">
         <v>0.5</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>898</v>
       </c>
       <c r="Q15" t="s">
         <v>876</v>
@@ -12902,7 +12909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FIX BUG: Changed variable name to avoid name masking.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -3357,11 +3357,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>filt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>filt</t>
+    <t>filtcap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filtcap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3960,10 +3960,10 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -6080,7 +6080,7 @@
         <v>483</v>
       </c>
       <c r="Q48" s="16" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -6116,7 +6116,7 @@
         <v>483</v>
       </c>
       <c r="Q49" s="16" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FIX BUG: better treating no response trials. There are sometimes trials without any response in Filtering task and the 'Resp' records this as -1. Take advantage of this.
</commit_message>
<xml_diff>
--- a/taskSettings.xlsx
+++ b/taskSettings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9336" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="838">
   <si>
     <t>符号判断</t>
   </si>
@@ -2965,46 +2965,6 @@
   </si>
   <si>
     <t>CQ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DongZB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BeiF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShiL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HuaiB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DongJMX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LiuLHZX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DouDZX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HuiWDY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>QingHFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShouDYK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3959,11 +3919,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
+      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3995,7 +3955,7 @@
         <v>143</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>755</v>
+        <v>745</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>27</v>
@@ -4004,13 +3964,13 @@
         <v>489</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>768</v>
+        <v>758</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>488</v>
@@ -4025,7 +3985,7 @@
         <v>472</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>470</v>
@@ -4063,11 +4023,11 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="19" t="s">
-        <v>833</v>
+        <v>823</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="16" t="s">
@@ -4113,7 +4073,7 @@
         <v>153</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="16" t="s">
@@ -4159,7 +4119,7 @@
         <v>469</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="Q4" s="36" t="s">
         <v>537</v>
@@ -4206,7 +4166,7 @@
         <v>153</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="P5" t="s">
         <v>471</v>
@@ -4256,7 +4216,7 @@
         <v>153</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="P6" t="s">
         <v>471</v>
@@ -4306,7 +4266,7 @@
         <v>153</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="Q7" s="17" t="s">
         <v>537</v>
@@ -4353,7 +4313,7 @@
         <v>166</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="Q8" s="17" t="s">
         <v>537</v>
@@ -4375,7 +4335,7 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>490</v>
@@ -4418,7 +4378,7 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>490</v>
@@ -4462,7 +4422,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>490</v>
@@ -4506,7 +4466,7 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>490</v>
@@ -4548,7 +4508,7 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="19" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>490</v>
@@ -4571,11 +4531,11 @@
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="16" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -4594,7 +4554,7 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="21" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>490</v>
@@ -4617,11 +4577,11 @@
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="16" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -4640,10 +4600,10 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="16" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
       <c r="H15" s="5" t="b">
         <v>0</v>
@@ -4659,11 +4619,11 @@
         <v>0.5</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="15" t="s">
-        <v>761</v>
+        <v>751</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4682,7 +4642,7 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="20" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>490</v>
@@ -4730,7 +4690,7 @@
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="18" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>490</v>
@@ -4803,11 +4763,11 @@
         <v>542</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="15" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -4930,7 +4890,7 @@
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="Q21" s="16" t="s">
         <v>540</v>
@@ -4981,17 +4941,17 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>794</v>
+        <v>784</v>
       </c>
       <c r="C23" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>580</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="16" t="s">
-        <v>798</v>
+        <v>788</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>490</v>
@@ -5002,10 +4962,10 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="O23" s="2" t="s">
-        <v>831</v>
+        <v>821</v>
       </c>
       <c r="Q23" s="16" t="s">
-        <v>799</v>
+        <v>789</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -5049,10 +5009,10 @@
         <v>161</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -5096,7 +5056,7 @@
         <v>555</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="Q25" s="16" t="s">
         <v>553</v>
@@ -5143,7 +5103,7 @@
         <v>556</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="Q26" s="16" t="s">
         <v>554</v>
@@ -5190,7 +5150,7 @@
         <v>556</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="Q27" s="16" t="s">
         <v>554</v>
@@ -5237,7 +5197,7 @@
         <v>166</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="Q28" s="16" t="s">
         <v>558</v>
@@ -5258,7 +5218,7 @@
         <v>129</v>
       </c>
       <c r="E29" s="33" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>182</v>
@@ -5282,7 +5242,7 @@
         <v>153</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="Q29" s="16" t="s">
         <v>535</v>
@@ -5303,7 +5263,7 @@
         <v>129</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>182</v>
@@ -5327,7 +5287,7 @@
         <v>153</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="Q30" s="16" t="s">
         <v>535</v>
@@ -5348,7 +5308,7 @@
         <v>129</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>182</v>
@@ -5372,7 +5332,7 @@
         <v>153</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="Q31" s="16" t="s">
         <v>535</v>
@@ -5393,7 +5353,7 @@
         <v>129</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>182</v>
@@ -5417,7 +5377,7 @@
         <v>153</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="Q32" s="16" t="s">
         <v>535</v>
@@ -5438,7 +5398,7 @@
         <v>129</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>182</v>
@@ -5462,7 +5422,7 @@
         <v>153</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="Q33" s="16" t="s">
         <v>535</v>
@@ -5483,7 +5443,7 @@
         <v>129</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>182</v>
@@ -5507,7 +5467,7 @@
         <v>153</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="Q34" s="16" t="s">
         <v>535</v>
@@ -5542,7 +5502,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="Q35" s="16" t="s">
         <v>535</v>
@@ -5587,7 +5547,7 @@
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="17" t="s">
@@ -5637,7 +5597,7 @@
         <v>153</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>830</v>
+        <v>820</v>
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="17" t="s">
@@ -5660,7 +5620,7 @@
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="15" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>490</v>
@@ -5685,7 +5645,7 @@
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="17" t="s">
@@ -5731,7 +5691,7 @@
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="17" t="s">
@@ -5775,7 +5735,7 @@
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="17" t="s">
@@ -5798,7 +5758,7 @@
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>490</v>
@@ -5841,7 +5801,7 @@
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>490</v>
@@ -5874,17 +5834,17 @@
         <v>42</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>782</v>
+        <v>772</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="15" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>490</v>
@@ -5915,20 +5875,20 @@
         <v>43</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>804</v>
+        <v>794</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="15" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="H44" s="2" t="b">
         <v>1</v>
@@ -5941,7 +5901,7 @@
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="Q44" s="16" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -6056,16 +6016,16 @@
         <v>716</v>
       </c>
       <c r="C48" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="H48" s="2" t="b">
         <v>1</v>
@@ -6073,14 +6033,14 @@
       <c r="I48">
         <v>300</v>
       </c>
-      <c r="K48">
-        <v>2000</v>
+      <c r="J48">
+        <v>2500</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>483</v>
       </c>
       <c r="Q48" s="16" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -6092,16 +6052,16 @@
         <v>719</v>
       </c>
       <c r="C49" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="H49" s="2" t="b">
         <v>1</v>
@@ -6109,14 +6069,14 @@
       <c r="I49">
         <v>300</v>
       </c>
-      <c r="K49">
-        <v>2000</v>
+      <c r="J49">
+        <v>2500</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>483</v>
       </c>
       <c r="Q49" s="16" t="s">
-        <v>846</v>
+        <v>836</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -8503,7 +8463,7 @@
         <v>191</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -8702,7 +8662,7 @@
         <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
@@ -8812,7 +8772,7 @@
         <v>578</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>767</v>
+        <v>757</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -8833,10 +8793,10 @@
         <v>593</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c r="F29" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -8866,19 +8826,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>785</v>
+        <v>775</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>800</v>
+        <v>790</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>788</v>
+        <v>778</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>790</v>
+        <v>780</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -8887,16 +8847,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>813</v>
+        <v>803</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -8908,16 +8868,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -9554,10 +9514,10 @@
         <v>718</v>
       </c>
       <c r="C34" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="D34" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="E34" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D34, settings!B$2:B$1048576, 0))</f>
@@ -9572,10 +9532,10 @@
         <v>579</v>
       </c>
       <c r="C35" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="D35" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="E35" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D35, settings!B$2:B$1048576, 0))</f>
@@ -9590,10 +9550,10 @@
         <v>639</v>
       </c>
       <c r="C36" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="D36" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="E36" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D36, settings!B$2:B$1048576, 0))</f>
@@ -9608,10 +9568,10 @@
         <v>640</v>
       </c>
       <c r="C37" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="D37" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="E37" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D37, settings!B$2:B$1048576, 0))</f>
@@ -9623,16 +9583,16 @@
         <v>97990</v>
       </c>
       <c r="B38" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
       <c r="C38" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
       <c r="D38" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
       <c r="E38" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -9676,10 +9636,10 @@
         <v>97985</v>
       </c>
       <c r="B41" t="s">
-        <v>805</v>
+        <v>795</v>
       </c>
       <c r="C41" t="s">
-        <v>805</v>
+        <v>795</v>
       </c>
       <c r="D41" t="s">
         <v>629</v>
@@ -10438,7 +10398,7 @@
         <v>636</v>
       </c>
       <c r="D83" t="s">
-        <v>758</v>
+        <v>748</v>
       </c>
       <c r="E83" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D83, settings!B$2:B$1048576, 0))</f>
@@ -10456,7 +10416,7 @@
         <v>635</v>
       </c>
       <c r="D84" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
       <c r="E84" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D84, settings!B$2:B$1048576, 0))</f>
@@ -10684,13 +10644,13 @@
         <v>97942</v>
       </c>
       <c r="B97" t="s">
-        <v>806</v>
+        <v>796</v>
       </c>
       <c r="C97" t="s">
-        <v>807</v>
+        <v>797</v>
       </c>
       <c r="D97" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="E97" t="str">
         <f>INDEX(settings!C$2:C$1048576, MATCH(taskname!D97, settings!B$2:B$1048576, 0))</f>
@@ -10711,8 +10671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -10754,9 +10714,6 @@
       <c r="C2" t="s">
         <v>174</v>
       </c>
-      <c r="D2" t="s">
-        <v>745</v>
-      </c>
       <c r="E2" t="s">
         <v>584</v>
       </c>
@@ -10775,9 +10732,7 @@
       <c r="C3" t="s">
         <v>173</v>
       </c>
-      <c r="D3" t="s">
-        <v>746</v>
-      </c>
+      <c r="D3"/>
       <c r="E3" t="s">
         <v>584</v>
       </c>
@@ -10796,9 +10751,6 @@
       <c r="C4" t="s">
         <v>178</v>
       </c>
-      <c r="D4" t="s">
-        <v>747</v>
-      </c>
       <c r="E4" t="s">
         <v>584</v>
       </c>
@@ -10817,9 +10769,6 @@
       <c r="C5" t="s">
         <v>549</v>
       </c>
-      <c r="D5" t="s">
-        <v>748</v>
-      </c>
       <c r="E5" t="s">
         <v>584</v>
       </c>
@@ -10838,9 +10787,6 @@
       <c r="C6" t="s">
         <v>603</v>
       </c>
-      <c r="D6" t="s">
-        <v>749</v>
-      </c>
       <c r="E6" t="s">
         <v>614</v>
       </c>
@@ -10859,9 +10805,6 @@
       <c r="C7" t="s">
         <v>604</v>
       </c>
-      <c r="D7" t="s">
-        <v>750</v>
-      </c>
       <c r="E7" t="s">
         <v>614</v>
       </c>
@@ -10880,9 +10823,6 @@
       <c r="C8" t="s">
         <v>606</v>
       </c>
-      <c r="D8" t="s">
-        <v>751</v>
-      </c>
       <c r="E8" t="s">
         <v>615</v>
       </c>
@@ -10901,9 +10841,6 @@
       <c r="C9" t="s">
         <v>608</v>
       </c>
-      <c r="D9" t="s">
-        <v>752</v>
-      </c>
       <c r="E9" t="s">
         <v>614</v>
       </c>
@@ -10922,9 +10859,6 @@
       <c r="C10" t="s">
         <v>610</v>
       </c>
-      <c r="D10" t="s">
-        <v>753</v>
-      </c>
       <c r="E10" t="s">
         <v>617</v>
       </c>
@@ -10942,9 +10876,6 @@
       </c>
       <c r="C11" t="s">
         <v>613</v>
-      </c>
-      <c r="D11" t="s">
-        <v>754</v>
       </c>
       <c r="E11" t="s">
         <v>620</v>
@@ -11879,66 +11810,66 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>771</v>
+        <v>761</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>772</v>
+        <v>762</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>773</v>
+        <v>763</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>778</v>
+        <v>768</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>779</v>
+        <v>769</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>780</v>
+        <v>770</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>816</v>
+        <v>806</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>816</v>
+        <v>806</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>